<commit_message>
Export of contour loads implemented.
</commit_message>
<xml_diff>
--- a/pyMaster_loads_tool.xlsx
+++ b/pyMaster_loads_tool.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://atlec-my.sharepoint.com/personal/mwo_woodthilsted_com/Documents/Professional/5_PYTHON/pyMasterLoadsTool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="11_AFB557827021BA1F9C2C107175FB6F18C44BF613" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C57E260F-088F-4880-AB57-AFA8040DAEED}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_5D32F417BDC4D05AA375E799C8C031A9731D5940" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7568026B-9348-425D-AFA3-6B959A48AC9C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="858" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39045" yWindow="4230" windowWidth="28800" windowHeight="15030" tabRatio="858" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Load case definition" sheetId="1" r:id="rId1"/>
     <sheet name="Load definition" sheetId="2" r:id="rId2"/>
     <sheet name="Load combination" sheetId="3" r:id="rId3"/>
     <sheet name="Contour load data" sheetId="4" r:id="rId4"/>
-    <sheet name="Screen capture" sheetId="5" r:id="rId5"/>
-    <sheet name="LaTeX code" sheetId="6" state="hidden" r:id="rId6"/>
-    <sheet name="LaTeX load combs apndx" sheetId="7" state="hidden" r:id="rId7"/>
+    <sheet name="Contour data template" sheetId="8" r:id="rId5"/>
+    <sheet name="Screen capture" sheetId="5" r:id="rId6"/>
+    <sheet name="LaTeX code" sheetId="6" state="hidden" r:id="rId7"/>
+    <sheet name="LaTeX load combs apndx" sheetId="7" state="hidden" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="BargePhoto">INDIRECT(#REF!)</definedName>
@@ -193,7 +194,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="256">
   <si>
     <t>Basic case no.</t>
   </si>
@@ -360,10 +361,16 @@
     <t>table 1</t>
   </si>
   <si>
+    <t>load on contour</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
     <t>global</t>
+  </si>
+  <si>
+    <t>load 3p on contour</t>
   </si>
   <si>
     <t>CAT_F</t>
@@ -390,19 +397,19 @@
     <t>-</t>
   </si>
   <si>
-    <t>Row: 9</t>
+    <t xml:space="preserve">Row: </t>
   </si>
   <si>
-    <t>Row: 10</t>
+    <t>9</t>
   </si>
   <si>
-    <t>Row: 11</t>
+    <t>10</t>
   </si>
   <si>
-    <t>Row: 12</t>
+    <t>11</t>
   </si>
   <si>
-    <t>3p definition</t>
+    <t>12</t>
   </si>
   <si>
     <t>Point number</t>
@@ -417,13 +424,16 @@
     <t>Z</t>
   </si>
   <si>
+    <t>3p definition</t>
+  </si>
+  <si>
     <t>A(-1, 2.5, 0.5, 0.0)</t>
   </si>
   <si>
-    <t>B(-1, 2.5, 0.5, 0.0)</t>
+    <t>B(-1, 3.5, 0.5, 0.0)</t>
   </si>
   <si>
-    <t>C(-1, 2.5, 0.5, 0.0)</t>
+    <t>C(-1, 3.0, 1.0, 0.0)</t>
   </si>
   <si>
     <t>Display settings</t>
@@ -1449,7 +1459,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="195">
+  <cellXfs count="194">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1852,6 +1862,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1860,13 +1876,13 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1923,16 +1939,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -2477,9 +2483,9 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFFFE699"/>
   </sheetPr>
-  <dimension ref="A1:N177"/>
+  <dimension ref="A1:M177"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
@@ -2496,43 +2502,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A1" s="163" t="s">
+      <c r="A1" s="165" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="167" t="s">
+      <c r="B1" s="169" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="164" t="s">
+      <c r="C1" s="168" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="165" t="s">
+      <c r="D1" s="166" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="166"/>
-      <c r="F1" s="166"/>
-      <c r="G1" s="166"/>
-      <c r="H1" s="166"/>
+      <c r="E1" s="167"/>
+      <c r="F1" s="167"/>
+      <c r="G1" s="167"/>
+      <c r="H1" s="167"/>
       <c r="K1" s="145" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="12.95" customHeight="1">
-      <c r="A2" s="161"/>
-      <c r="B2" s="161"/>
-      <c r="C2" s="161"/>
-      <c r="D2" s="160" t="s">
+      <c r="A2" s="163"/>
+      <c r="B2" s="163"/>
+      <c r="C2" s="163"/>
+      <c r="D2" s="162" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="160" t="s">
+      <c r="E2" s="162" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="160" t="s">
+      <c r="F2" s="162" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="160" t="s">
+      <c r="G2" s="162" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="160" t="s">
+      <c r="H2" s="162" t="s">
         <v>9</v>
       </c>
       <c r="J2" s="145" t="s">
@@ -2546,14 +2552,14 @@
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="161"/>
-      <c r="B3" s="161"/>
-      <c r="C3" s="161"/>
-      <c r="D3" s="161"/>
-      <c r="E3" s="161"/>
-      <c r="F3" s="161"/>
-      <c r="G3" s="161"/>
-      <c r="H3" s="161"/>
+      <c r="A3" s="163"/>
+      <c r="B3" s="163"/>
+      <c r="C3" s="163"/>
+      <c r="D3" s="163"/>
+      <c r="E3" s="163"/>
+      <c r="F3" s="163"/>
+      <c r="G3" s="163"/>
+      <c r="H3" s="163"/>
       <c r="J3" s="145" t="s">
         <v>12</v>
       </c>
@@ -2565,14 +2571,14 @@
       </c>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="161"/>
-      <c r="B4" s="161"/>
-      <c r="C4" s="161"/>
-      <c r="D4" s="161"/>
-      <c r="E4" s="161"/>
-      <c r="F4" s="161"/>
-      <c r="G4" s="161"/>
-      <c r="H4" s="161"/>
+      <c r="A4" s="163"/>
+      <c r="B4" s="163"/>
+      <c r="C4" s="163"/>
+      <c r="D4" s="163"/>
+      <c r="E4" s="163"/>
+      <c r="F4" s="163"/>
+      <c r="G4" s="163"/>
+      <c r="H4" s="163"/>
       <c r="J4" s="145" t="s">
         <v>14</v>
       </c>
@@ -2584,14 +2590,14 @@
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="161"/>
-      <c r="B5" s="161"/>
-      <c r="C5" s="161"/>
-      <c r="D5" s="161"/>
-      <c r="E5" s="161"/>
-      <c r="F5" s="161"/>
-      <c r="G5" s="161"/>
-      <c r="H5" s="161"/>
+      <c r="A5" s="163"/>
+      <c r="B5" s="163"/>
+      <c r="C5" s="163"/>
+      <c r="D5" s="163"/>
+      <c r="E5" s="163"/>
+      <c r="F5" s="163"/>
+      <c r="G5" s="163"/>
+      <c r="H5" s="163"/>
       <c r="J5" s="145" t="s">
         <v>16</v>
       </c>
@@ -2603,14 +2609,14 @@
       </c>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="162"/>
-      <c r="B6" s="162"/>
-      <c r="C6" s="162"/>
-      <c r="D6" s="162"/>
-      <c r="E6" s="162"/>
-      <c r="F6" s="162"/>
-      <c r="G6" s="162"/>
-      <c r="H6" s="162"/>
+      <c r="A6" s="164"/>
+      <c r="B6" s="164"/>
+      <c r="C6" s="164"/>
+      <c r="D6" s="164"/>
+      <c r="E6" s="164"/>
+      <c r="F6" s="164"/>
+      <c r="G6" s="164"/>
+      <c r="H6" s="164"/>
       <c r="J6" s="145" t="s">
         <v>18</v>
       </c>
@@ -4409,15 +4415,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="D2:D6"/>
+    <mergeCell ref="G2:G6"/>
+    <mergeCell ref="E2:E6"/>
     <mergeCell ref="F2:F6"/>
-    <mergeCell ref="D2:D6"/>
+    <mergeCell ref="A1:A6"/>
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="C1:C6"/>
+    <mergeCell ref="B1:B6"/>
     <mergeCell ref="H2:H6"/>
-    <mergeCell ref="E2:E6"/>
-    <mergeCell ref="A1:A6"/>
-    <mergeCell ref="C1:C6"/>
-    <mergeCell ref="D1:H1"/>
-    <mergeCell ref="B1:B6"/>
-    <mergeCell ref="G2:G6"/>
   </mergeCells>
   <conditionalFormatting sqref="F7:F177">
     <cfRule type="expression" dxfId="31" priority="2">
@@ -4433,23 +4439,23 @@
   <dataValidations count="9">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the load case number_x000a__x000a_Try to stick to a consistent naming convention and leave 100 possibilities for each load type. For example: _x000a_200-299 are live loads,_x000a_300-399 could be padeye loads,_x000a_400-499 could be HOP loads etc._x000a_ " sqref="A1:A6" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the name of the load case_x000a__x000a_Please keep naming of similar loads as consistent as possible" sqref="B1:B6" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576 F2:F6 F7:G1048576" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576 F2:F6 F7:G1048576" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"1,0"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="1- for Auxiliary case, 0 - if not." sqref="H2:H6" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7:C22" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="1- for Auxiliary case, 0 - if not." sqref="H2:H6" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7:C22" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>$J$2:$J$8</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E8:E177" xr:uid="{00000000-0002-0000-0000-000006000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E8:E177" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>IF(D8=1,$K$13:$K$15,$K$10:$K$13)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7" xr:uid="{00000000-0002-0000-0000-000007000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7" xr:uid="{00000000-0002-0000-0000-000006000000}">
       <formula1>IF(D7=1,$K$11:$K$15,$K$10:$K$13)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H7:H177" xr:uid="{00000000-0002-0000-0000-000008000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H7:H177" xr:uid="{00000000-0002-0000-0000-000007000000}">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose nature of the loadcase" sqref="C1:C6" xr:uid="{0261A2AE-29D1-4049-A6AF-7C1E09BD6AE2}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose nature of the loadcase" sqref="C1:C6" xr:uid="{00000000-0002-0000-0000-000008000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -4466,7 +4472,7 @@
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="AE13" sqref="AE13"/>
-      <selection pane="bottomLeft" activeCell="G129" sqref="G129"/>
+      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
@@ -4492,8 +4498,8 @@
     <col min="32" max="32" width="28.28515625" style="19" customWidth="1"/>
     <col min="33" max="33" width="8.7109375" style="19" customWidth="1"/>
     <col min="34" max="37" width="8.7109375" customWidth="1"/>
-    <col min="38" max="49" width="8.7109375" style="19" customWidth="1"/>
-    <col min="50" max="16384" width="8.7109375" style="19"/>
+    <col min="38" max="50" width="8.7109375" style="19" customWidth="1"/>
+    <col min="51" max="16384" width="8.7109375" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="23.1" customHeight="1">
@@ -4526,262 +4532,262 @@
       <c r="Y1" s="17"/>
       <c r="Z1" s="17"/>
       <c r="AA1" s="17"/>
-      <c r="AC1" s="185" t="s">
+      <c r="AC1" s="187" t="s">
         <v>30</v>
       </c>
-      <c r="AD1" s="169"/>
-      <c r="AE1" s="169"/>
-      <c r="AF1" s="170"/>
+      <c r="AD1" s="171"/>
+      <c r="AE1" s="171"/>
+      <c r="AF1" s="172"/>
     </row>
     <row r="2" spans="1:32" ht="12.4" customHeight="1">
-      <c r="A2" s="163" t="s">
+      <c r="A2" s="165" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="167" t="s">
+      <c r="B2" s="169" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="164" t="s">
+      <c r="C2" s="168" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="180"/>
-      <c r="E2" s="183"/>
-      <c r="F2" s="181"/>
-      <c r="G2" s="164" t="s">
+      <c r="D2" s="182"/>
+      <c r="E2" s="185"/>
+      <c r="F2" s="183"/>
+      <c r="G2" s="168" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="182" t="s">
+      <c r="H2" s="184" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="179" t="s">
+      <c r="I2" s="181" t="s">
         <v>32</v>
       </c>
-      <c r="J2" s="168" t="s">
+      <c r="J2" s="170" t="s">
         <v>33</v>
       </c>
-      <c r="K2" s="169"/>
-      <c r="L2" s="169"/>
-      <c r="M2" s="169"/>
-      <c r="N2" s="169"/>
-      <c r="O2" s="169"/>
-      <c r="P2" s="169"/>
-      <c r="Q2" s="169"/>
-      <c r="R2" s="169"/>
-      <c r="S2" s="169"/>
-      <c r="T2" s="169"/>
-      <c r="U2" s="169"/>
-      <c r="V2" s="169"/>
-      <c r="W2" s="169"/>
-      <c r="X2" s="169"/>
-      <c r="Y2" s="169"/>
-      <c r="Z2" s="170"/>
-      <c r="AA2" s="160" t="s">
+      <c r="K2" s="171"/>
+      <c r="L2" s="171"/>
+      <c r="M2" s="171"/>
+      <c r="N2" s="171"/>
+      <c r="O2" s="171"/>
+      <c r="P2" s="171"/>
+      <c r="Q2" s="171"/>
+      <c r="R2" s="171"/>
+      <c r="S2" s="171"/>
+      <c r="T2" s="171"/>
+      <c r="U2" s="171"/>
+      <c r="V2" s="171"/>
+      <c r="W2" s="171"/>
+      <c r="X2" s="171"/>
+      <c r="Y2" s="171"/>
+      <c r="Z2" s="172"/>
+      <c r="AA2" s="162" t="s">
         <v>34</v>
       </c>
-      <c r="AC2" s="164" t="s">
+      <c r="AC2" s="168" t="s">
         <v>35</v>
       </c>
-      <c r="AD2" s="164" t="s">
+      <c r="AD2" s="168" t="s">
         <v>36</v>
       </c>
-      <c r="AE2" s="164" t="s">
+      <c r="AE2" s="168" t="s">
         <v>37</v>
       </c>
-      <c r="AF2" s="164" t="s">
+      <c r="AF2" s="168" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:32" ht="12.6" customHeight="1">
-      <c r="A3" s="161"/>
-      <c r="B3" s="161"/>
-      <c r="C3" s="161"/>
-      <c r="D3" s="174"/>
-      <c r="E3" s="175"/>
-      <c r="F3" s="176"/>
-      <c r="G3" s="161"/>
-      <c r="H3" s="174"/>
-      <c r="I3" s="161"/>
-      <c r="J3" s="171" t="s">
+      <c r="A3" s="163"/>
+      <c r="B3" s="163"/>
+      <c r="C3" s="163"/>
+      <c r="D3" s="176"/>
+      <c r="E3" s="177"/>
+      <c r="F3" s="178"/>
+      <c r="G3" s="163"/>
+      <c r="H3" s="176"/>
+      <c r="I3" s="163"/>
+      <c r="J3" s="173" t="s">
         <v>39</v>
       </c>
-      <c r="K3" s="172"/>
-      <c r="L3" s="173"/>
-      <c r="M3" s="184" t="s">
+      <c r="K3" s="174"/>
+      <c r="L3" s="175"/>
+      <c r="M3" s="186" t="s">
         <v>40</v>
       </c>
-      <c r="N3" s="172"/>
-      <c r="O3" s="173"/>
-      <c r="P3" s="164" t="s">
+      <c r="N3" s="174"/>
+      <c r="O3" s="175"/>
+      <c r="P3" s="168" t="s">
         <v>41</v>
       </c>
-      <c r="Q3" s="172"/>
-      <c r="R3" s="173"/>
-      <c r="S3" s="160" t="s">
+      <c r="Q3" s="174"/>
+      <c r="R3" s="175"/>
+      <c r="S3" s="162" t="s">
         <v>42</v>
       </c>
-      <c r="T3" s="172"/>
-      <c r="U3" s="173"/>
-      <c r="V3" s="160" t="s">
+      <c r="T3" s="174"/>
+      <c r="U3" s="175"/>
+      <c r="V3" s="162" t="s">
         <v>43</v>
       </c>
-      <c r="W3" s="160" t="s">
+      <c r="W3" s="162" t="s">
         <v>44</v>
       </c>
-      <c r="X3" s="173"/>
-      <c r="Y3" s="160" t="s">
+      <c r="X3" s="175"/>
+      <c r="Y3" s="162" t="s">
         <v>45</v>
       </c>
-      <c r="Z3" s="160" t="s">
+      <c r="Z3" s="162" t="s">
         <v>46</v>
       </c>
-      <c r="AA3" s="161"/>
-      <c r="AC3" s="161"/>
-      <c r="AD3" s="161"/>
-      <c r="AE3" s="161"/>
-      <c r="AF3" s="161"/>
+      <c r="AA3" s="163"/>
+      <c r="AC3" s="163"/>
+      <c r="AD3" s="163"/>
+      <c r="AE3" s="163"/>
+      <c r="AF3" s="163"/>
     </row>
     <row r="4" spans="1:32" ht="12.6" customHeight="1">
-      <c r="A4" s="161"/>
-      <c r="B4" s="161"/>
-      <c r="C4" s="161"/>
-      <c r="D4" s="174"/>
-      <c r="E4" s="175"/>
-      <c r="F4" s="176"/>
-      <c r="G4" s="161"/>
-      <c r="H4" s="174"/>
-      <c r="I4" s="161"/>
-      <c r="J4" s="174"/>
-      <c r="K4" s="175"/>
-      <c r="L4" s="176"/>
-      <c r="M4" s="174"/>
-      <c r="N4" s="175"/>
-      <c r="O4" s="176"/>
-      <c r="P4" s="174"/>
-      <c r="Q4" s="175"/>
-      <c r="R4" s="176"/>
-      <c r="S4" s="174"/>
-      <c r="T4" s="175"/>
-      <c r="U4" s="176"/>
-      <c r="V4" s="161"/>
-      <c r="W4" s="174"/>
-      <c r="X4" s="176"/>
-      <c r="Y4" s="161"/>
-      <c r="Z4" s="161"/>
-      <c r="AA4" s="161"/>
-      <c r="AC4" s="161"/>
-      <c r="AD4" s="161"/>
-      <c r="AE4" s="161"/>
-      <c r="AF4" s="161"/>
+      <c r="A4" s="163"/>
+      <c r="B4" s="163"/>
+      <c r="C4" s="163"/>
+      <c r="D4" s="176"/>
+      <c r="E4" s="177"/>
+      <c r="F4" s="178"/>
+      <c r="G4" s="163"/>
+      <c r="H4" s="176"/>
+      <c r="I4" s="163"/>
+      <c r="J4" s="176"/>
+      <c r="K4" s="177"/>
+      <c r="L4" s="178"/>
+      <c r="M4" s="176"/>
+      <c r="N4" s="177"/>
+      <c r="O4" s="178"/>
+      <c r="P4" s="176"/>
+      <c r="Q4" s="177"/>
+      <c r="R4" s="178"/>
+      <c r="S4" s="176"/>
+      <c r="T4" s="177"/>
+      <c r="U4" s="178"/>
+      <c r="V4" s="163"/>
+      <c r="W4" s="176"/>
+      <c r="X4" s="178"/>
+      <c r="Y4" s="163"/>
+      <c r="Z4" s="163"/>
+      <c r="AA4" s="163"/>
+      <c r="AC4" s="163"/>
+      <c r="AD4" s="163"/>
+      <c r="AE4" s="163"/>
+      <c r="AF4" s="163"/>
     </row>
     <row r="5" spans="1:32" ht="25.15" customHeight="1">
-      <c r="A5" s="161"/>
-      <c r="B5" s="161"/>
-      <c r="C5" s="161"/>
-      <c r="D5" s="174"/>
-      <c r="E5" s="175"/>
-      <c r="F5" s="176"/>
-      <c r="G5" s="161"/>
-      <c r="H5" s="174"/>
-      <c r="I5" s="161"/>
-      <c r="J5" s="174"/>
-      <c r="K5" s="175"/>
-      <c r="L5" s="176"/>
-      <c r="M5" s="174"/>
-      <c r="N5" s="175"/>
-      <c r="O5" s="176"/>
-      <c r="P5" s="174"/>
-      <c r="Q5" s="175"/>
-      <c r="R5" s="176"/>
-      <c r="S5" s="174"/>
-      <c r="T5" s="175"/>
-      <c r="U5" s="176"/>
-      <c r="V5" s="161"/>
-      <c r="W5" s="174"/>
-      <c r="X5" s="176"/>
-      <c r="Y5" s="161"/>
-      <c r="Z5" s="161"/>
-      <c r="AA5" s="161"/>
-      <c r="AC5" s="161"/>
-      <c r="AD5" s="161"/>
-      <c r="AE5" s="161"/>
-      <c r="AF5" s="161"/>
+      <c r="A5" s="163"/>
+      <c r="B5" s="163"/>
+      <c r="C5" s="163"/>
+      <c r="D5" s="176"/>
+      <c r="E5" s="177"/>
+      <c r="F5" s="178"/>
+      <c r="G5" s="163"/>
+      <c r="H5" s="176"/>
+      <c r="I5" s="163"/>
+      <c r="J5" s="176"/>
+      <c r="K5" s="177"/>
+      <c r="L5" s="178"/>
+      <c r="M5" s="176"/>
+      <c r="N5" s="177"/>
+      <c r="O5" s="178"/>
+      <c r="P5" s="176"/>
+      <c r="Q5" s="177"/>
+      <c r="R5" s="178"/>
+      <c r="S5" s="176"/>
+      <c r="T5" s="177"/>
+      <c r="U5" s="178"/>
+      <c r="V5" s="163"/>
+      <c r="W5" s="176"/>
+      <c r="X5" s="178"/>
+      <c r="Y5" s="163"/>
+      <c r="Z5" s="163"/>
+      <c r="AA5" s="163"/>
+      <c r="AC5" s="163"/>
+      <c r="AD5" s="163"/>
+      <c r="AE5" s="163"/>
+      <c r="AF5" s="163"/>
     </row>
     <row r="6" spans="1:32" ht="12.6" customHeight="1">
-      <c r="A6" s="161"/>
-      <c r="B6" s="161"/>
-      <c r="C6" s="161"/>
-      <c r="D6" s="174"/>
-      <c r="E6" s="175"/>
-      <c r="F6" s="176"/>
-      <c r="G6" s="161"/>
-      <c r="H6" s="174"/>
-      <c r="I6" s="161"/>
-      <c r="J6" s="177"/>
-      <c r="K6" s="166"/>
-      <c r="L6" s="178"/>
-      <c r="M6" s="177"/>
-      <c r="N6" s="166"/>
-      <c r="O6" s="178"/>
-      <c r="P6" s="174"/>
-      <c r="Q6" s="175"/>
-      <c r="R6" s="176"/>
-      <c r="S6" s="177"/>
-      <c r="T6" s="166"/>
-      <c r="U6" s="178"/>
-      <c r="V6" s="161"/>
-      <c r="W6" s="174"/>
-      <c r="X6" s="176"/>
-      <c r="Y6" s="161"/>
-      <c r="Z6" s="161"/>
-      <c r="AA6" s="161"/>
-      <c r="AC6" s="161"/>
-      <c r="AD6" s="161"/>
-      <c r="AE6" s="161"/>
-      <c r="AF6" s="161"/>
+      <c r="A6" s="163"/>
+      <c r="B6" s="163"/>
+      <c r="C6" s="163"/>
+      <c r="D6" s="176"/>
+      <c r="E6" s="177"/>
+      <c r="F6" s="178"/>
+      <c r="G6" s="163"/>
+      <c r="H6" s="176"/>
+      <c r="I6" s="163"/>
+      <c r="J6" s="179"/>
+      <c r="K6" s="167"/>
+      <c r="L6" s="180"/>
+      <c r="M6" s="179"/>
+      <c r="N6" s="167"/>
+      <c r="O6" s="180"/>
+      <c r="P6" s="176"/>
+      <c r="Q6" s="177"/>
+      <c r="R6" s="178"/>
+      <c r="S6" s="179"/>
+      <c r="T6" s="167"/>
+      <c r="U6" s="180"/>
+      <c r="V6" s="163"/>
+      <c r="W6" s="176"/>
+      <c r="X6" s="178"/>
+      <c r="Y6" s="163"/>
+      <c r="Z6" s="163"/>
+      <c r="AA6" s="163"/>
+      <c r="AC6" s="163"/>
+      <c r="AD6" s="163"/>
+      <c r="AE6" s="163"/>
+      <c r="AF6" s="163"/>
     </row>
     <row r="7" spans="1:32">
-      <c r="A7" s="162"/>
-      <c r="B7" s="162"/>
-      <c r="C7" s="162"/>
-      <c r="D7" s="174"/>
-      <c r="E7" s="175"/>
-      <c r="F7" s="176"/>
-      <c r="G7" s="162"/>
-      <c r="H7" s="174"/>
-      <c r="I7" s="162"/>
-      <c r="J7" s="168" t="s">
+      <c r="A7" s="164"/>
+      <c r="B7" s="164"/>
+      <c r="C7" s="164"/>
+      <c r="D7" s="176"/>
+      <c r="E7" s="177"/>
+      <c r="F7" s="178"/>
+      <c r="G7" s="164"/>
+      <c r="H7" s="179"/>
+      <c r="I7" s="164"/>
+      <c r="J7" s="170" t="s">
         <v>47</v>
       </c>
-      <c r="K7" s="169"/>
-      <c r="L7" s="170"/>
-      <c r="M7" s="168" t="s">
+      <c r="K7" s="171"/>
+      <c r="L7" s="172"/>
+      <c r="M7" s="170" t="s">
         <v>48</v>
       </c>
-      <c r="N7" s="169"/>
-      <c r="O7" s="170"/>
-      <c r="P7" s="177"/>
-      <c r="Q7" s="166"/>
-      <c r="R7" s="178"/>
-      <c r="S7" s="168" t="s">
+      <c r="N7" s="171"/>
+      <c r="O7" s="172"/>
+      <c r="P7" s="179"/>
+      <c r="Q7" s="167"/>
+      <c r="R7" s="180"/>
+      <c r="S7" s="170" t="s">
         <v>49</v>
       </c>
-      <c r="T7" s="169"/>
-      <c r="U7" s="170"/>
-      <c r="V7" s="162"/>
-      <c r="W7" s="177"/>
-      <c r="X7" s="178"/>
-      <c r="Y7" s="162"/>
-      <c r="Z7" s="162"/>
-      <c r="AA7" s="162"/>
-      <c r="AC7" s="162"/>
-      <c r="AD7" s="162"/>
-      <c r="AE7" s="162"/>
-      <c r="AF7" s="162"/>
+      <c r="T7" s="171"/>
+      <c r="U7" s="172"/>
+      <c r="V7" s="164"/>
+      <c r="W7" s="179"/>
+      <c r="X7" s="180"/>
+      <c r="Y7" s="164"/>
+      <c r="Z7" s="164"/>
+      <c r="AA7" s="164"/>
+      <c r="AC7" s="164"/>
+      <c r="AD7" s="164"/>
+      <c r="AE7" s="164"/>
+      <c r="AF7" s="164"/>
     </row>
     <row r="8" spans="1:32">
       <c r="A8" s="153">
         <v>1</v>
       </c>
-      <c r="B8" s="193" t="s">
+      <c r="B8" s="160" t="s">
         <v>20</v>
       </c>
       <c r="C8" s="94" t="str">
@@ -4832,7 +4838,7 @@
       <c r="A9" s="154">
         <v>1</v>
       </c>
-      <c r="B9" s="194" t="s">
+      <c r="B9" s="161" t="s">
         <v>20</v>
       </c>
       <c r="C9" s="94" t="str">
@@ -4849,10 +4855,10 @@
         <v>1:STA1</v>
       </c>
       <c r="H9" s="67" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I9" s="141" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J9" s="116">
         <v>0</v>
@@ -4892,7 +4898,7 @@
       </c>
       <c r="V9" s="119"/>
       <c r="W9" s="120" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="X9" s="111"/>
       <c r="Y9" s="17">
@@ -4911,7 +4917,7 @@
       <c r="A10" s="154">
         <v>1</v>
       </c>
-      <c r="B10" s="194" t="s">
+      <c r="B10" s="161" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="94" t="str">
@@ -4926,10 +4932,10 @@
         <v>1:STA1</v>
       </c>
       <c r="H10" s="67" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I10" s="141" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J10" s="116">
         <v>0</v>
@@ -4969,7 +4975,7 @@
       </c>
       <c r="V10" s="119"/>
       <c r="W10" s="120" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="X10" s="111"/>
       <c r="Y10" s="17">
@@ -5005,10 +5011,10 @@
         <v>1:STA1</v>
       </c>
       <c r="H11" s="67" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I11" s="141" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J11" s="116">
         <v>0</v>
@@ -5048,7 +5054,7 @@
       </c>
       <c r="V11" s="119"/>
       <c r="W11" s="120" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="X11" s="111"/>
       <c r="Y11" s="17">
@@ -5083,9 +5089,11 @@
         <f t="shared" si="0"/>
         <v>1:STA1</v>
       </c>
-      <c r="H12" s="67"/>
+      <c r="H12" s="67" t="s">
+        <v>56</v>
+      </c>
       <c r="I12" s="142" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J12" s="116">
         <v>0</v>
@@ -5125,7 +5133,7 @@
       </c>
       <c r="V12" s="100"/>
       <c r="W12" s="120" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="X12" s="111"/>
       <c r="Y12" s="17">
@@ -5307,7 +5315,7 @@
       </c>
       <c r="D17" s="17"/>
       <c r="E17" s="95" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F17" s="17"/>
       <c r="G17" s="21" t="str">
@@ -5426,7 +5434,7 @@
       </c>
       <c r="D20" s="17"/>
       <c r="E20" s="95" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F20" s="17"/>
       <c r="G20" s="21" t="str">
@@ -5545,7 +5553,7 @@
       </c>
       <c r="D23" s="17"/>
       <c r="E23" s="95" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F23" s="17"/>
       <c r="G23" s="21" t="str">
@@ -5664,7 +5672,7 @@
       </c>
       <c r="D26" s="17"/>
       <c r="E26" s="95" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F26" s="17"/>
       <c r="G26" s="21" t="str">
@@ -5713,7 +5721,7 @@
       <c r="H27" s="67"/>
       <c r="I27" s="141"/>
       <c r="J27" s="116"/>
-      <c r="K27" s="192"/>
+      <c r="K27" s="117"/>
       <c r="L27" s="118"/>
       <c r="M27" s="97"/>
       <c r="N27" s="96"/>
@@ -5783,7 +5791,7 @@
       </c>
       <c r="D29" s="17"/>
       <c r="E29" s="95" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F29" s="17"/>
       <c r="G29" s="21" t="str">
@@ -5832,7 +5840,7 @@
       <c r="H30" s="67"/>
       <c r="I30" s="141"/>
       <c r="J30" s="116"/>
-      <c r="K30" s="192"/>
+      <c r="K30" s="117"/>
       <c r="L30" s="118"/>
       <c r="M30" s="97"/>
       <c r="N30" s="96"/>
@@ -5902,7 +5910,7 @@
       </c>
       <c r="D32" s="17"/>
       <c r="E32" s="95" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F32" s="17"/>
       <c r="G32" s="21" t="str">
@@ -5951,7 +5959,7 @@
       <c r="H33" s="67"/>
       <c r="I33" s="141"/>
       <c r="J33" s="116"/>
-      <c r="K33" s="192"/>
+      <c r="K33" s="117"/>
       <c r="L33" s="118"/>
       <c r="M33" s="97"/>
       <c r="N33" s="96"/>
@@ -6021,7 +6029,7 @@
       </c>
       <c r="D35" s="17"/>
       <c r="E35" s="95" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F35" s="17"/>
       <c r="G35" s="21" t="str">
@@ -6070,7 +6078,7 @@
       <c r="H36" s="67"/>
       <c r="I36" s="141"/>
       <c r="J36" s="116"/>
-      <c r="K36" s="192"/>
+      <c r="K36" s="117"/>
       <c r="L36" s="118"/>
       <c r="M36" s="97"/>
       <c r="N36" s="96"/>
@@ -6133,7 +6141,7 @@
     </row>
     <row r="38" spans="1:32">
       <c r="A38" s="154"/>
-      <c r="B38" s="194"/>
+      <c r="B38" s="161"/>
       <c r="C38" s="94" t="e">
         <f>VLOOKUP(A38,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -6172,7 +6180,7 @@
     </row>
     <row r="39" spans="1:32">
       <c r="A39" s="154"/>
-      <c r="B39" s="194"/>
+      <c r="B39" s="161"/>
       <c r="C39" s="94" t="e">
         <f>VLOOKUP(A39,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -6211,7 +6219,7 @@
     </row>
     <row r="40" spans="1:32">
       <c r="A40" s="154"/>
-      <c r="B40" s="194"/>
+      <c r="B40" s="161"/>
       <c r="C40" s="94" t="e">
         <f>VLOOKUP(A40,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -6250,7 +6258,7 @@
     </row>
     <row r="41" spans="1:32">
       <c r="A41" s="154"/>
-      <c r="B41" s="194"/>
+      <c r="B41" s="161"/>
       <c r="C41" s="94" t="e">
         <f>VLOOKUP(A41,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -6289,7 +6297,7 @@
     </row>
     <row r="42" spans="1:32">
       <c r="A42" s="154"/>
-      <c r="B42" s="194"/>
+      <c r="B42" s="161"/>
       <c r="C42" s="94" t="e">
         <f>VLOOKUP(A42,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -6328,7 +6336,7 @@
     </row>
     <row r="43" spans="1:32">
       <c r="A43" s="154"/>
-      <c r="B43" s="194"/>
+      <c r="B43" s="161"/>
       <c r="C43" s="94" t="e">
         <f>VLOOKUP(A43,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -6367,7 +6375,7 @@
     </row>
     <row r="44" spans="1:32">
       <c r="A44" s="154"/>
-      <c r="B44" s="194"/>
+      <c r="B44" s="161"/>
       <c r="C44" s="94" t="e">
         <f>VLOOKUP(A44,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -6406,7 +6414,7 @@
     </row>
     <row r="45" spans="1:32">
       <c r="A45" s="155"/>
-      <c r="B45" s="194"/>
+      <c r="B45" s="161"/>
       <c r="C45" s="94" t="e">
         <f>VLOOKUP(A45,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -6445,7 +6453,7 @@
     </row>
     <row r="46" spans="1:32">
       <c r="A46" s="155"/>
-      <c r="B46" s="194"/>
+      <c r="B46" s="161"/>
       <c r="C46" s="94" t="e">
         <f>VLOOKUP(A46,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -6484,7 +6492,7 @@
     </row>
     <row r="47" spans="1:32">
       <c r="A47" s="155"/>
-      <c r="B47" s="194"/>
+      <c r="B47" s="161"/>
       <c r="C47" s="94" t="e">
         <f>VLOOKUP(A47,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -6523,7 +6531,7 @@
     </row>
     <row r="48" spans="1:32">
       <c r="A48" s="155"/>
-      <c r="B48" s="194"/>
+      <c r="B48" s="161"/>
       <c r="C48" s="94" t="e">
         <f>VLOOKUP(A48,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -6562,7 +6570,7 @@
     </row>
     <row r="49" spans="1:32">
       <c r="A49" s="155"/>
-      <c r="B49" s="194"/>
+      <c r="B49" s="161"/>
       <c r="C49" s="94" t="e">
         <f>VLOOKUP(A49,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -6601,7 +6609,7 @@
     </row>
     <row r="50" spans="1:32">
       <c r="A50" s="155"/>
-      <c r="B50" s="194"/>
+      <c r="B50" s="161"/>
       <c r="C50" s="94" t="e">
         <f>VLOOKUP(A50,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -6640,7 +6648,7 @@
     </row>
     <row r="51" spans="1:32">
       <c r="A51" s="155"/>
-      <c r="B51" s="194"/>
+      <c r="B51" s="161"/>
       <c r="C51" s="94" t="e">
         <f>VLOOKUP(A51,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -6679,7 +6687,7 @@
     </row>
     <row r="52" spans="1:32">
       <c r="A52" s="155"/>
-      <c r="B52" s="194"/>
+      <c r="B52" s="161"/>
       <c r="C52" s="94" t="e">
         <f>VLOOKUP(A52,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -6718,7 +6726,7 @@
     </row>
     <row r="53" spans="1:32">
       <c r="A53" s="155"/>
-      <c r="B53" s="194"/>
+      <c r="B53" s="161"/>
       <c r="C53" s="94" t="e">
         <f>VLOOKUP(A53,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -6757,7 +6765,7 @@
     </row>
     <row r="54" spans="1:32" ht="13.15" customHeight="1">
       <c r="A54" s="155"/>
-      <c r="B54" s="194"/>
+      <c r="B54" s="161"/>
       <c r="C54" s="94" t="e">
         <f>VLOOKUP(A54,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -6796,7 +6804,7 @@
     </row>
     <row r="55" spans="1:32">
       <c r="A55" s="155"/>
-      <c r="B55" s="194"/>
+      <c r="B55" s="161"/>
       <c r="C55" s="94" t="e">
         <f>VLOOKUP(A55,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -6835,7 +6843,7 @@
     </row>
     <row r="56" spans="1:32">
       <c r="A56" s="155"/>
-      <c r="B56" s="194"/>
+      <c r="B56" s="161"/>
       <c r="C56" s="94" t="e">
         <f>VLOOKUP(A56,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -6874,7 +6882,7 @@
     </row>
     <row r="57" spans="1:32">
       <c r="A57" s="155"/>
-      <c r="B57" s="194"/>
+      <c r="B57" s="161"/>
       <c r="C57" s="94" t="e">
         <f>VLOOKUP(A57,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -6913,7 +6921,7 @@
     </row>
     <row r="58" spans="1:32">
       <c r="A58" s="155"/>
-      <c r="B58" s="194"/>
+      <c r="B58" s="161"/>
       <c r="C58" s="94" t="e">
         <f>VLOOKUP(A58,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -6952,7 +6960,7 @@
     </row>
     <row r="59" spans="1:32">
       <c r="A59" s="155"/>
-      <c r="B59" s="194"/>
+      <c r="B59" s="161"/>
       <c r="C59" s="94" t="e">
         <f>VLOOKUP(A59,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -6991,7 +6999,7 @@
     </row>
     <row r="60" spans="1:32">
       <c r="A60" s="155"/>
-      <c r="B60" s="194"/>
+      <c r="B60" s="161"/>
       <c r="C60" s="94" t="e">
         <f>VLOOKUP(A60,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -7030,7 +7038,7 @@
     </row>
     <row r="61" spans="1:32">
       <c r="A61" s="155"/>
-      <c r="B61" s="194"/>
+      <c r="B61" s="161"/>
       <c r="C61" s="94" t="e">
         <f>VLOOKUP(A61,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -7069,7 +7077,7 @@
     </row>
     <row r="62" spans="1:32">
       <c r="A62" s="155"/>
-      <c r="B62" s="194"/>
+      <c r="B62" s="161"/>
       <c r="C62" s="94" t="e">
         <f>VLOOKUP(A62,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -7108,7 +7116,7 @@
     </row>
     <row r="63" spans="1:32">
       <c r="A63" s="155"/>
-      <c r="B63" s="194"/>
+      <c r="B63" s="161"/>
       <c r="C63" s="94" t="e">
         <f>VLOOKUP(A63,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -7147,7 +7155,7 @@
     </row>
     <row r="64" spans="1:32">
       <c r="A64" s="155"/>
-      <c r="B64" s="194"/>
+      <c r="B64" s="161"/>
       <c r="C64" s="94" t="e">
         <f>VLOOKUP(A64,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -7186,7 +7194,7 @@
     </row>
     <row r="65" spans="1:32">
       <c r="A65" s="155"/>
-      <c r="B65" s="194"/>
+      <c r="B65" s="161"/>
       <c r="C65" s="94" t="e">
         <f>VLOOKUP(A65,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -7225,7 +7233,7 @@
     </row>
     <row r="66" spans="1:32">
       <c r="A66" s="155"/>
-      <c r="B66" s="194"/>
+      <c r="B66" s="161"/>
       <c r="C66" s="94" t="e">
         <f>VLOOKUP(A66,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -7264,7 +7272,7 @@
     </row>
     <row r="67" spans="1:32">
       <c r="A67" s="155"/>
-      <c r="B67" s="194"/>
+      <c r="B67" s="161"/>
       <c r="C67" s="94" t="e">
         <f>VLOOKUP(A67,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -7303,7 +7311,7 @@
     </row>
     <row r="68" spans="1:32">
       <c r="A68" s="155"/>
-      <c r="B68" s="194"/>
+      <c r="B68" s="161"/>
       <c r="C68" s="94" t="e">
         <f>VLOOKUP(A68,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -7342,7 +7350,7 @@
     </row>
     <row r="69" spans="1:32">
       <c r="A69" s="155"/>
-      <c r="B69" s="194"/>
+      <c r="B69" s="161"/>
       <c r="C69" s="94" t="e">
         <f>VLOOKUP(A69,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -7381,7 +7389,7 @@
     </row>
     <row r="70" spans="1:32">
       <c r="A70" s="155"/>
-      <c r="B70" s="194"/>
+      <c r="B70" s="161"/>
       <c r="C70" s="94" t="e">
         <f>VLOOKUP(A70,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -7420,7 +7428,7 @@
     </row>
     <row r="71" spans="1:32">
       <c r="A71" s="155"/>
-      <c r="B71" s="194"/>
+      <c r="B71" s="161"/>
       <c r="C71" s="94" t="e">
         <f>VLOOKUP(A71,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -7459,7 +7467,7 @@
     </row>
     <row r="72" spans="1:32">
       <c r="A72" s="155"/>
-      <c r="B72" s="194"/>
+      <c r="B72" s="161"/>
       <c r="C72" s="94" t="e">
         <f>VLOOKUP(A72,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -7498,7 +7506,7 @@
     </row>
     <row r="73" spans="1:32">
       <c r="A73" s="155"/>
-      <c r="B73" s="194"/>
+      <c r="B73" s="161"/>
       <c r="C73" s="94" t="e">
         <f>VLOOKUP(A73,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -7537,7 +7545,7 @@
     </row>
     <row r="74" spans="1:32">
       <c r="A74" s="155"/>
-      <c r="B74" s="194"/>
+      <c r="B74" s="161"/>
       <c r="C74" s="94" t="e">
         <f>VLOOKUP(A74,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -7576,7 +7584,7 @@
     </row>
     <row r="75" spans="1:32">
       <c r="A75" s="155"/>
-      <c r="B75" s="194"/>
+      <c r="B75" s="161"/>
       <c r="C75" s="94" t="e">
         <f>VLOOKUP(A75,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -7615,7 +7623,7 @@
     </row>
     <row r="76" spans="1:32">
       <c r="A76" s="155"/>
-      <c r="B76" s="194"/>
+      <c r="B76" s="161"/>
       <c r="C76" s="94" t="e">
         <f>VLOOKUP(A76,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -7654,7 +7662,7 @@
     </row>
     <row r="77" spans="1:32">
       <c r="A77" s="155"/>
-      <c r="B77" s="194"/>
+      <c r="B77" s="161"/>
       <c r="C77" s="94" t="e">
         <f>VLOOKUP(A77,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -7693,7 +7701,7 @@
     </row>
     <row r="78" spans="1:32">
       <c r="A78" s="155"/>
-      <c r="B78" s="194"/>
+      <c r="B78" s="161"/>
       <c r="C78" s="94" t="e">
         <f>VLOOKUP(A78,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -7732,7 +7740,7 @@
     </row>
     <row r="79" spans="1:32">
       <c r="A79" s="155"/>
-      <c r="B79" s="194"/>
+      <c r="B79" s="161"/>
       <c r="C79" s="94" t="e">
         <f>VLOOKUP(A79,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -7771,7 +7779,7 @@
     </row>
     <row r="80" spans="1:32">
       <c r="A80" s="155"/>
-      <c r="B80" s="194"/>
+      <c r="B80" s="161"/>
       <c r="C80" s="94" t="e">
         <f>VLOOKUP(A80,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -7810,7 +7818,7 @@
     </row>
     <row r="81" spans="1:32">
       <c r="A81" s="155"/>
-      <c r="B81" s="194"/>
+      <c r="B81" s="161"/>
       <c r="C81" s="94" t="e">
         <f>VLOOKUP(A81,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -7849,7 +7857,7 @@
     </row>
     <row r="82" spans="1:32">
       <c r="A82" s="155"/>
-      <c r="B82" s="194"/>
+      <c r="B82" s="161"/>
       <c r="C82" s="94" t="e">
         <f>VLOOKUP(A82,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -7888,7 +7896,7 @@
     </row>
     <row r="83" spans="1:32">
       <c r="A83" s="155"/>
-      <c r="B83" s="194"/>
+      <c r="B83" s="161"/>
       <c r="C83" s="94" t="e">
         <f>VLOOKUP(A83,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -7927,7 +7935,7 @@
     </row>
     <row r="84" spans="1:32">
       <c r="A84" s="155"/>
-      <c r="B84" s="194"/>
+      <c r="B84" s="161"/>
       <c r="C84" s="94" t="e">
         <f>VLOOKUP(A84,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -7966,7 +7974,7 @@
     </row>
     <row r="85" spans="1:32">
       <c r="A85" s="155"/>
-      <c r="B85" s="194"/>
+      <c r="B85" s="161"/>
       <c r="C85" s="94" t="e">
         <f>VLOOKUP(A85,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -8005,7 +8013,7 @@
     </row>
     <row r="86" spans="1:32">
       <c r="A86" s="155"/>
-      <c r="B86" s="194"/>
+      <c r="B86" s="161"/>
       <c r="C86" s="94" t="e">
         <f>VLOOKUP(A86,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -8044,7 +8052,7 @@
     </row>
     <row r="87" spans="1:32">
       <c r="A87" s="155"/>
-      <c r="B87" s="194"/>
+      <c r="B87" s="161"/>
       <c r="C87" s="94" t="e">
         <f>VLOOKUP(A87,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -8083,7 +8091,7 @@
     </row>
     <row r="88" spans="1:32">
       <c r="A88" s="155"/>
-      <c r="B88" s="194"/>
+      <c r="B88" s="161"/>
       <c r="C88" s="94" t="e">
         <f>VLOOKUP(A88,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -8122,7 +8130,7 @@
     </row>
     <row r="89" spans="1:32">
       <c r="A89" s="155"/>
-      <c r="B89" s="194"/>
+      <c r="B89" s="161"/>
       <c r="C89" s="94" t="e">
         <f>VLOOKUP(A89,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -8161,7 +8169,7 @@
     </row>
     <row r="90" spans="1:32">
       <c r="A90" s="155"/>
-      <c r="B90" s="194"/>
+      <c r="B90" s="161"/>
       <c r="C90" s="94" t="e">
         <f>VLOOKUP(A90,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -8200,7 +8208,7 @@
     </row>
     <row r="91" spans="1:32">
       <c r="A91" s="155"/>
-      <c r="B91" s="194"/>
+      <c r="B91" s="161"/>
       <c r="C91" s="94" t="e">
         <f>VLOOKUP(A91,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -8239,7 +8247,7 @@
     </row>
     <row r="92" spans="1:32">
       <c r="A92" s="155"/>
-      <c r="B92" s="194"/>
+      <c r="B92" s="161"/>
       <c r="C92" s="94" t="e">
         <f>VLOOKUP(A92,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -8278,7 +8286,7 @@
     </row>
     <row r="93" spans="1:32">
       <c r="A93" s="155"/>
-      <c r="B93" s="194"/>
+      <c r="B93" s="161"/>
       <c r="C93" s="94" t="e">
         <f>VLOOKUP(A93,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -8317,7 +8325,7 @@
     </row>
     <row r="94" spans="1:32">
       <c r="A94" s="155"/>
-      <c r="B94" s="194"/>
+      <c r="B94" s="161"/>
       <c r="C94" s="94" t="e">
         <f>VLOOKUP(A94,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -8356,7 +8364,7 @@
     </row>
     <row r="95" spans="1:32">
       <c r="A95" s="155"/>
-      <c r="B95" s="194"/>
+      <c r="B95" s="161"/>
       <c r="C95" s="94" t="e">
         <f>VLOOKUP(A95,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -8395,7 +8403,7 @@
     </row>
     <row r="96" spans="1:32">
       <c r="A96" s="155"/>
-      <c r="B96" s="194"/>
+      <c r="B96" s="161"/>
       <c r="C96" s="94" t="e">
         <f>VLOOKUP(A96,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -8434,7 +8442,7 @@
     </row>
     <row r="97" spans="1:32">
       <c r="A97" s="155"/>
-      <c r="B97" s="194"/>
+      <c r="B97" s="161"/>
       <c r="C97" s="94" t="e">
         <f>VLOOKUP(A97,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -8473,7 +8481,7 @@
     </row>
     <row r="98" spans="1:32">
       <c r="A98" s="155"/>
-      <c r="B98" s="194"/>
+      <c r="B98" s="161"/>
       <c r="C98" s="94" t="e">
         <f>VLOOKUP(A98,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -8512,7 +8520,7 @@
     </row>
     <row r="99" spans="1:32">
       <c r="A99" s="155"/>
-      <c r="B99" s="194"/>
+      <c r="B99" s="161"/>
       <c r="C99" s="94" t="e">
         <f>VLOOKUP(A99,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -8551,7 +8559,7 @@
     </row>
     <row r="100" spans="1:32">
       <c r="A100" s="155"/>
-      <c r="B100" s="194"/>
+      <c r="B100" s="161"/>
       <c r="C100" s="94" t="e">
         <f>VLOOKUP(A100,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -8590,7 +8598,7 @@
     </row>
     <row r="101" spans="1:32">
       <c r="A101" s="155"/>
-      <c r="B101" s="194"/>
+      <c r="B101" s="161"/>
       <c r="C101" s="94" t="e">
         <f>VLOOKUP(A101,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -8629,7 +8637,7 @@
     </row>
     <row r="102" spans="1:32">
       <c r="A102" s="155"/>
-      <c r="B102" s="194"/>
+      <c r="B102" s="161"/>
       <c r="C102" s="94" t="e">
         <f>VLOOKUP(A102,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -8668,7 +8676,7 @@
     </row>
     <row r="103" spans="1:32">
       <c r="A103" s="155"/>
-      <c r="B103" s="194"/>
+      <c r="B103" s="161"/>
       <c r="C103" s="94" t="e">
         <f>VLOOKUP(A103,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -8707,7 +8715,7 @@
     </row>
     <row r="104" spans="1:32">
       <c r="A104" s="155"/>
-      <c r="B104" s="194"/>
+      <c r="B104" s="161"/>
       <c r="C104" s="94" t="e">
         <f>VLOOKUP(A104,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -8746,7 +8754,7 @@
     </row>
     <row r="105" spans="1:32">
       <c r="A105" s="155"/>
-      <c r="B105" s="194"/>
+      <c r="B105" s="161"/>
       <c r="C105" s="94" t="e">
         <f>VLOOKUP(A105,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -8785,7 +8793,7 @@
     </row>
     <row r="106" spans="1:32">
       <c r="A106" s="155"/>
-      <c r="B106" s="194"/>
+      <c r="B106" s="161"/>
       <c r="C106" s="94" t="e">
         <f>VLOOKUP(A106,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -8824,7 +8832,7 @@
     </row>
     <row r="107" spans="1:32">
       <c r="A107" s="155"/>
-      <c r="B107" s="194"/>
+      <c r="B107" s="161"/>
       <c r="C107" s="94" t="e">
         <f>VLOOKUP(A107,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -8863,7 +8871,7 @@
     </row>
     <row r="108" spans="1:32">
       <c r="A108" s="155"/>
-      <c r="B108" s="194"/>
+      <c r="B108" s="161"/>
       <c r="C108" s="94" t="e">
         <f>VLOOKUP(A108,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -8902,7 +8910,7 @@
     </row>
     <row r="109" spans="1:32">
       <c r="A109" s="155"/>
-      <c r="B109" s="194"/>
+      <c r="B109" s="161"/>
       <c r="C109" s="94" t="e">
         <f>VLOOKUP(A109,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -8941,7 +8949,7 @@
     </row>
     <row r="110" spans="1:32">
       <c r="A110" s="155"/>
-      <c r="B110" s="194"/>
+      <c r="B110" s="161"/>
       <c r="C110" s="94" t="e">
         <f>VLOOKUP(A110,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -8980,7 +8988,7 @@
     </row>
     <row r="111" spans="1:32">
       <c r="A111" s="155"/>
-      <c r="B111" s="194"/>
+      <c r="B111" s="161"/>
       <c r="C111" s="94" t="e">
         <f>VLOOKUP(A111,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -9019,7 +9027,7 @@
     </row>
     <row r="112" spans="1:32">
       <c r="A112" s="155"/>
-      <c r="B112" s="194"/>
+      <c r="B112" s="161"/>
       <c r="C112" s="94" t="e">
         <f>VLOOKUP(A112,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -9058,7 +9066,7 @@
     </row>
     <row r="113" spans="1:32">
       <c r="A113" s="155"/>
-      <c r="B113" s="194"/>
+      <c r="B113" s="161"/>
       <c r="C113" s="94" t="e">
         <f>VLOOKUP(A113,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -9097,7 +9105,7 @@
     </row>
     <row r="114" spans="1:32">
       <c r="A114" s="155"/>
-      <c r="B114" s="194"/>
+      <c r="B114" s="161"/>
       <c r="C114" s="94" t="e">
         <f>VLOOKUP(A114,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -9136,7 +9144,7 @@
     </row>
     <row r="115" spans="1:32">
       <c r="A115" s="155"/>
-      <c r="B115" s="194"/>
+      <c r="B115" s="161"/>
       <c r="C115" s="94" t="e">
         <f>VLOOKUP(A115,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -9175,7 +9183,7 @@
     </row>
     <row r="116" spans="1:32">
       <c r="A116" s="155"/>
-      <c r="B116" s="194"/>
+      <c r="B116" s="161"/>
       <c r="C116" s="94" t="e">
         <f>VLOOKUP(A116,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -9214,7 +9222,7 @@
     </row>
     <row r="117" spans="1:32">
       <c r="A117" s="155"/>
-      <c r="B117" s="194"/>
+      <c r="B117" s="161"/>
       <c r="C117" s="94" t="e">
         <f>VLOOKUP(A117,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -9253,7 +9261,7 @@
     </row>
     <row r="118" spans="1:32">
       <c r="A118" s="155"/>
-      <c r="B118" s="194"/>
+      <c r="B118" s="161"/>
       <c r="C118" s="94" t="e">
         <f>VLOOKUP(A118,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -9292,7 +9300,7 @@
     </row>
     <row r="119" spans="1:32">
       <c r="A119" s="155"/>
-      <c r="B119" s="194"/>
+      <c r="B119" s="161"/>
       <c r="C119" s="94" t="e">
         <f>VLOOKUP(A119,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -9331,7 +9339,7 @@
     </row>
     <row r="120" spans="1:32">
       <c r="A120" s="155"/>
-      <c r="B120" s="194"/>
+      <c r="B120" s="161"/>
       <c r="C120" s="94" t="e">
         <f>VLOOKUP(A120,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -9370,7 +9378,7 @@
     </row>
     <row r="121" spans="1:32">
       <c r="A121" s="155"/>
-      <c r="B121" s="194"/>
+      <c r="B121" s="161"/>
       <c r="C121" s="94" t="e">
         <f>VLOOKUP(A121,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -9409,7 +9417,7 @@
     </row>
     <row r="122" spans="1:32">
       <c r="A122" s="155"/>
-      <c r="B122" s="194"/>
+      <c r="B122" s="161"/>
       <c r="C122" s="94" t="e">
         <f>VLOOKUP(A122,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -9448,7 +9456,7 @@
     </row>
     <row r="123" spans="1:32">
       <c r="A123" s="155"/>
-      <c r="B123" s="194"/>
+      <c r="B123" s="161"/>
       <c r="C123" s="94" t="e">
         <f>VLOOKUP(A123,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -9487,7 +9495,7 @@
     </row>
     <row r="124" spans="1:32">
       <c r="A124" s="155"/>
-      <c r="B124" s="194"/>
+      <c r="B124" s="161"/>
       <c r="C124" s="94" t="e">
         <f>VLOOKUP(A124,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -9526,7 +9534,7 @@
     </row>
     <row r="125" spans="1:32">
       <c r="A125" s="155"/>
-      <c r="B125" s="194"/>
+      <c r="B125" s="161"/>
       <c r="C125" s="94" t="e">
         <f>VLOOKUP(A125,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -9565,7 +9573,7 @@
     </row>
     <row r="126" spans="1:32">
       <c r="A126" s="155"/>
-      <c r="B126" s="194"/>
+      <c r="B126" s="161"/>
       <c r="C126" s="94" t="e">
         <f>VLOOKUP(A126,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -9604,7 +9612,7 @@
     </row>
     <row r="127" spans="1:32">
       <c r="A127" s="155"/>
-      <c r="B127" s="194"/>
+      <c r="B127" s="161"/>
       <c r="C127" s="94" t="e">
         <f>VLOOKUP(A127,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -9643,7 +9651,7 @@
     </row>
     <row r="128" spans="1:32">
       <c r="A128" s="155"/>
-      <c r="B128" s="194"/>
+      <c r="B128" s="161"/>
       <c r="C128" s="94" t="e">
         <f>VLOOKUP(A128,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -9682,7 +9690,7 @@
     </row>
     <row r="129" spans="1:32">
       <c r="A129" s="155"/>
-      <c r="B129" s="194"/>
+      <c r="B129" s="161"/>
       <c r="C129" s="94" t="e">
         <f>VLOOKUP(A129,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -9721,7 +9729,7 @@
     </row>
     <row r="130" spans="1:32">
       <c r="A130" s="155"/>
-      <c r="B130" s="194"/>
+      <c r="B130" s="161"/>
       <c r="C130" s="94" t="e">
         <f>VLOOKUP(A130,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -9760,7 +9768,7 @@
     </row>
     <row r="131" spans="1:32">
       <c r="A131" s="155"/>
-      <c r="B131" s="194"/>
+      <c r="B131" s="161"/>
       <c r="C131" s="94" t="e">
         <f>VLOOKUP(A131,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -9799,7 +9807,7 @@
     </row>
     <row r="132" spans="1:32">
       <c r="A132" s="155"/>
-      <c r="B132" s="194"/>
+      <c r="B132" s="161"/>
       <c r="C132" s="94" t="e">
         <f>VLOOKUP(A132,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -9838,7 +9846,7 @@
     </row>
     <row r="133" spans="1:32">
       <c r="A133" s="155"/>
-      <c r="B133" s="194"/>
+      <c r="B133" s="161"/>
       <c r="C133" s="94" t="e">
         <f>VLOOKUP(A133,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -9877,7 +9885,7 @@
     </row>
     <row r="134" spans="1:32">
       <c r="A134" s="155"/>
-      <c r="B134" s="194"/>
+      <c r="B134" s="161"/>
       <c r="C134" s="94" t="e">
         <f>VLOOKUP(A134,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -9916,7 +9924,7 @@
     </row>
     <row r="135" spans="1:32">
       <c r="A135" s="155"/>
-      <c r="B135" s="194"/>
+      <c r="B135" s="161"/>
       <c r="C135" s="94" t="e">
         <f>VLOOKUP(A135,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -9955,7 +9963,7 @@
     </row>
     <row r="136" spans="1:32">
       <c r="A136" s="155"/>
-      <c r="B136" s="194"/>
+      <c r="B136" s="161"/>
       <c r="C136" s="94" t="e">
         <f>VLOOKUP(A136,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -9994,7 +10002,7 @@
     </row>
     <row r="137" spans="1:32">
       <c r="A137" s="155"/>
-      <c r="B137" s="194"/>
+      <c r="B137" s="161"/>
       <c r="C137" s="94" t="e">
         <f>VLOOKUP(A137,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -10033,7 +10041,7 @@
     </row>
     <row r="138" spans="1:32">
       <c r="A138" s="155"/>
-      <c r="B138" s="194"/>
+      <c r="B138" s="161"/>
       <c r="C138" s="94" t="e">
         <f>VLOOKUP(A138,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -10072,7 +10080,7 @@
     </row>
     <row r="139" spans="1:32">
       <c r="A139" s="155"/>
-      <c r="B139" s="194"/>
+      <c r="B139" s="161"/>
       <c r="C139" s="94" t="e">
         <f>VLOOKUP(A139,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -10111,7 +10119,7 @@
     </row>
     <row r="140" spans="1:32">
       <c r="A140" s="155"/>
-      <c r="B140" s="194"/>
+      <c r="B140" s="161"/>
       <c r="C140" s="94" t="e">
         <f>VLOOKUP(A140,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -10150,7 +10158,7 @@
     </row>
     <row r="141" spans="1:32">
       <c r="A141" s="155"/>
-      <c r="B141" s="194"/>
+      <c r="B141" s="161"/>
       <c r="C141" s="94" t="e">
         <f>VLOOKUP(A141,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -10189,7 +10197,7 @@
     </row>
     <row r="142" spans="1:32">
       <c r="A142" s="155"/>
-      <c r="B142" s="194"/>
+      <c r="B142" s="161"/>
       <c r="C142" s="94" t="e">
         <f>VLOOKUP(A142,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -10228,7 +10236,7 @@
     </row>
     <row r="143" spans="1:32">
       <c r="A143" s="155"/>
-      <c r="B143" s="194"/>
+      <c r="B143" s="161"/>
       <c r="C143" s="94" t="e">
         <f>VLOOKUP(A143,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -10267,7 +10275,7 @@
     </row>
     <row r="144" spans="1:32">
       <c r="A144" s="155"/>
-      <c r="B144" s="194"/>
+      <c r="B144" s="161"/>
       <c r="C144" s="94" t="e">
         <f>VLOOKUP(A144,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -10306,7 +10314,7 @@
     </row>
     <row r="145" spans="1:32">
       <c r="A145" s="155"/>
-      <c r="B145" s="194"/>
+      <c r="B145" s="161"/>
       <c r="C145" s="94" t="e">
         <f>VLOOKUP(A145,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -10345,7 +10353,7 @@
     </row>
     <row r="146" spans="1:32">
       <c r="A146" s="155"/>
-      <c r="B146" s="194"/>
+      <c r="B146" s="161"/>
       <c r="C146" s="94" t="e">
         <f>VLOOKUP(A146,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -10384,7 +10392,7 @@
     </row>
     <row r="147" spans="1:32">
       <c r="A147" s="155"/>
-      <c r="B147" s="194"/>
+      <c r="B147" s="161"/>
       <c r="C147" s="94" t="e">
         <f>VLOOKUP(A147,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -10423,7 +10431,7 @@
     </row>
     <row r="148" spans="1:32">
       <c r="A148" s="155"/>
-      <c r="B148" s="194"/>
+      <c r="B148" s="161"/>
       <c r="C148" s="94" t="e">
         <f>VLOOKUP(A148,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -10462,7 +10470,7 @@
     </row>
     <row r="149" spans="1:32">
       <c r="A149" s="155"/>
-      <c r="B149" s="194"/>
+      <c r="B149" s="161"/>
       <c r="C149" s="94" t="e">
         <f>VLOOKUP(A149,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -10501,7 +10509,7 @@
     </row>
     <row r="150" spans="1:32">
       <c r="A150" s="155"/>
-      <c r="B150" s="194"/>
+      <c r="B150" s="161"/>
       <c r="C150" s="94" t="e">
         <f>VLOOKUP(A150,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -10540,7 +10548,7 @@
     </row>
     <row r="151" spans="1:32">
       <c r="A151" s="155"/>
-      <c r="B151" s="194"/>
+      <c r="B151" s="161"/>
       <c r="C151" s="94" t="e">
         <f>VLOOKUP(A151,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -10579,7 +10587,7 @@
     </row>
     <row r="152" spans="1:32">
       <c r="A152" s="155"/>
-      <c r="B152" s="194"/>
+      <c r="B152" s="161"/>
       <c r="C152" s="94" t="e">
         <f>VLOOKUP(A152,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -10618,7 +10626,7 @@
     </row>
     <row r="153" spans="1:32">
       <c r="A153" s="155"/>
-      <c r="B153" s="194"/>
+      <c r="B153" s="161"/>
       <c r="C153" s="94" t="e">
         <f>VLOOKUP(A153,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -10657,7 +10665,7 @@
     </row>
     <row r="154" spans="1:32">
       <c r="A154" s="155"/>
-      <c r="B154" s="194"/>
+      <c r="B154" s="161"/>
       <c r="C154" s="94" t="e">
         <f>VLOOKUP(A154,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -10696,7 +10704,7 @@
     </row>
     <row r="155" spans="1:32">
       <c r="A155" s="155"/>
-      <c r="B155" s="194"/>
+      <c r="B155" s="161"/>
       <c r="C155" s="94" t="e">
         <f>VLOOKUP(A155,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -10735,7 +10743,7 @@
     </row>
     <row r="156" spans="1:32">
       <c r="A156" s="155"/>
-      <c r="B156" s="194"/>
+      <c r="B156" s="161"/>
       <c r="C156" s="94" t="e">
         <f>VLOOKUP(A156,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -10774,7 +10782,7 @@
     </row>
     <row r="157" spans="1:32">
       <c r="A157" s="155"/>
-      <c r="B157" s="194"/>
+      <c r="B157" s="161"/>
       <c r="C157" s="94" t="e">
         <f>VLOOKUP(A157,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -10813,7 +10821,7 @@
     </row>
     <row r="158" spans="1:32">
       <c r="A158" s="155"/>
-      <c r="B158" s="194"/>
+      <c r="B158" s="161"/>
       <c r="C158" s="94" t="e">
         <f>VLOOKUP(A158,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -10852,7 +10860,7 @@
     </row>
     <row r="159" spans="1:32">
       <c r="A159" s="155"/>
-      <c r="B159" s="194"/>
+      <c r="B159" s="161"/>
       <c r="C159" s="94" t="e">
         <f>VLOOKUP(A159,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -10891,7 +10899,7 @@
     </row>
     <row r="160" spans="1:32">
       <c r="A160" s="155"/>
-      <c r="B160" s="194"/>
+      <c r="B160" s="161"/>
       <c r="C160" s="94" t="e">
         <f>VLOOKUP(A160,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -10930,7 +10938,7 @@
     </row>
     <row r="161" spans="1:32">
       <c r="A161" s="155"/>
-      <c r="B161" s="194"/>
+      <c r="B161" s="161"/>
       <c r="C161" s="94" t="e">
         <f>VLOOKUP(A161,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -10969,7 +10977,7 @@
     </row>
     <row r="162" spans="1:32">
       <c r="A162" s="155"/>
-      <c r="B162" s="194"/>
+      <c r="B162" s="161"/>
       <c r="C162" s="94" t="e">
         <f>VLOOKUP(A162,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -11008,7 +11016,7 @@
     </row>
     <row r="163" spans="1:32">
       <c r="A163" s="155"/>
-      <c r="B163" s="194"/>
+      <c r="B163" s="161"/>
       <c r="C163" s="94" t="e">
         <f>VLOOKUP(A163,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -11047,7 +11055,7 @@
     </row>
     <row r="164" spans="1:32">
       <c r="A164" s="155"/>
-      <c r="B164" s="194"/>
+      <c r="B164" s="161"/>
       <c r="C164" s="94" t="e">
         <f>VLOOKUP(A164,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -11086,7 +11094,7 @@
     </row>
     <row r="165" spans="1:32">
       <c r="A165" s="155"/>
-      <c r="B165" s="194"/>
+      <c r="B165" s="161"/>
       <c r="C165" s="94" t="e">
         <f>VLOOKUP(A165,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -11125,7 +11133,7 @@
     </row>
     <row r="166" spans="1:32">
       <c r="A166" s="155"/>
-      <c r="B166" s="194"/>
+      <c r="B166" s="161"/>
       <c r="C166" s="94" t="e">
         <f>VLOOKUP(A166,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -11164,7 +11172,7 @@
     </row>
     <row r="167" spans="1:32">
       <c r="A167" s="155"/>
-      <c r="B167" s="194"/>
+      <c r="B167" s="161"/>
       <c r="C167" s="94" t="e">
         <f>VLOOKUP(A167,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -11203,7 +11211,7 @@
     </row>
     <row r="168" spans="1:32">
       <c r="A168" s="155"/>
-      <c r="B168" s="194"/>
+      <c r="B168" s="161"/>
       <c r="C168" s="94" t="e">
         <f>VLOOKUP(A168,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -11242,7 +11250,7 @@
     </row>
     <row r="169" spans="1:32">
       <c r="A169" s="155"/>
-      <c r="B169" s="194"/>
+      <c r="B169" s="161"/>
       <c r="C169" s="94" t="e">
         <f>VLOOKUP(A169,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -11281,7 +11289,7 @@
     </row>
     <row r="170" spans="1:32">
       <c r="A170" s="155"/>
-      <c r="B170" s="194"/>
+      <c r="B170" s="161"/>
       <c r="C170" s="94" t="e">
         <f>VLOOKUP(A170,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -11320,7 +11328,7 @@
     </row>
     <row r="171" spans="1:32">
       <c r="A171" s="155"/>
-      <c r="B171" s="194"/>
+      <c r="B171" s="161"/>
       <c r="C171" s="94" t="e">
         <f>VLOOKUP(A171,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -11359,7 +11367,7 @@
     </row>
     <row r="172" spans="1:32">
       <c r="A172" s="155"/>
-      <c r="B172" s="194"/>
+      <c r="B172" s="161"/>
       <c r="C172" s="94" t="e">
         <f>VLOOKUP(A172,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -11398,7 +11406,7 @@
     </row>
     <row r="173" spans="1:32">
       <c r="A173" s="155"/>
-      <c r="B173" s="194"/>
+      <c r="B173" s="161"/>
       <c r="C173" s="94" t="e">
         <f>VLOOKUP(A173,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -11437,7 +11445,7 @@
     </row>
     <row r="174" spans="1:32">
       <c r="A174" s="155"/>
-      <c r="B174" s="194"/>
+      <c r="B174" s="161"/>
       <c r="C174" s="94" t="e">
         <f>VLOOKUP(A174,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -11476,7 +11484,7 @@
     </row>
     <row r="175" spans="1:32">
       <c r="A175" s="155"/>
-      <c r="B175" s="194"/>
+      <c r="B175" s="161"/>
       <c r="C175" s="94" t="e">
         <f>VLOOKUP(A175,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -11515,7 +11523,7 @@
     </row>
     <row r="176" spans="1:32">
       <c r="A176" s="155"/>
-      <c r="B176" s="194"/>
+      <c r="B176" s="161"/>
       <c r="C176" s="94" t="e">
         <f>VLOOKUP(A176,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -11554,7 +11562,7 @@
     </row>
     <row r="177" spans="1:32">
       <c r="A177" s="156"/>
-      <c r="B177" s="194"/>
+      <c r="B177" s="161"/>
       <c r="C177" s="94" t="e">
         <f>VLOOKUP(A177,'Load case definition'!$A$7:$C$180,3,FALSE)</f>
         <v>#N/A</v>
@@ -11595,8 +11603,8 @@
   <mergeCells count="27">
     <mergeCell ref="AC1:AF1"/>
     <mergeCell ref="A2:A7"/>
+    <mergeCell ref="AD2:AD7"/>
     <mergeCell ref="C2:C7"/>
-    <mergeCell ref="AD2:AD7"/>
     <mergeCell ref="AF2:AF7"/>
     <mergeCell ref="E2:E7"/>
     <mergeCell ref="W3:X7"/>
@@ -11611,8 +11619,8 @@
     <mergeCell ref="D2:D7"/>
     <mergeCell ref="F2:F7"/>
     <mergeCell ref="H2:H7"/>
+    <mergeCell ref="S3:U6"/>
     <mergeCell ref="Y3:Y7"/>
-    <mergeCell ref="S3:U6"/>
     <mergeCell ref="P3:R7"/>
     <mergeCell ref="S7:U7"/>
     <mergeCell ref="M7:O7"/>
@@ -11751,9 +11759,9 @@
       <formula1>1</formula1>
       <formula2>150</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="1-Projected, 0- Not projected_x000a_" sqref="Y3:Y7" xr:uid="{00000000-0002-0000-0100-000017000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="1, 0 - For load on contour auto detect panels_x000a_" sqref="Z3:Z7" xr:uid="{00000000-0002-0000-0100-000018000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H8:H177" xr:uid="{7F8ACE34-5166-49D6-A57A-72F756B526CD}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="1-Projected, 0- Not projected_x000a_" sqref="Y3:Y7" xr:uid="{00000000-0002-0000-0100-000016000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="1, 0 - For load on contour auto detect panels_x000a_" sqref="Z3:Z7" xr:uid="{00000000-0002-0000-0100-000017000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H8:H177" xr:uid="{00000000-0002-0000-0100-000018000000}">
       <formula1>"(FE) uniform, nodal force, Body forces, member force, self-weight, trapezoidal load (2p), uniform load, (FE) linear load on edges, load on contour, load 3p on contour"</formula1>
     </dataValidation>
   </dataValidations>
@@ -12164,17 +12172,17 @@
     </row>
     <row r="3" spans="1:4605" s="7" customFormat="1" ht="218.65" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="92" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="108" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F3" s="108" t="s">
         <v>7</v>
@@ -16787,12 +16795,12 @@
       <c r="A4" s="3"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
-      <c r="D4" s="186" t="s">
+      <c r="D4" s="188" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="172"/>
-      <c r="F4" s="172"/>
-      <c r="G4" s="172"/>
+      <c r="E4" s="174"/>
+      <c r="F4" s="174"/>
+      <c r="G4" s="174"/>
       <c r="H4" s="123">
         <v>1</v>
       </c>
@@ -21398,10 +21406,10 @@
       <c r="A5" s="33"/>
       <c r="B5" s="23"/>
       <c r="C5" s="23"/>
-      <c r="D5" s="177"/>
-      <c r="E5" s="166"/>
-      <c r="F5" s="166"/>
-      <c r="G5" s="166"/>
+      <c r="D5" s="179"/>
+      <c r="E5" s="167"/>
+      <c r="F5" s="167"/>
+      <c r="G5" s="167"/>
       <c r="H5" s="123"/>
       <c r="I5" s="123"/>
       <c r="J5" s="123"/>
@@ -21773,25 +21781,25 @@
     </row>
     <row r="6" spans="1:4605" s="16" customFormat="1" ht="14.45" customHeight="1">
       <c r="A6" s="13" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D6" s="89" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E6" s="89" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F6" s="89" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="G6" s="89" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:4605" s="16" customFormat="1">
@@ -32290,77 +32298,89 @@
   </sheetPr>
   <dimension ref="A1:W16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J41" sqref="J41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <sheetData>
     <row r="1" spans="1:23">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>65</v>
+      </c>
+      <c r="B1" t="s">
+        <v>66</v>
       </c>
       <c r="G1" t="s">
-        <v>64</v>
+        <v>65</v>
+      </c>
+      <c r="H1" t="s">
+        <v>67</v>
       </c>
       <c r="M1" t="s">
         <v>65</v>
       </c>
+      <c r="N1" t="s">
+        <v>68</v>
+      </c>
       <c r="S1" t="s">
-        <v>66</v>
+        <v>65</v>
+      </c>
+      <c r="T1" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:23">
       <c r="A2" s="145" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B2" s="145" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C2" s="145" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" t="s">
         <v>70</v>
       </c>
-      <c r="D2" t="s">
+      <c r="H2" t="s">
         <v>71</v>
       </c>
-      <c r="G2" t="s">
-        <v>68</v>
-      </c>
-      <c r="H2" t="s">
-        <v>69</v>
-      </c>
       <c r="I2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J2" t="s">
+        <v>73</v>
+      </c>
+      <c r="M2" t="s">
         <v>70</v>
       </c>
-      <c r="J2" t="s">
+      <c r="N2" t="s">
         <v>71</v>
       </c>
-      <c r="M2" t="s">
-        <v>68</v>
-      </c>
-      <c r="N2" t="s">
-        <v>69</v>
-      </c>
       <c r="O2" t="s">
+        <v>72</v>
+      </c>
+      <c r="P2" t="s">
+        <v>73</v>
+      </c>
+      <c r="S2" t="s">
         <v>70</v>
       </c>
-      <c r="P2" t="s">
+      <c r="T2" t="s">
         <v>71</v>
       </c>
-      <c r="S2" t="s">
-        <v>68</v>
-      </c>
-      <c r="T2" t="s">
-        <v>69</v>
-      </c>
       <c r="U2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="V2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="W2" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:23">
@@ -32413,7 +32433,7 @@
         <v>0</v>
       </c>
       <c r="W3" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:23">
@@ -32466,7 +32486,7 @@
         <v>0</v>
       </c>
       <c r="W4" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:23">
@@ -32519,7 +32539,7 @@
         <v>0</v>
       </c>
       <c r="W5" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:23">
@@ -32706,6 +32726,437 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BA9356C-2006-43BE-87F9-E2FE5DB18E00}">
+  <dimension ref="A1:W16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q38" sqref="Q38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetData>
+    <row r="1" spans="1:23">
+      <c r="A1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" t="s">
+        <v>67</v>
+      </c>
+      <c r="M1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S1" t="s">
+        <v>65</v>
+      </c>
+      <c r="T1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23">
+      <c r="A2" s="145" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="145" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="145" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J2" t="s">
+        <v>73</v>
+      </c>
+      <c r="M2" t="s">
+        <v>70</v>
+      </c>
+      <c r="N2" t="s">
+        <v>71</v>
+      </c>
+      <c r="O2" t="s">
+        <v>72</v>
+      </c>
+      <c r="P2" t="s">
+        <v>73</v>
+      </c>
+      <c r="S2" t="s">
+        <v>70</v>
+      </c>
+      <c r="T2" t="s">
+        <v>71</v>
+      </c>
+      <c r="U2" t="s">
+        <v>72</v>
+      </c>
+      <c r="V2" t="s">
+        <v>73</v>
+      </c>
+      <c r="W2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>3</v>
+      </c>
+      <c r="I3">
+        <v>-1.5</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>5</v>
+      </c>
+      <c r="O3">
+        <v>-1.5</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>1</v>
+      </c>
+      <c r="T3">
+        <v>2.5</v>
+      </c>
+      <c r="U3">
+        <v>0.5</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="I4">
+        <v>-0.5</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>2</v>
+      </c>
+      <c r="N4">
+        <v>5</v>
+      </c>
+      <c r="O4">
+        <v>-1</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>2</v>
+      </c>
+      <c r="T4">
+        <v>3</v>
+      </c>
+      <c r="U4">
+        <v>1</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5">
+        <v>-0.5</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>3</v>
+      </c>
+      <c r="N5">
+        <v>5.5</v>
+      </c>
+      <c r="O5">
+        <v>-0.5</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>3</v>
+      </c>
+      <c r="T5">
+        <v>3.5</v>
+      </c>
+      <c r="U5">
+        <v>0.5</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>4</v>
+      </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
+      <c r="I6">
+        <v>-1.5</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>4</v>
+      </c>
+      <c r="N6">
+        <v>6</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23">
+      <c r="M7">
+        <v>5</v>
+      </c>
+      <c r="N7">
+        <v>6.5</v>
+      </c>
+      <c r="O7">
+        <v>0.5</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23">
+      <c r="M8">
+        <v>6</v>
+      </c>
+      <c r="N8">
+        <v>7</v>
+      </c>
+      <c r="O8">
+        <v>0.5</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23">
+      <c r="M9">
+        <v>7</v>
+      </c>
+      <c r="N9">
+        <v>7</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23">
+      <c r="M10">
+        <v>8</v>
+      </c>
+      <c r="N10">
+        <v>7.5</v>
+      </c>
+      <c r="O10">
+        <v>-0.5</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23">
+      <c r="M11">
+        <v>9</v>
+      </c>
+      <c r="N11">
+        <v>7.5</v>
+      </c>
+      <c r="O11">
+        <v>-1</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23">
+      <c r="M12">
+        <v>10</v>
+      </c>
+      <c r="N12">
+        <v>7</v>
+      </c>
+      <c r="O12">
+        <v>-1</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23">
+      <c r="M13">
+        <v>11</v>
+      </c>
+      <c r="N13">
+        <v>7</v>
+      </c>
+      <c r="O13">
+        <v>-1.5</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23">
+      <c r="M14">
+        <v>12</v>
+      </c>
+      <c r="N14">
+        <v>6.5</v>
+      </c>
+      <c r="O14">
+        <v>-1.5</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23">
+      <c r="M15">
+        <v>13</v>
+      </c>
+      <c r="N15">
+        <v>6</v>
+      </c>
+      <c r="O15">
+        <v>-1</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23">
+      <c r="M16">
+        <v>14</v>
+      </c>
+      <c r="N16">
+        <v>6</v>
+      </c>
+      <c r="O16">
+        <v>-1.5</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="ScreenCapture">
     <tabColor theme="0"/>
@@ -32729,8 +33180,8 @@
     <col min="29" max="33" width="5.7109375" style="35" customWidth="1"/>
     <col min="34" max="49" width="8.7109375" style="35" customWidth="1"/>
     <col min="50" max="50" width="9.42578125" style="35" customWidth="1"/>
-    <col min="51" max="62" width="8.7109375" style="35" customWidth="1"/>
-    <col min="63" max="16384" width="8.7109375" style="35"/>
+    <col min="51" max="63" width="8.7109375" style="35" customWidth="1"/>
+    <col min="64" max="16384" width="8.7109375" style="35"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:55" ht="62.1" customHeight="1" thickBot="1">
@@ -32795,246 +33246,246 @@
       <c r="D3" s="46"/>
       <c r="E3" s="51"/>
       <c r="F3" s="72"/>
-      <c r="G3" s="191" t="s">
-        <v>75</v>
-      </c>
-      <c r="H3" s="169"/>
-      <c r="I3" s="169"/>
-      <c r="J3" s="169"/>
-      <c r="K3" s="169"/>
-      <c r="L3" s="169"/>
-      <c r="M3" s="169"/>
-      <c r="N3" s="169"/>
-      <c r="O3" s="170"/>
-      <c r="P3" s="189" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q3" s="169"/>
-      <c r="R3" s="169"/>
-      <c r="S3" s="169"/>
-      <c r="T3" s="169"/>
-      <c r="U3" s="169"/>
-      <c r="V3" s="169"/>
-      <c r="W3" s="170"/>
-      <c r="X3" s="189" t="s">
-        <v>77</v>
-      </c>
-      <c r="Y3" s="169"/>
-      <c r="Z3" s="170"/>
-      <c r="AA3" s="188" t="s">
+      <c r="G3" s="193" t="s">
         <v>78</v>
       </c>
-      <c r="AB3" s="169"/>
-      <c r="AC3" s="190" t="s">
+      <c r="H3" s="171"/>
+      <c r="I3" s="171"/>
+      <c r="J3" s="171"/>
+      <c r="K3" s="171"/>
+      <c r="L3" s="171"/>
+      <c r="M3" s="171"/>
+      <c r="N3" s="171"/>
+      <c r="O3" s="172"/>
+      <c r="P3" s="191" t="s">
         <v>79</v>
       </c>
-      <c r="AD3" s="172"/>
-      <c r="AE3" s="173"/>
+      <c r="Q3" s="171"/>
+      <c r="R3" s="171"/>
+      <c r="S3" s="171"/>
+      <c r="T3" s="171"/>
+      <c r="U3" s="171"/>
+      <c r="V3" s="171"/>
+      <c r="W3" s="172"/>
+      <c r="X3" s="191" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y3" s="171"/>
+      <c r="Z3" s="172"/>
+      <c r="AA3" s="190" t="s">
+        <v>81</v>
+      </c>
+      <c r="AB3" s="171"/>
+      <c r="AC3" s="192" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD3" s="174"/>
+      <c r="AE3" s="175"/>
       <c r="AF3" s="134" t="s">
-        <v>80</v>
-      </c>
-      <c r="AG3" s="189" t="s">
-        <v>81</v>
-      </c>
-      <c r="AH3" s="169"/>
-      <c r="AI3" s="169"/>
-      <c r="AJ3" s="169"/>
-      <c r="AK3" s="169"/>
-      <c r="AL3" s="169"/>
-      <c r="AM3" s="169"/>
-      <c r="AN3" s="170"/>
-      <c r="AO3" s="187" t="s">
-        <v>82</v>
-      </c>
-      <c r="AP3" s="169"/>
-      <c r="AQ3" s="169"/>
-      <c r="AR3" s="169"/>
-      <c r="AS3" s="169"/>
-      <c r="AT3" s="169"/>
-      <c r="AU3" s="169"/>
-      <c r="AV3" s="187" t="s">
         <v>83</v>
       </c>
-      <c r="AW3" s="169"/>
-      <c r="AX3" s="169"/>
-      <c r="AY3" s="169"/>
-      <c r="AZ3" s="169"/>
-      <c r="BA3" s="189" t="s">
+      <c r="AG3" s="191" t="s">
         <v>84</v>
       </c>
-      <c r="BB3" s="169"/>
-      <c r="BC3" s="170"/>
+      <c r="AH3" s="171"/>
+      <c r="AI3" s="171"/>
+      <c r="AJ3" s="171"/>
+      <c r="AK3" s="171"/>
+      <c r="AL3" s="171"/>
+      <c r="AM3" s="171"/>
+      <c r="AN3" s="172"/>
+      <c r="AO3" s="189" t="s">
+        <v>85</v>
+      </c>
+      <c r="AP3" s="171"/>
+      <c r="AQ3" s="171"/>
+      <c r="AR3" s="171"/>
+      <c r="AS3" s="171"/>
+      <c r="AT3" s="171"/>
+      <c r="AU3" s="171"/>
+      <c r="AV3" s="189" t="s">
+        <v>86</v>
+      </c>
+      <c r="AW3" s="171"/>
+      <c r="AX3" s="171"/>
+      <c r="AY3" s="171"/>
+      <c r="AZ3" s="171"/>
+      <c r="BA3" s="191" t="s">
+        <v>87</v>
+      </c>
+      <c r="BB3" s="171"/>
+      <c r="BC3" s="172"/>
     </row>
     <row r="4" spans="1:55" ht="111" customHeight="1">
       <c r="A4" s="42" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B4" s="42" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C4" s="42" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="D4" s="41" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E4" s="44" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="F4" s="73" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="G4" s="43" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="H4" s="43" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="I4" s="43" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="J4" s="43" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="K4" s="43" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="L4" s="43" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="M4" s="43" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="N4" s="43" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="O4" s="43" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="P4" s="44" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="Q4" s="43" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="R4" s="43" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="S4" s="43" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="T4" s="43" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="U4" s="43" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="V4" s="43" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="W4" s="43" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="X4" s="44" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="Y4" s="43" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="Z4" s="43" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="AA4" s="44" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="AB4" s="43" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="AC4" s="44" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="AD4" s="43" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="AE4" s="42" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="AF4" s="41" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="AG4" s="135" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="AH4" s="136" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="AI4" s="135" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="AJ4" s="135" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="AK4" s="135" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="AL4" s="136" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="AM4" s="135" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="AN4" s="137" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="AO4" s="41" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="AP4" s="41" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="AQ4" s="41" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="AR4" s="41" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="AS4" s="41" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="AT4" s="41" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="AU4" s="136" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="AV4" s="41" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="AW4" s="41" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="AX4" s="41" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="AY4" s="41" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="AZ4" s="41" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="BA4" s="41" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="BB4" s="41" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="BC4" s="41" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:55">
       <c r="A5" s="40" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B5" s="40" t="e">
         <f>PlatformName &amp; " Robot layout"</f>
@@ -33196,7 +33647,7 @@
     </row>
     <row r="6" spans="1:55">
       <c r="A6" s="40" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B6" s="40" t="e">
         <f>PlatformName &amp; " Robot layout plan"</f>
@@ -33358,7 +33809,7 @@
     </row>
     <row r="7" spans="1:55">
       <c r="A7" s="40" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B7" s="40" t="e">
         <f>PlatformName &amp; " Robot layout plan cladding"</f>
@@ -33520,7 +33971,7 @@
     </row>
     <row r="8" spans="1:55">
       <c r="A8" s="40" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B8" s="40" t="e">
         <f>PlatformName &amp; " Robot boundary conditions and connections"</f>
@@ -33682,7 +34133,7 @@
     </row>
     <row r="9" spans="1:55">
       <c r="A9" s="40" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B9" s="40" t="e">
         <f>PlatformName &amp; " Utilised members"</f>
@@ -34758,7 +35209,7 @@
     <row r="26" spans="1:55" ht="15.75" customHeight="1" thickBot="1">
       <c r="A26" s="55"/>
       <c r="B26" s="56" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="C26" s="57"/>
       <c r="D26" s="57"/>
@@ -34919,16 +35370,16 @@
         <v>1</v>
       </c>
       <c r="B27" s="49" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C27" s="48" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="D27" s="48" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="E27" s="47" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="F27" s="76">
         <v>0</v>
@@ -37110,7 +37561,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="LaTeXCode">
     <tabColor theme="1" tint="0.499984740745262"/>
@@ -37137,13 +37588,13 @@
     <col min="12" max="18" width="8.7109375" style="19" customWidth="1"/>
     <col min="19" max="19" width="18.42578125" style="19" customWidth="1"/>
     <col min="20" max="20" width="15.28515625" style="19" customWidth="1"/>
-    <col min="21" max="32" width="8.7109375" style="19" customWidth="1"/>
-    <col min="33" max="16384" width="8.7109375" style="19"/>
+    <col min="21" max="33" width="8.7109375" style="19" customWidth="1"/>
+    <col min="34" max="16384" width="8.7109375" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="13.5" customHeight="1" thickBot="1">
       <c r="A1" s="19" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="F1" s="26">
         <v>0.5</v>
@@ -37152,45 +37603,45 @@
         <v>0.1</v>
       </c>
       <c r="M1" s="19" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="S1" s="19" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="15.75" customHeight="1">
       <c r="A2" s="19" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="F2" s="19" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="G2" s="19" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="H2" s="27" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="J2" s="19" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="K2" s="19" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="M2" s="19" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="N2" s="19" t="s">
         <v>52</v>
@@ -37199,30 +37650,30 @@
         <v>1</v>
       </c>
       <c r="P2" s="19" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="S2" s="19" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="T2" s="19" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="39" customHeight="1">
       <c r="A3" s="19" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="C3" s="19" t="s">
         <v>52</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="F3" s="27" t="e">
         <f>PlatformName &amp;" member utilisations $&gt;" &amp;F1&amp;"$"</f>
@@ -37237,13 +37688,13 @@
         <v>#REF!</v>
       </c>
       <c r="J3" s="28" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="K3" s="27" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="M3" s="19" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="N3" s="19" t="s">
         <v>52</v>
@@ -37252,42 +37703,42 @@
         <v>1</v>
       </c>
       <c r="P3" s="19" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="S3" s="19" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="T3" s="28" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="15.75" customHeight="1">
       <c r="A4" s="19" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="G4" s="19" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="H4" s="27" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="M4" s="19" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="N4" s="19" t="s">
         <v>52</v>
@@ -37296,36 +37747,36 @@
         <v>1</v>
       </c>
       <c r="P4" s="19" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="S4" s="19" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="15.75" customHeight="1">
       <c r="B5" s="19" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="H5" s="27" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="M5" s="19" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="N5" s="19" t="s">
         <v>52</v>
@@ -37334,10 +37785,10 @@
         <v>1</v>
       </c>
       <c r="P5" s="19" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="S5" s="19" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="15.75" customHeight="1">
@@ -37366,10 +37817,10 @@
         <v>#REF!</v>
       </c>
       <c r="H6" s="27" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="M6" s="19" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="N6" s="19" t="s">
         <v>52</v>
@@ -37378,7 +37829,7 @@
         <v>1</v>
       </c>
       <c r="P6" s="19" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="S6" s="19" t="e">
         <f>"\includegraphics[width=\textwidth]{\"&amp;LaTeXFiguresFolder &amp;"\"&amp;PlatformName&amp; " "&amp;S3&amp;".png} "</f>
@@ -37411,14 +37862,14 @@
         <v>#REF!</v>
       </c>
       <c r="H7" s="27" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="J7" s="19">
         <f>COLUMN(J1)</f>
         <v>10</v>
       </c>
       <c r="M7" s="19" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="N7" s="19" t="s">
         <v>52</v>
@@ -37427,36 +37878,36 @@
         <v>1</v>
       </c>
       <c r="P7" s="19" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="S7" s="19" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="15.75" customHeight="1">
       <c r="B8" s="19" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="G8" s="19" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="H8" s="27" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="M8" s="19" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="N8" s="19" t="s">
         <v>52</v>
@@ -37465,7 +37916,7 @@
         <v>1</v>
       </c>
       <c r="P8" s="19" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="S8" s="19" t="e">
         <f>"    \caption{" &amp;PlatformName&amp; " " &amp; S3 &amp;".}"</f>
@@ -37474,28 +37925,28 @@
     </row>
     <row r="9" spans="1:20" ht="15.75" customHeight="1">
       <c r="B9" s="19" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="G9" s="19" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="H9" s="27" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="M9" s="19" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="N9" s="19" t="s">
         <v>52</v>
@@ -37504,7 +37955,7 @@
         <v>1</v>
       </c>
       <c r="P9" s="19" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="S9" s="19" t="e">
         <f>"    \label{tabl:" &amp; PlatformName &amp;" "&amp;S3 &amp;"}"</f>
@@ -37513,28 +37964,28 @@
     </row>
     <row r="10" spans="1:20" ht="16.5" customHeight="1">
       <c r="B10" s="85" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="G10" s="19" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="H10" s="27" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="M10" s="19" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="N10" s="19" t="s">
         <v>52</v>
@@ -37543,33 +37994,33 @@
         <v>1</v>
       </c>
       <c r="P10" s="19" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="11" spans="1:20" ht="16.5" customHeight="1">
       <c r="B11" s="85" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="C11" s="85" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="D11" s="85" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="E11" s="85" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="F11" s="85" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="G11" s="85" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="H11" s="27" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="M11" s="19" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="N11" s="19" t="s">
         <v>52</v>
@@ -37578,15 +38029,15 @@
         <v>1</v>
       </c>
       <c r="P11" s="19" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="15.75" customHeight="1">
       <c r="H12" s="27" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="M12" s="19" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="N12" s="19" t="s">
         <v>52</v>
@@ -37595,16 +38046,16 @@
         <v>1</v>
       </c>
       <c r="P12" s="19" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="16.5" customHeight="1">
       <c r="C13" s="85"/>
       <c r="H13" s="27" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="M13" s="19" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="N13" s="19" t="s">
         <v>52</v>
@@ -37613,7 +38064,7 @@
         <v>1</v>
       </c>
       <c r="P13" s="19" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="16.5" customHeight="1">
@@ -37623,7 +38074,7 @@
         <v>#REF!</v>
       </c>
       <c r="M14" s="19" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="N14" s="19" t="s">
         <v>52</v>
@@ -37632,7 +38083,7 @@
         <v>1</v>
       </c>
       <c r="P14" s="19" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="S14" s="28"/>
     </row>
@@ -37643,7 +38094,7 @@
         <v>#REF!</v>
       </c>
       <c r="M15" s="19" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="N15" s="19" t="s">
         <v>52</v>
@@ -37652,16 +38103,16 @@
         <v>1</v>
       </c>
       <c r="P15" s="19" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="16.5" customHeight="1">
       <c r="C16" s="85"/>
       <c r="H16" s="27" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="M16" s="19" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="N16" s="19" t="s">
         <v>52</v>
@@ -37670,13 +38121,13 @@
         <v>1</v>
       </c>
       <c r="P16" s="19" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="17" spans="3:16" ht="16.5" customHeight="1">
       <c r="C17" s="85"/>
       <c r="M17" s="19" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="N17" s="19" t="s">
         <v>52</v>
@@ -37685,7 +38136,7 @@
         <v>1</v>
       </c>
       <c r="P17" s="19" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="18" spans="3:16" ht="16.5" customHeight="1">
@@ -37725,7 +38176,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr codeName="LaTeXLcombApp">
     <tabColor theme="1" tint="0.499984740745262"/>
@@ -37743,85 +38194,85 @@
     <col min="3" max="3" width="22.7109375" style="27" customWidth="1"/>
     <col min="4" max="24" width="11.5703125" style="27" customWidth="1"/>
     <col min="25" max="25" width="204.42578125" style="27" bestFit="1" customWidth="1"/>
-    <col min="26" max="37" width="11.5703125" style="27" customWidth="1"/>
-    <col min="38" max="16384" width="11.5703125" style="27"/>
+    <col min="26" max="38" width="11.5703125" style="27" customWidth="1"/>
+    <col min="39" max="16384" width="11.5703125" style="27"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25">
       <c r="A1" s="30" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="C1" s="31" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D1" s="32" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="E1" s="31" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="F1" s="31" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="G1" s="31" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="H1" s="31" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="I1" s="31" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="J1" s="31" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="K1" s="31" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="L1" s="31" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="M1" s="31" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="N1" s="31" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="O1" s="31" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="P1" s="31" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="Q1" s="31" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="R1" s="31" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="S1" s="31" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="T1" s="31" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="U1" s="31" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="V1" s="31" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="W1" s="31" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="X1" s="60" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="Y1" s="31" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
     </row>
     <row r="2" spans="1:25">
@@ -37829,10 +38280,10 @@
         <v>1000</v>
       </c>
       <c r="B2" s="125" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="C2" s="126" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="D2" s="124">
         <v>1</v>
@@ -37872,10 +38323,10 @@
         <v>1001</v>
       </c>
       <c r="B3" s="129" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="C3" s="126" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="D3" s="126">
         <v>2</v>
@@ -37915,10 +38366,10 @@
         <v>2000</v>
       </c>
       <c r="B4" s="129" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="C4" s="126" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="D4" s="126">
         <v>2</v>
@@ -37966,10 +38417,10 @@
         <v>2001</v>
       </c>
       <c r="B5" s="129" t="s">
+        <v>238</v>
+      </c>
+      <c r="C5" s="126" t="s">
         <v>235</v>
-      </c>
-      <c r="C5" s="126" t="s">
-        <v>232</v>
       </c>
       <c r="D5" s="126">
         <v>2</v>
@@ -38017,10 +38468,10 @@
         <v>2002</v>
       </c>
       <c r="B6" s="129" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="C6" s="126" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="D6" s="126">
         <v>2</v>
@@ -38068,10 +38519,10 @@
         <v>2100</v>
       </c>
       <c r="B7" s="129" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="C7" s="126" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="D7" s="126">
         <v>1</v>
@@ -38119,10 +38570,10 @@
         <v>2101</v>
       </c>
       <c r="B8" s="129" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="C8" s="126" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="D8" s="126">
         <v>1</v>
@@ -38170,10 +38621,10 @@
         <v>2102</v>
       </c>
       <c r="B9" s="129" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="C9" s="126" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="D9" s="126">
         <v>1</v>
@@ -38221,10 +38672,10 @@
         <v>2103</v>
       </c>
       <c r="B10" s="129" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="C10" s="126" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="D10" s="126">
         <v>1</v>
@@ -38272,10 +38723,10 @@
         <v>2104</v>
       </c>
       <c r="B11" s="129" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="C11" s="126" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="D11" s="126">
         <v>1</v>
@@ -38323,10 +38774,10 @@
         <v>2105</v>
       </c>
       <c r="B12" s="129" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="C12" s="126" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="D12" s="126">
         <v>1</v>
@@ -38374,10 +38825,10 @@
         <v>2106</v>
       </c>
       <c r="B13" s="129" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="C13" s="126" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="D13" s="126">
         <v>1</v>
@@ -38425,10 +38876,10 @@
         <v>2107</v>
       </c>
       <c r="B14" s="129" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="C14" s="126" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="D14" s="126">
         <v>1</v>
@@ -38476,10 +38927,10 @@
         <v>2108</v>
       </c>
       <c r="B15" s="129" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="C15" s="126" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="D15" s="126">
         <v>1</v>
@@ -38527,10 +38978,10 @@
         <v>2109</v>
       </c>
       <c r="B16" s="129" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="C16" s="126" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="D16" s="126">
         <v>1</v>
@@ -38578,10 +39029,10 @@
         <v>3001</v>
       </c>
       <c r="B17" s="129" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="C17" s="126" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="D17" s="126">
         <v>1</v>
@@ -38625,10 +39076,10 @@
         <v>3002</v>
       </c>
       <c r="B18" s="129" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="C18" s="126" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="D18" s="126">
         <v>2</v>
@@ -38672,10 +39123,10 @@
         <v>3004</v>
       </c>
       <c r="B19" s="129" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="C19" s="126" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="D19" s="126">
         <v>2</v>
@@ -38723,10 +39174,10 @@
         <v>3005</v>
       </c>
       <c r="B20" s="129" t="s">
+        <v>254</v>
+      </c>
+      <c r="C20" s="126" t="s">
         <v>251</v>
-      </c>
-      <c r="C20" s="126" t="s">
-        <v>248</v>
       </c>
       <c r="D20" s="126">
         <v>2</v>
@@ -38774,10 +39225,10 @@
         <v>3006</v>
       </c>
       <c r="B21" s="129" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="C21" s="126" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="D21" s="126">
         <v>2</v>

</xml_diff>

<commit_message>
Import of self-weight improved
</commit_message>
<xml_diff>
--- a/pyMaster_loads_tool.xlsx
+++ b/pyMaster_loads_tool.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://atlec-my.sharepoint.com/personal/mwo_woodthilsted_com/Documents/Professional/5_PYTHON/pyMasterLoadsTool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="11_8A5DF8D2319AF32EF13E9B2AED69841309E87D61" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55F88F0D-420B-4104-BA83-70867C8E4EB6}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="11_8A5DF8D2319AF32EF13E9B2AED69841309E87D61" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0ED5F1F-AC44-4162-90F5-7FE24293BCD5}"/>
   <bookViews>
-    <workbookView xWindow="6570" yWindow="1815" windowWidth="28800" windowHeight="15030" tabRatio="858" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16440" yWindow="4470" windowWidth="18945" windowHeight="14850" tabRatio="858" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Load case definition" sheetId="1" r:id="rId1"/>
@@ -172,10 +172,6 @@
 PX                 PY               PZ
 AX                 AY               AZ 
 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">         CX              CY             CZ
-objects/masses          </t>
   </si>
   <si>
     <t>AL                 BE                GA</t>
@@ -601,6 +597,10 @@
   </si>
   <si>
     <t>SLS_QPR_DL_LL_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         CX              CY             CZ
+          </t>
   </si>
 </sst>
 </file>
@@ -1252,41 +1252,41 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1836,7 +1836,7 @@
   </sheetPr>
   <dimension ref="A1:M177"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -3827,10 +3827,10 @@
   </sheetPr>
   <dimension ref="A1:AK177"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="AE13" sqref="AE13"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2:I7"/>
+      <selection pane="bottomLeft" activeCell="M3" sqref="M3:O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
@@ -3890,12 +3890,12 @@
       <c r="Y1" s="17"/>
       <c r="Z1" s="17"/>
       <c r="AA1" s="17"/>
-      <c r="AC1" s="128" t="s">
+      <c r="AC1" s="142" t="s">
         <v>30</v>
       </c>
-      <c r="AD1" s="129"/>
-      <c r="AE1" s="129"/>
-      <c r="AF1" s="130"/>
+      <c r="AD1" s="138"/>
+      <c r="AE1" s="138"/>
+      <c r="AF1" s="139"/>
     </row>
     <row r="2" spans="1:32" ht="12.4" customHeight="1">
       <c r="A2" s="123" t="s">
@@ -3907,37 +3907,37 @@
       <c r="C2" s="126" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="141"/>
-      <c r="E2" s="131"/>
-      <c r="F2" s="142"/>
+      <c r="D2" s="145"/>
+      <c r="E2" s="143"/>
+      <c r="F2" s="128"/>
       <c r="G2" s="126" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="143" t="s">
+      <c r="H2" s="130" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="145" t="s">
+      <c r="I2" s="141" t="s">
         <v>32</v>
       </c>
-      <c r="J2" s="140" t="s">
+      <c r="J2" s="137" t="s">
         <v>33</v>
       </c>
-      <c r="K2" s="129"/>
-      <c r="L2" s="129"/>
-      <c r="M2" s="129"/>
-      <c r="N2" s="129"/>
-      <c r="O2" s="129"/>
-      <c r="P2" s="129"/>
-      <c r="Q2" s="129"/>
-      <c r="R2" s="129"/>
-      <c r="S2" s="129"/>
-      <c r="T2" s="129"/>
-      <c r="U2" s="129"/>
-      <c r="V2" s="129"/>
-      <c r="W2" s="129"/>
-      <c r="X2" s="129"/>
-      <c r="Y2" s="129"/>
-      <c r="Z2" s="130"/>
+      <c r="K2" s="138"/>
+      <c r="L2" s="138"/>
+      <c r="M2" s="138"/>
+      <c r="N2" s="138"/>
+      <c r="O2" s="138"/>
+      <c r="P2" s="138"/>
+      <c r="Q2" s="138"/>
+      <c r="R2" s="138"/>
+      <c r="S2" s="138"/>
+      <c r="T2" s="138"/>
+      <c r="U2" s="138"/>
+      <c r="V2" s="138"/>
+      <c r="W2" s="138"/>
+      <c r="X2" s="138"/>
+      <c r="Y2" s="138"/>
+      <c r="Z2" s="139"/>
       <c r="AA2" s="120" t="s">
         <v>34</v>
       </c>
@@ -3958,44 +3958,44 @@
       <c r="A3" s="121"/>
       <c r="B3" s="121"/>
       <c r="C3" s="121"/>
-      <c r="D3" s="134"/>
-      <c r="E3" s="132"/>
-      <c r="F3" s="135"/>
+      <c r="D3" s="131"/>
+      <c r="E3" s="135"/>
+      <c r="F3" s="129"/>
       <c r="G3" s="121"/>
-      <c r="H3" s="134"/>
+      <c r="H3" s="131"/>
       <c r="I3" s="121"/>
-      <c r="J3" s="144" t="s">
+      <c r="J3" s="140" t="s">
         <v>39</v>
       </c>
-      <c r="K3" s="139"/>
-      <c r="L3" s="133"/>
-      <c r="M3" s="138" t="s">
+      <c r="K3" s="133"/>
+      <c r="L3" s="134"/>
+      <c r="M3" s="144" t="s">
+        <v>180</v>
+      </c>
+      <c r="N3" s="133"/>
+      <c r="O3" s="134"/>
+      <c r="P3" s="126" t="s">
         <v>40</v>
       </c>
-      <c r="N3" s="139"/>
-      <c r="O3" s="133"/>
-      <c r="P3" s="126" t="s">
+      <c r="Q3" s="133"/>
+      <c r="R3" s="134"/>
+      <c r="S3" s="120" t="s">
         <v>41</v>
       </c>
-      <c r="Q3" s="139"/>
-      <c r="R3" s="133"/>
-      <c r="S3" s="120" t="s">
+      <c r="T3" s="133"/>
+      <c r="U3" s="134"/>
+      <c r="V3" s="120" t="s">
         <v>42</v>
       </c>
-      <c r="T3" s="139"/>
-      <c r="U3" s="133"/>
-      <c r="V3" s="120" t="s">
+      <c r="W3" s="120" t="s">
         <v>43</v>
       </c>
-      <c r="W3" s="120" t="s">
+      <c r="X3" s="134"/>
+      <c r="Y3" s="120" t="s">
         <v>44</v>
       </c>
-      <c r="X3" s="133"/>
-      <c r="Y3" s="120" t="s">
+      <c r="Z3" s="120" t="s">
         <v>45</v>
-      </c>
-      <c r="Z3" s="120" t="s">
-        <v>46</v>
       </c>
       <c r="AA3" s="121"/>
       <c r="AC3" s="121"/>
@@ -4007,27 +4007,27 @@
       <c r="A4" s="121"/>
       <c r="B4" s="121"/>
       <c r="C4" s="121"/>
-      <c r="D4" s="134"/>
-      <c r="E4" s="132"/>
-      <c r="F4" s="135"/>
+      <c r="D4" s="131"/>
+      <c r="E4" s="135"/>
+      <c r="F4" s="129"/>
       <c r="G4" s="121"/>
-      <c r="H4" s="134"/>
+      <c r="H4" s="131"/>
       <c r="I4" s="121"/>
-      <c r="J4" s="134"/>
-      <c r="K4" s="132"/>
-      <c r="L4" s="135"/>
-      <c r="M4" s="134"/>
-      <c r="N4" s="132"/>
-      <c r="O4" s="135"/>
-      <c r="P4" s="134"/>
-      <c r="Q4" s="132"/>
-      <c r="R4" s="135"/>
-      <c r="S4" s="134"/>
-      <c r="T4" s="132"/>
-      <c r="U4" s="135"/>
+      <c r="J4" s="131"/>
+      <c r="K4" s="135"/>
+      <c r="L4" s="129"/>
+      <c r="M4" s="131"/>
+      <c r="N4" s="135"/>
+      <c r="O4" s="129"/>
+      <c r="P4" s="131"/>
+      <c r="Q4" s="135"/>
+      <c r="R4" s="129"/>
+      <c r="S4" s="131"/>
+      <c r="T4" s="135"/>
+      <c r="U4" s="129"/>
       <c r="V4" s="121"/>
-      <c r="W4" s="134"/>
-      <c r="X4" s="135"/>
+      <c r="W4" s="131"/>
+      <c r="X4" s="129"/>
       <c r="Y4" s="121"/>
       <c r="Z4" s="121"/>
       <c r="AA4" s="121"/>
@@ -4040,27 +4040,27 @@
       <c r="A5" s="121"/>
       <c r="B5" s="121"/>
       <c r="C5" s="121"/>
-      <c r="D5" s="134"/>
-      <c r="E5" s="132"/>
-      <c r="F5" s="135"/>
+      <c r="D5" s="131"/>
+      <c r="E5" s="135"/>
+      <c r="F5" s="129"/>
       <c r="G5" s="121"/>
-      <c r="H5" s="134"/>
+      <c r="H5" s="131"/>
       <c r="I5" s="121"/>
-      <c r="J5" s="134"/>
-      <c r="K5" s="132"/>
-      <c r="L5" s="135"/>
-      <c r="M5" s="134"/>
-      <c r="N5" s="132"/>
-      <c r="O5" s="135"/>
-      <c r="P5" s="134"/>
-      <c r="Q5" s="132"/>
-      <c r="R5" s="135"/>
-      <c r="S5" s="134"/>
-      <c r="T5" s="132"/>
-      <c r="U5" s="135"/>
+      <c r="J5" s="131"/>
+      <c r="K5" s="135"/>
+      <c r="L5" s="129"/>
+      <c r="M5" s="131"/>
+      <c r="N5" s="135"/>
+      <c r="O5" s="129"/>
+      <c r="P5" s="131"/>
+      <c r="Q5" s="135"/>
+      <c r="R5" s="129"/>
+      <c r="S5" s="131"/>
+      <c r="T5" s="135"/>
+      <c r="U5" s="129"/>
       <c r="V5" s="121"/>
-      <c r="W5" s="134"/>
-      <c r="X5" s="135"/>
+      <c r="W5" s="131"/>
+      <c r="X5" s="129"/>
       <c r="Y5" s="121"/>
       <c r="Z5" s="121"/>
       <c r="AA5" s="121"/>
@@ -4073,27 +4073,27 @@
       <c r="A6" s="121"/>
       <c r="B6" s="121"/>
       <c r="C6" s="121"/>
-      <c r="D6" s="134"/>
-      <c r="E6" s="132"/>
-      <c r="F6" s="135"/>
+      <c r="D6" s="131"/>
+      <c r="E6" s="135"/>
+      <c r="F6" s="129"/>
       <c r="G6" s="121"/>
-      <c r="H6" s="134"/>
+      <c r="H6" s="131"/>
       <c r="I6" s="121"/>
-      <c r="J6" s="136"/>
+      <c r="J6" s="132"/>
       <c r="K6" s="125"/>
-      <c r="L6" s="137"/>
-      <c r="M6" s="136"/>
+      <c r="L6" s="136"/>
+      <c r="M6" s="132"/>
       <c r="N6" s="125"/>
-      <c r="O6" s="137"/>
-      <c r="P6" s="134"/>
-      <c r="Q6" s="132"/>
-      <c r="R6" s="135"/>
-      <c r="S6" s="136"/>
+      <c r="O6" s="136"/>
+      <c r="P6" s="131"/>
+      <c r="Q6" s="135"/>
+      <c r="R6" s="129"/>
+      <c r="S6" s="132"/>
       <c r="T6" s="125"/>
-      <c r="U6" s="137"/>
+      <c r="U6" s="136"/>
       <c r="V6" s="121"/>
-      <c r="W6" s="134"/>
-      <c r="X6" s="135"/>
+      <c r="W6" s="131"/>
+      <c r="X6" s="129"/>
       <c r="Y6" s="121"/>
       <c r="Z6" s="121"/>
       <c r="AA6" s="121"/>
@@ -4106,33 +4106,33 @@
       <c r="A7" s="122"/>
       <c r="B7" s="122"/>
       <c r="C7" s="122"/>
-      <c r="D7" s="134"/>
-      <c r="E7" s="132"/>
-      <c r="F7" s="135"/>
+      <c r="D7" s="131"/>
+      <c r="E7" s="135"/>
+      <c r="F7" s="129"/>
       <c r="G7" s="122"/>
-      <c r="H7" s="136"/>
+      <c r="H7" s="132"/>
       <c r="I7" s="122"/>
-      <c r="J7" s="140" t="s">
+      <c r="J7" s="137" t="s">
+        <v>46</v>
+      </c>
+      <c r="K7" s="138"/>
+      <c r="L7" s="139"/>
+      <c r="M7" s="137" t="s">
         <v>47</v>
       </c>
-      <c r="K7" s="129"/>
-      <c r="L7" s="130"/>
-      <c r="M7" s="140" t="s">
+      <c r="N7" s="138"/>
+      <c r="O7" s="139"/>
+      <c r="P7" s="132"/>
+      <c r="Q7" s="125"/>
+      <c r="R7" s="136"/>
+      <c r="S7" s="137" t="s">
         <v>48</v>
       </c>
-      <c r="N7" s="129"/>
-      <c r="O7" s="130"/>
-      <c r="P7" s="136"/>
-      <c r="Q7" s="125"/>
-      <c r="R7" s="137"/>
-      <c r="S7" s="140" t="s">
-        <v>49</v>
-      </c>
-      <c r="T7" s="129"/>
-      <c r="U7" s="130"/>
+      <c r="T7" s="138"/>
+      <c r="U7" s="139"/>
       <c r="V7" s="122"/>
-      <c r="W7" s="136"/>
-      <c r="X7" s="137"/>
+      <c r="W7" s="132"/>
+      <c r="X7" s="136"/>
       <c r="Y7" s="122"/>
       <c r="Z7" s="122"/>
       <c r="AA7" s="122"/>
@@ -4154,7 +4154,7 @@
       </c>
       <c r="D8" s="17"/>
       <c r="E8" s="59" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F8" s="17"/>
       <c r="G8" s="20" t="str">
@@ -4162,7 +4162,7 @@
         <v>1:STA1</v>
       </c>
       <c r="H8" s="42" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I8" s="99">
         <v>1</v>
@@ -4189,7 +4189,7 @@
       <c r="AD8" s="63"/>
       <c r="AE8" s="63"/>
       <c r="AF8" s="63" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:32">
@@ -4205,7 +4205,7 @@
       </c>
       <c r="D9" s="17"/>
       <c r="E9" s="59" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F9" s="17"/>
       <c r="G9" s="21" t="str">
@@ -4213,10 +4213,10 @@
         <v>1:STA1</v>
       </c>
       <c r="H9" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="I9" s="99" t="s">
         <v>53</v>
-      </c>
-      <c r="I9" s="99" t="s">
-        <v>54</v>
       </c>
       <c r="J9" s="80">
         <v>0</v>
@@ -4256,7 +4256,7 @@
       </c>
       <c r="V9" s="83"/>
       <c r="W9" s="84" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="X9" s="75"/>
       <c r="Y9" s="17">
@@ -4268,7 +4268,7 @@
       <c r="AD9" s="64"/>
       <c r="AE9" s="64"/>
       <c r="AF9" s="64" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:32">
@@ -4290,10 +4290,10 @@
         <v>1:STA1</v>
       </c>
       <c r="H10" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="I10" s="99" t="s">
         <v>53</v>
-      </c>
-      <c r="I10" s="99" t="s">
-        <v>54</v>
       </c>
       <c r="J10" s="80">
         <v>0</v>
@@ -4333,7 +4333,7 @@
       </c>
       <c r="V10" s="83"/>
       <c r="W10" s="84" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="X10" s="75"/>
       <c r="Y10" s="17">
@@ -4345,7 +4345,7 @@
       <c r="AD10" s="64"/>
       <c r="AE10" s="64"/>
       <c r="AF10" s="64" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:32">
@@ -4361,7 +4361,7 @@
       </c>
       <c r="D11" s="17"/>
       <c r="E11" s="59" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F11" s="17"/>
       <c r="G11" s="21" t="str">
@@ -4369,10 +4369,10 @@
         <v>1:STA1</v>
       </c>
       <c r="H11" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="I11" s="99" t="s">
         <v>53</v>
-      </c>
-      <c r="I11" s="99" t="s">
-        <v>54</v>
       </c>
       <c r="J11" s="80">
         <v>0</v>
@@ -4412,7 +4412,7 @@
       </c>
       <c r="V11" s="83"/>
       <c r="W11" s="84" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="X11" s="75"/>
       <c r="Y11" s="17">
@@ -4424,7 +4424,7 @@
       <c r="AD11" s="64"/>
       <c r="AE11" s="64"/>
       <c r="AF11" s="64" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:32">
@@ -4440,7 +4440,7 @@
       </c>
       <c r="D12" s="17"/>
       <c r="E12" s="59" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F12" s="17"/>
       <c r="G12" s="21" t="str">
@@ -4448,10 +4448,10 @@
         <v>1:STA1</v>
       </c>
       <c r="H12" s="42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I12" s="100" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J12" s="80">
         <v>0</v>
@@ -4491,7 +4491,7 @@
       </c>
       <c r="V12" s="64"/>
       <c r="W12" s="84" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="X12" s="75"/>
       <c r="Y12" s="17">
@@ -4513,7 +4513,7 @@
       </c>
       <c r="D13" s="17"/>
       <c r="E13" s="59" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F13" s="17"/>
       <c r="G13" s="21" t="str">
@@ -4554,7 +4554,7 @@
       </c>
       <c r="D14" s="17"/>
       <c r="E14" s="59" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F14" s="17"/>
       <c r="G14" s="21" t="str">
@@ -4673,7 +4673,7 @@
       </c>
       <c r="D17" s="17"/>
       <c r="E17" s="59" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F17" s="17"/>
       <c r="G17" s="21" t="str">
@@ -4792,7 +4792,7 @@
       </c>
       <c r="D20" s="17"/>
       <c r="E20" s="59" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F20" s="17"/>
       <c r="G20" s="21" t="str">
@@ -4911,7 +4911,7 @@
       </c>
       <c r="D23" s="17"/>
       <c r="E23" s="59" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F23" s="17"/>
       <c r="G23" s="21" t="str">
@@ -5030,7 +5030,7 @@
       </c>
       <c r="D26" s="17"/>
       <c r="E26" s="59" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F26" s="17"/>
       <c r="G26" s="21" t="str">
@@ -5149,7 +5149,7 @@
       </c>
       <c r="D29" s="17"/>
       <c r="E29" s="59" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F29" s="17"/>
       <c r="G29" s="21" t="str">
@@ -5268,7 +5268,7 @@
       </c>
       <c r="D32" s="17"/>
       <c r="E32" s="59" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F32" s="17"/>
       <c r="G32" s="21" t="str">
@@ -5387,7 +5387,7 @@
       </c>
       <c r="D35" s="17"/>
       <c r="E35" s="59" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F35" s="17"/>
       <c r="G35" s="21" t="str">
@@ -10959,17 +10959,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="F2:F7"/>
-    <mergeCell ref="H2:H7"/>
-    <mergeCell ref="Y3:Y7"/>
-    <mergeCell ref="S3:U6"/>
-    <mergeCell ref="P3:R7"/>
-    <mergeCell ref="S7:U7"/>
-    <mergeCell ref="M7:O7"/>
-    <mergeCell ref="J3:L6"/>
-    <mergeCell ref="G2:G7"/>
-    <mergeCell ref="I2:I7"/>
-    <mergeCell ref="J7:L7"/>
     <mergeCell ref="AC1:AF1"/>
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="C2:C7"/>
@@ -10986,6 +10975,17 @@
     <mergeCell ref="B2:B7"/>
     <mergeCell ref="AE2:AE7"/>
     <mergeCell ref="D2:D7"/>
+    <mergeCell ref="F2:F7"/>
+    <mergeCell ref="H2:H7"/>
+    <mergeCell ref="Y3:Y7"/>
+    <mergeCell ref="S3:U6"/>
+    <mergeCell ref="P3:R7"/>
+    <mergeCell ref="S7:U7"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="J3:L6"/>
+    <mergeCell ref="G2:G7"/>
+    <mergeCell ref="I2:I7"/>
+    <mergeCell ref="J7:L7"/>
   </mergeCells>
   <conditionalFormatting sqref="I1:I1048576">
     <cfRule type="expression" dxfId="28" priority="41">
@@ -11103,7 +11103,7 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the name of the load case_x000a__x000a_Please keep naming of similar loads as consistent as possible" sqref="B2:B7" xr:uid="{00000000-0002-0000-0100-00000C000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the load case number_x000a__x000a_Try to stick to a consistent naming convention and leave 100 possibilities for each load type. For example: _x000a_200-299 are live loads,_x000a_300-399 could be padeye loads,_x000a_400-499 could be HOP loads etc._x000a_ " sqref="A2:A7" xr:uid="{00000000-0002-0000-0100-00000D000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="FX / PX / AX - Enter the force / pressure / acceleration in the X direction_x000a__x000a_FY / PY / AY - Enter the force / pressure / acceleration in the Y direction_x000a__x000a_FZ / PZ / AZ - Enter the force / pressure / acceleration in the Z direction_x000a__x000a_(kN / kPa / m/s2)_x000a_" sqref="J3:L6" xr:uid="{00000000-0002-0000-0100-00000E000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="CX - Enter the moment about the X axis (kN*m)_x000a_objects/masses - Enter either 'objects' or 'masses'. This applies only to a body force._x000a__x000a_CY - Enter the moment about the Y axis (kN*m)_x000a__x000a_CZ - Enter the moment about the Z axis (kN*m)" sqref="M3:O6" xr:uid="{00000000-0002-0000-0100-00000F000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="CX - Enter the moment about the X axis (kN*m)_x000a__x000a_CY - Enter the moment about the Y axis (kN*m)_x000a__x000a_CZ - Enter the moment about the Z axis (kN*m)" sqref="M3:O6" xr:uid="{00000000-0002-0000-0100-00000F000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the node(s), member(s) or object(s) number which each load case is applied to" sqref="I2:I7" xr:uid="{00000000-0002-0000-0100-000010000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the load type from the drop down menu_x000a__x000a_Currently, the options are:_x000a_(FE) uniform, nodal force, Body forces, member force,  self-weight, trapezoidal (2p), uniform load " sqref="H2:H7" xr:uid="{00000000-0002-0000-0100-000011000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please enter the total value of the load that you are applying and a reference for the value._x000a__x000a_This column is just for checking purposes and is not used by any macros." sqref="AA2:AA7" xr:uid="{00000000-0002-0000-0100-000012000000}"/>
@@ -11530,17 +11530,17 @@
     </row>
     <row r="3" spans="1:4605" s="7" customFormat="1" ht="218.65" customHeight="1">
       <c r="A3" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>59</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="56" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="72" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F3" s="72" t="s">
         <v>7</v>
@@ -16156,9 +16156,9 @@
       <c r="D4" s="146" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="139"/>
-      <c r="F4" s="139"/>
-      <c r="G4" s="139"/>
+      <c r="E4" s="133"/>
+      <c r="F4" s="133"/>
+      <c r="G4" s="133"/>
       <c r="H4" s="87">
         <v>1</v>
       </c>
@@ -20764,7 +20764,7 @@
       <c r="A5" s="33"/>
       <c r="B5" s="23"/>
       <c r="C5" s="23"/>
-      <c r="D5" s="136"/>
+      <c r="D5" s="132"/>
       <c r="E5" s="125"/>
       <c r="F5" s="125"/>
       <c r="G5" s="125"/>
@@ -21139,25 +21139,25 @@
     </row>
     <row r="6" spans="1:4605" s="16" customFormat="1" ht="14.45" customHeight="1">
       <c r="A6" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="C6" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="D6" s="53" t="s">
         <v>63</v>
       </c>
-      <c r="D6" s="53" t="s">
-        <v>64</v>
-      </c>
       <c r="E6" s="53" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F6" s="53" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G6" s="53" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:4605" s="16" customFormat="1">
@@ -31667,81 +31667,81 @@
   <sheetData>
     <row r="1" spans="1:23">
       <c r="A1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" t="s">
         <v>65</v>
       </c>
-      <c r="B1" t="s">
+      <c r="G1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" t="s">
         <v>66</v>
       </c>
-      <c r="G1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="M1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N1" t="s">
         <v>67</v>
       </c>
-      <c r="M1" t="s">
-        <v>65</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="S1" t="s">
+        <v>64</v>
+      </c>
+      <c r="T1" t="s">
         <v>68</v>
-      </c>
-      <c r="S1" t="s">
-        <v>65</v>
-      </c>
-      <c r="T1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:23">
       <c r="A2" s="103" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="103" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="103" t="s">
+      <c r="C2" s="103" t="s">
         <v>71</v>
       </c>
-      <c r="C2" s="103" t="s">
+      <c r="D2" t="s">
         <v>72</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" t="s">
+        <v>70</v>
+      </c>
+      <c r="I2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J2" t="s">
+        <v>72</v>
+      </c>
+      <c r="M2" t="s">
+        <v>69</v>
+      </c>
+      <c r="N2" t="s">
+        <v>70</v>
+      </c>
+      <c r="O2" t="s">
+        <v>71</v>
+      </c>
+      <c r="P2" t="s">
+        <v>72</v>
+      </c>
+      <c r="S2" t="s">
+        <v>69</v>
+      </c>
+      <c r="T2" t="s">
+        <v>70</v>
+      </c>
+      <c r="U2" t="s">
+        <v>71</v>
+      </c>
+      <c r="V2" t="s">
+        <v>72</v>
+      </c>
+      <c r="W2" t="s">
         <v>73</v>
-      </c>
-      <c r="G2" t="s">
-        <v>70</v>
-      </c>
-      <c r="H2" t="s">
-        <v>71</v>
-      </c>
-      <c r="I2" t="s">
-        <v>72</v>
-      </c>
-      <c r="J2" t="s">
-        <v>73</v>
-      </c>
-      <c r="M2" t="s">
-        <v>70</v>
-      </c>
-      <c r="N2" t="s">
-        <v>71</v>
-      </c>
-      <c r="O2" t="s">
-        <v>72</v>
-      </c>
-      <c r="P2" t="s">
-        <v>73</v>
-      </c>
-      <c r="S2" t="s">
-        <v>70</v>
-      </c>
-      <c r="T2" t="s">
-        <v>71</v>
-      </c>
-      <c r="U2" t="s">
-        <v>72</v>
-      </c>
-      <c r="V2" t="s">
-        <v>73</v>
-      </c>
-      <c r="W2" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:23">
@@ -31794,7 +31794,7 @@
         <v>0</v>
       </c>
       <c r="W3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:23">
@@ -31847,7 +31847,7 @@
         <v>0</v>
       </c>
       <c r="W4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:23">
@@ -31900,7 +31900,7 @@
         <v>0</v>
       </c>
       <c r="W5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:23">
@@ -32098,81 +32098,81 @@
   <sheetData>
     <row r="1" spans="1:23">
       <c r="A1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" t="s">
         <v>65</v>
       </c>
-      <c r="B1" t="s">
+      <c r="G1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" t="s">
         <v>66</v>
       </c>
-      <c r="G1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="M1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N1" t="s">
         <v>67</v>
       </c>
-      <c r="M1" t="s">
-        <v>65</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="S1" t="s">
+        <v>64</v>
+      </c>
+      <c r="T1" t="s">
         <v>68</v>
-      </c>
-      <c r="S1" t="s">
-        <v>65</v>
-      </c>
-      <c r="T1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:23">
       <c r="A2" s="103" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="103" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="103" t="s">
+      <c r="C2" s="103" t="s">
         <v>71</v>
       </c>
-      <c r="C2" s="103" t="s">
+      <c r="D2" t="s">
         <v>72</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" t="s">
+        <v>70</v>
+      </c>
+      <c r="I2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J2" t="s">
+        <v>72</v>
+      </c>
+      <c r="M2" t="s">
+        <v>69</v>
+      </c>
+      <c r="N2" t="s">
+        <v>70</v>
+      </c>
+      <c r="O2" t="s">
+        <v>71</v>
+      </c>
+      <c r="P2" t="s">
+        <v>72</v>
+      </c>
+      <c r="S2" t="s">
+        <v>69</v>
+      </c>
+      <c r="T2" t="s">
+        <v>70</v>
+      </c>
+      <c r="U2" t="s">
+        <v>71</v>
+      </c>
+      <c r="V2" t="s">
+        <v>72</v>
+      </c>
+      <c r="W2" t="s">
         <v>73</v>
-      </c>
-      <c r="G2" t="s">
-        <v>70</v>
-      </c>
-      <c r="H2" t="s">
-        <v>71</v>
-      </c>
-      <c r="I2" t="s">
-        <v>72</v>
-      </c>
-      <c r="J2" t="s">
-        <v>73</v>
-      </c>
-      <c r="M2" t="s">
-        <v>70</v>
-      </c>
-      <c r="N2" t="s">
-        <v>71</v>
-      </c>
-      <c r="O2" t="s">
-        <v>72</v>
-      </c>
-      <c r="P2" t="s">
-        <v>73</v>
-      </c>
-      <c r="S2" t="s">
-        <v>70</v>
-      </c>
-      <c r="T2" t="s">
-        <v>71</v>
-      </c>
-      <c r="U2" t="s">
-        <v>72</v>
-      </c>
-      <c r="V2" t="s">
-        <v>73</v>
-      </c>
-      <c r="W2" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:23">
@@ -32225,7 +32225,7 @@
         <v>0</v>
       </c>
       <c r="W3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:23">
@@ -32278,7 +32278,7 @@
         <v>0</v>
       </c>
       <c r="W4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:23">
@@ -32331,7 +32331,7 @@
         <v>0</v>
       </c>
       <c r="W5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:23">
@@ -32550,7 +32550,7 @@
   <sheetData>
     <row r="1" spans="1:20" ht="13.5" customHeight="1" thickBot="1">
       <c r="A1" s="19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F1" s="26">
         <v>0.5</v>
@@ -32559,77 +32559,77 @@
         <v>0.1</v>
       </c>
       <c r="M1" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="S1" s="19" t="s">
         <v>79</v>
-      </c>
-      <c r="S1" s="19" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="15.75" customHeight="1">
       <c r="A2" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="C2" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="D2" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="E2" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="F2" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="G2" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="H2" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="H2" s="27" t="s">
+      <c r="J2" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="J2" s="19" t="s">
+      <c r="K2" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="K2" s="19" t="s">
+      <c r="M2" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="M2" s="19" t="s">
-        <v>91</v>
-      </c>
       <c r="N2" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O2" s="19">
         <v>1</v>
       </c>
       <c r="P2" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="S2" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="S2" s="19" t="s">
+      <c r="T2" s="19" t="s">
         <v>93</v>
-      </c>
-      <c r="T2" s="19" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="39" customHeight="1">
       <c r="A3" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="C3" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="C3" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3" s="19" t="s">
+      <c r="E3" s="19" t="s">
         <v>97</v>
-      </c>
-      <c r="E3" s="19" t="s">
-        <v>98</v>
       </c>
       <c r="F3" s="27" t="e">
         <f>PlatformName &amp;" member utilisations $&gt;" &amp;F1&amp;"$"</f>
@@ -32644,107 +32644,107 @@
         <v>#REF!</v>
       </c>
       <c r="J3" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="K3" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="K3" s="27" t="s">
+      <c r="M3" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="M3" s="19" t="s">
-        <v>101</v>
-      </c>
       <c r="N3" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O3" s="19">
         <v>1</v>
       </c>
       <c r="P3" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="S3" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="T3" s="28" t="s">
         <v>102</v>
-      </c>
-      <c r="T3" s="28" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="15.75" customHeight="1">
       <c r="A4" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="C4" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="H4" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="C4" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="D4" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="F4" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="G4" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="H4" s="27" t="s">
+      <c r="M4" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="M4" s="19" t="s">
-        <v>107</v>
-      </c>
       <c r="N4" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O4" s="19">
         <v>1</v>
       </c>
       <c r="P4" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="S4" s="19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="15.75" customHeight="1">
       <c r="B5" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="H5" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="C5" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="E5" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="F5" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="G5" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="H5" s="27" t="s">
+      <c r="M5" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="M5" s="19" t="s">
-        <v>111</v>
-      </c>
       <c r="N5" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O5" s="19">
         <v>1</v>
       </c>
       <c r="P5" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="S5" s="19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="15.75" customHeight="1">
@@ -32773,19 +32773,19 @@
         <v>#REF!</v>
       </c>
       <c r="H6" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="M6" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="M6" s="19" t="s">
-        <v>114</v>
-      </c>
       <c r="N6" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O6" s="19">
         <v>1</v>
       </c>
       <c r="P6" s="19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="S6" s="19" t="e">
         <f>"\includegraphics[width=\textwidth]{\"&amp;LaTeXFiguresFolder &amp;"\"&amp;PlatformName&amp; " "&amp;S3&amp;".png} "</f>
@@ -32818,61 +32818,61 @@
         <v>#REF!</v>
       </c>
       <c r="H7" s="27" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J7" s="19">
         <f>COLUMN(J1)</f>
         <v>10</v>
       </c>
       <c r="M7" s="19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="N7" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O7" s="19">
         <v>1</v>
       </c>
       <c r="P7" s="19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="S7" s="19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="15.75" customHeight="1">
       <c r="B8" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="C8" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="D8" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="E8" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="F8" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="F8" s="19" t="s">
+      <c r="G8" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="G8" s="19" t="s">
+      <c r="H8" s="27" t="s">
         <v>124</v>
       </c>
-      <c r="H8" s="27" t="s">
+      <c r="M8" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="M8" s="19" t="s">
-        <v>126</v>
-      </c>
       <c r="N8" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O8" s="19">
         <v>1</v>
       </c>
       <c r="P8" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="S8" s="19" t="e">
         <f>"    \caption{" &amp;PlatformName&amp; " " &amp; S3 &amp;".}"</f>
@@ -32881,37 +32881,37 @@
     </row>
     <row r="9" spans="1:20" ht="15.75" customHeight="1">
       <c r="B9" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="C9" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="D9" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="E9" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="F9" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="F9" s="19" t="s">
+      <c r="G9" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="G9" s="19" t="s">
+      <c r="H9" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="M9" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="H9" s="27" t="s">
-        <v>110</v>
-      </c>
-      <c r="M9" s="19" t="s">
-        <v>133</v>
-      </c>
       <c r="N9" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O9" s="19">
         <v>1</v>
       </c>
       <c r="P9" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="S9" s="19" t="e">
         <f>"    \label{tabl:" &amp; PlatformName &amp;" "&amp;S3 &amp;"}"</f>
@@ -32920,107 +32920,107 @@
     </row>
     <row r="10" spans="1:20" ht="16.5" customHeight="1">
       <c r="B10" s="49" t="s">
+        <v>133</v>
+      </c>
+      <c r="C10" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="D10" s="19" t="s">
         <v>135</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="E10" s="19" t="s">
         <v>136</v>
       </c>
-      <c r="E10" s="19" t="s">
+      <c r="F10" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="F10" s="19" t="s">
+      <c r="G10" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="H10" s="27" t="s">
         <v>138</v>
       </c>
-      <c r="G10" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="H10" s="27" t="s">
+      <c r="M10" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="M10" s="19" t="s">
-        <v>140</v>
-      </c>
       <c r="N10" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O10" s="19">
         <v>1</v>
       </c>
       <c r="P10" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:20" ht="16.5" customHeight="1">
       <c r="B11" s="49" t="s">
+        <v>140</v>
+      </c>
+      <c r="C11" s="49" t="s">
+        <v>140</v>
+      </c>
+      <c r="D11" s="49" t="s">
+        <v>140</v>
+      </c>
+      <c r="E11" s="49" t="s">
+        <v>140</v>
+      </c>
+      <c r="F11" s="49" t="s">
+        <v>140</v>
+      </c>
+      <c r="G11" s="49" t="s">
+        <v>140</v>
+      </c>
+      <c r="H11" s="27" t="s">
         <v>141</v>
       </c>
-      <c r="C11" s="49" t="s">
-        <v>141</v>
-      </c>
-      <c r="D11" s="49" t="s">
-        <v>141</v>
-      </c>
-      <c r="E11" s="49" t="s">
-        <v>141</v>
-      </c>
-      <c r="F11" s="49" t="s">
-        <v>141</v>
-      </c>
-      <c r="G11" s="49" t="s">
-        <v>141</v>
-      </c>
-      <c r="H11" s="27" t="s">
+      <c r="M11" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="M11" s="19" t="s">
-        <v>143</v>
-      </c>
       <c r="N11" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O11" s="19">
         <v>1</v>
       </c>
       <c r="P11" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="15.75" customHeight="1">
       <c r="H12" s="27" t="s">
+        <v>143</v>
+      </c>
+      <c r="M12" s="19" t="s">
         <v>144</v>
       </c>
-      <c r="M12" s="19" t="s">
-        <v>145</v>
-      </c>
       <c r="N12" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O12" s="19">
         <v>1</v>
       </c>
       <c r="P12" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="16.5" customHeight="1">
       <c r="C13" s="49"/>
       <c r="H13" s="27" t="s">
+        <v>145</v>
+      </c>
+      <c r="M13" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="M13" s="19" t="s">
-        <v>147</v>
-      </c>
       <c r="N13" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O13" s="19">
         <v>1</v>
       </c>
       <c r="P13" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="16.5" customHeight="1">
@@ -33030,16 +33030,16 @@
         <v>#REF!</v>
       </c>
       <c r="M14" s="19" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="N14" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O14" s="19">
         <v>1</v>
       </c>
       <c r="P14" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="S14" s="28"/>
     </row>
@@ -33050,49 +33050,49 @@
         <v>#REF!</v>
       </c>
       <c r="M15" s="19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="N15" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O15" s="19">
         <v>1</v>
       </c>
       <c r="P15" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="16.5" customHeight="1">
       <c r="C16" s="49"/>
       <c r="H16" s="27" t="s">
+        <v>149</v>
+      </c>
+      <c r="M16" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="M16" s="19" t="s">
-        <v>151</v>
-      </c>
       <c r="N16" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O16" s="19">
         <v>1</v>
       </c>
       <c r="P16" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="3:16" ht="16.5" customHeight="1">
       <c r="C17" s="49"/>
       <c r="M17" s="19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="N17" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O17" s="19">
         <v>1</v>
       </c>
       <c r="P17" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="3:16" ht="16.5" customHeight="1">
@@ -33156,79 +33156,79 @@
   <sheetData>
     <row r="1" spans="1:25">
       <c r="A1" s="30" t="s">
+        <v>152</v>
+      </c>
+      <c r="B1" s="31" t="s">
         <v>153</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="C1" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="32" t="s">
         <v>154</v>
       </c>
-      <c r="C1" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="D1" s="32" t="s">
+      <c r="E1" s="31" t="s">
         <v>155</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="F1" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="G1" s="31" t="s">
+        <v>155</v>
+      </c>
+      <c r="H1" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="I1" s="31" t="s">
+        <v>155</v>
+      </c>
+      <c r="J1" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="K1" s="31" t="s">
+        <v>155</v>
+      </c>
+      <c r="L1" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="M1" s="31" t="s">
+        <v>155</v>
+      </c>
+      <c r="N1" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="O1" s="31" t="s">
+        <v>155</v>
+      </c>
+      <c r="P1" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q1" s="31" t="s">
+        <v>155</v>
+      </c>
+      <c r="R1" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="S1" s="31" t="s">
+        <v>155</v>
+      </c>
+      <c r="T1" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="U1" s="31" t="s">
+        <v>155</v>
+      </c>
+      <c r="V1" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="W1" s="31" t="s">
+        <v>155</v>
+      </c>
+      <c r="X1" s="35" t="s">
         <v>156</v>
       </c>
-      <c r="F1" s="31" t="s">
-        <v>155</v>
-      </c>
-      <c r="G1" s="31" t="s">
-        <v>156</v>
-      </c>
-      <c r="H1" s="31" t="s">
-        <v>155</v>
-      </c>
-      <c r="I1" s="31" t="s">
-        <v>156</v>
-      </c>
-      <c r="J1" s="31" t="s">
-        <v>155</v>
-      </c>
-      <c r="K1" s="31" t="s">
-        <v>156</v>
-      </c>
-      <c r="L1" s="31" t="s">
-        <v>155</v>
-      </c>
-      <c r="M1" s="31" t="s">
-        <v>156</v>
-      </c>
-      <c r="N1" s="31" t="s">
-        <v>155</v>
-      </c>
-      <c r="O1" s="31" t="s">
-        <v>156</v>
-      </c>
-      <c r="P1" s="31" t="s">
-        <v>155</v>
-      </c>
-      <c r="Q1" s="31" t="s">
-        <v>156</v>
-      </c>
-      <c r="R1" s="31" t="s">
-        <v>155</v>
-      </c>
-      <c r="S1" s="31" t="s">
-        <v>156</v>
-      </c>
-      <c r="T1" s="31" t="s">
-        <v>155</v>
-      </c>
-      <c r="U1" s="31" t="s">
-        <v>156</v>
-      </c>
-      <c r="V1" s="31" t="s">
-        <v>155</v>
-      </c>
-      <c r="W1" s="31" t="s">
-        <v>156</v>
-      </c>
-      <c r="X1" s="35" t="s">
+      <c r="Y1" s="31" t="s">
         <v>157</v>
-      </c>
-      <c r="Y1" s="31" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:25">
@@ -33236,10 +33236,10 @@
         <v>1000</v>
       </c>
       <c r="B2" s="89" t="s">
+        <v>158</v>
+      </c>
+      <c r="C2" s="90" t="s">
         <v>159</v>
-      </c>
-      <c r="C2" s="90" t="s">
-        <v>160</v>
       </c>
       <c r="D2" s="88">
         <v>1</v>
@@ -33279,10 +33279,10 @@
         <v>1001</v>
       </c>
       <c r="B3" s="93" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C3" s="90" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D3" s="90">
         <v>2</v>
@@ -33322,10 +33322,10 @@
         <v>2000</v>
       </c>
       <c r="B4" s="93" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C4" s="90" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D4" s="90">
         <v>2</v>
@@ -33373,10 +33373,10 @@
         <v>2001</v>
       </c>
       <c r="B5" s="93" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C5" s="90" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D5" s="90">
         <v>2</v>
@@ -33424,10 +33424,10 @@
         <v>2002</v>
       </c>
       <c r="B6" s="93" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C6" s="90" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D6" s="90">
         <v>2</v>
@@ -33475,10 +33475,10 @@
         <v>2100</v>
       </c>
       <c r="B7" s="93" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C7" s="90" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D7" s="90">
         <v>1</v>
@@ -33526,10 +33526,10 @@
         <v>2101</v>
       </c>
       <c r="B8" s="93" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C8" s="90" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D8" s="90">
         <v>1</v>
@@ -33577,10 +33577,10 @@
         <v>2102</v>
       </c>
       <c r="B9" s="93" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C9" s="90" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D9" s="90">
         <v>1</v>
@@ -33628,10 +33628,10 @@
         <v>2103</v>
       </c>
       <c r="B10" s="93" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C10" s="90" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D10" s="90">
         <v>1</v>
@@ -33679,10 +33679,10 @@
         <v>2104</v>
       </c>
       <c r="B11" s="93" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C11" s="90" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D11" s="90">
         <v>1</v>
@@ -33730,10 +33730,10 @@
         <v>2105</v>
       </c>
       <c r="B12" s="93" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C12" s="90" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D12" s="90">
         <v>1</v>
@@ -33781,10 +33781,10 @@
         <v>2106</v>
       </c>
       <c r="B13" s="93" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C13" s="90" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D13" s="90">
         <v>1</v>
@@ -33832,10 +33832,10 @@
         <v>2107</v>
       </c>
       <c r="B14" s="93" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C14" s="90" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D14" s="90">
         <v>1</v>
@@ -33883,10 +33883,10 @@
         <v>2108</v>
       </c>
       <c r="B15" s="93" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C15" s="90" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D15" s="90">
         <v>1</v>
@@ -33934,10 +33934,10 @@
         <v>2109</v>
       </c>
       <c r="B16" s="93" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C16" s="90" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D16" s="90">
         <v>1</v>
@@ -33985,10 +33985,10 @@
         <v>3001</v>
       </c>
       <c r="B17" s="93" t="s">
+        <v>174</v>
+      </c>
+      <c r="C17" s="90" t="s">
         <v>175</v>
-      </c>
-      <c r="C17" s="90" t="s">
-        <v>176</v>
       </c>
       <c r="D17" s="90">
         <v>1</v>
@@ -34032,10 +34032,10 @@
         <v>3002</v>
       </c>
       <c r="B18" s="93" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C18" s="90" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D18" s="90">
         <v>2</v>
@@ -34079,10 +34079,10 @@
         <v>3004</v>
       </c>
       <c r="B19" s="93" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C19" s="90" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D19" s="90">
         <v>2</v>
@@ -34130,10 +34130,10 @@
         <v>3005</v>
       </c>
       <c r="B20" s="93" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C20" s="90" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D20" s="90">
         <v>2</v>
@@ -34181,10 +34181,10 @@
         <v>3006</v>
       </c>
       <c r="B21" s="93" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C21" s="90" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D21" s="90">
         <v>2</v>

</xml_diff>

<commit_message>
Revert "Merge branch 'main' of https://github.com/WT-MWO/pyMasterLoadsTool"
This reverts commit 32c366d4a70f42f1258006f59159d75493cfea1d, reversing
changes made to 1751765ecc837680665f991d32648c2dd55810d5.
</commit_message>
<xml_diff>
--- a/pyMaster_loads_tool.xlsx
+++ b/pyMaster_loads_tool.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://atlec-my.sharepoint.com/personal/mwo_woodthilsted_com/Documents/Professional/5_PYTHON/pyMasterLoadsTool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="11_8A5DF8D2319AF32EF13E9B2AED69841309E87D61" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{83D54F16-90C7-443E-ABBD-7DDC4607E1FD}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="11_8A5DF8D2319AF32EF13E9B2AED69841309E87D61" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{45CF6D4B-FCBF-473E-A9E9-D8A8F18C7DE1}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="858" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8385" yWindow="4260" windowWidth="25860" windowHeight="14880" tabRatio="858" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Load case definition" sheetId="1" r:id="rId1"/>
@@ -189,6 +189,9 @@
   </si>
   <si>
     <t>Projected</t>
+  </si>
+  <si>
+    <t>Auto detect</t>
   </si>
   <si>
     <t xml:space="preserve"> PX2              PY2             PZ2</t>
@@ -589,9 +592,6 @@
   <si>
     <t xml:space="preserve">         CX              CY             CZ
           </t>
-  </si>
-  <si>
-    <t>Contour index</t>
   </si>
 </sst>
 </file>
@@ -1220,13 +1220,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1245,46 +1238,53 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1847,43 +1847,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A1" s="123" t="s">
+      <c r="A1" s="120" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="127" t="s">
+      <c r="B1" s="124" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="126" t="s">
+      <c r="C1" s="123" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="124" t="s">
+      <c r="D1" s="121" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="125"/>
-      <c r="F1" s="125"/>
-      <c r="G1" s="125"/>
-      <c r="H1" s="125"/>
+      <c r="E1" s="122"/>
+      <c r="F1" s="122"/>
+      <c r="G1" s="122"/>
+      <c r="H1" s="122"/>
       <c r="K1" s="100" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="12.95" customHeight="1">
-      <c r="A2" s="121"/>
-      <c r="B2" s="121"/>
-      <c r="C2" s="121"/>
-      <c r="D2" s="120" t="s">
+      <c r="A2" s="118"/>
+      <c r="B2" s="118"/>
+      <c r="C2" s="118"/>
+      <c r="D2" s="117" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="120" t="s">
+      <c r="E2" s="117" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="120" t="s">
+      <c r="F2" s="117" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="120" t="s">
+      <c r="G2" s="117" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="120" t="s">
+      <c r="H2" s="117" t="s">
         <v>9</v>
       </c>
       <c r="J2" s="100" t="s">
@@ -1897,14 +1897,14 @@
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="121"/>
-      <c r="B3" s="121"/>
-      <c r="C3" s="121"/>
-      <c r="D3" s="121"/>
-      <c r="E3" s="121"/>
-      <c r="F3" s="121"/>
-      <c r="G3" s="121"/>
-      <c r="H3" s="121"/>
+      <c r="A3" s="118"/>
+      <c r="B3" s="118"/>
+      <c r="C3" s="118"/>
+      <c r="D3" s="118"/>
+      <c r="E3" s="118"/>
+      <c r="F3" s="118"/>
+      <c r="G3" s="118"/>
+      <c r="H3" s="118"/>
       <c r="J3" s="100" t="s">
         <v>12</v>
       </c>
@@ -1916,14 +1916,14 @@
       </c>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="121"/>
-      <c r="B4" s="121"/>
-      <c r="C4" s="121"/>
-      <c r="D4" s="121"/>
-      <c r="E4" s="121"/>
-      <c r="F4" s="121"/>
-      <c r="G4" s="121"/>
-      <c r="H4" s="121"/>
+      <c r="A4" s="118"/>
+      <c r="B4" s="118"/>
+      <c r="C4" s="118"/>
+      <c r="D4" s="118"/>
+      <c r="E4" s="118"/>
+      <c r="F4" s="118"/>
+      <c r="G4" s="118"/>
+      <c r="H4" s="118"/>
       <c r="J4" s="100" t="s">
         <v>14</v>
       </c>
@@ -1935,14 +1935,14 @@
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="121"/>
-      <c r="B5" s="121"/>
-      <c r="C5" s="121"/>
-      <c r="D5" s="121"/>
-      <c r="E5" s="121"/>
-      <c r="F5" s="121"/>
-      <c r="G5" s="121"/>
-      <c r="H5" s="121"/>
+      <c r="A5" s="118"/>
+      <c r="B5" s="118"/>
+      <c r="C5" s="118"/>
+      <c r="D5" s="118"/>
+      <c r="E5" s="118"/>
+      <c r="F5" s="118"/>
+      <c r="G5" s="118"/>
+      <c r="H5" s="118"/>
       <c r="J5" s="100" t="s">
         <v>16</v>
       </c>
@@ -1954,14 +1954,14 @@
       </c>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="122"/>
-      <c r="B6" s="122"/>
-      <c r="C6" s="122"/>
-      <c r="D6" s="122"/>
-      <c r="E6" s="122"/>
-      <c r="F6" s="122"/>
-      <c r="G6" s="122"/>
-      <c r="H6" s="122"/>
+      <c r="A6" s="119"/>
+      <c r="B6" s="119"/>
+      <c r="C6" s="119"/>
+      <c r="D6" s="119"/>
+      <c r="E6" s="119"/>
+      <c r="F6" s="119"/>
+      <c r="G6" s="119"/>
+      <c r="H6" s="119"/>
       <c r="J6" s="100" t="s">
         <v>18</v>
       </c>
@@ -3821,10 +3821,10 @@
   </sheetPr>
   <dimension ref="A1:AK177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="AE13" sqref="AE13"/>
-      <selection pane="bottomLeft" activeCell="Z9" sqref="Z9"/>
+      <selection pane="bottomLeft" activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
@@ -3884,256 +3884,256 @@
       <c r="Y1" s="15"/>
       <c r="Z1" s="15"/>
       <c r="AA1" s="15"/>
-      <c r="AC1" s="142" t="s">
+      <c r="AC1" s="125" t="s">
         <v>30</v>
       </c>
-      <c r="AD1" s="138"/>
-      <c r="AE1" s="138"/>
-      <c r="AF1" s="139"/>
+      <c r="AD1" s="126"/>
+      <c r="AE1" s="126"/>
+      <c r="AF1" s="127"/>
     </row>
     <row r="2" spans="1:32" ht="12.4" customHeight="1">
-      <c r="A2" s="123" t="s">
+      <c r="A2" s="120" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="127" t="s">
+      <c r="B2" s="124" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="126" t="s">
+      <c r="C2" s="123" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="145"/>
-      <c r="E2" s="143"/>
-      <c r="F2" s="128"/>
-      <c r="G2" s="126" t="s">
+      <c r="D2" s="138"/>
+      <c r="E2" s="128"/>
+      <c r="F2" s="139"/>
+      <c r="G2" s="123" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="130" t="s">
+      <c r="H2" s="140" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="141" t="s">
+      <c r="I2" s="142" t="s">
         <v>32</v>
       </c>
       <c r="J2" s="137" t="s">
         <v>33</v>
       </c>
-      <c r="K2" s="138"/>
-      <c r="L2" s="138"/>
-      <c r="M2" s="138"/>
-      <c r="N2" s="138"/>
-      <c r="O2" s="138"/>
-      <c r="P2" s="138"/>
-      <c r="Q2" s="138"/>
-      <c r="R2" s="138"/>
-      <c r="S2" s="138"/>
-      <c r="T2" s="138"/>
-      <c r="U2" s="138"/>
-      <c r="V2" s="138"/>
-      <c r="W2" s="138"/>
-      <c r="X2" s="138"/>
-      <c r="Y2" s="138"/>
-      <c r="Z2" s="139"/>
-      <c r="AA2" s="120" t="s">
+      <c r="K2" s="126"/>
+      <c r="L2" s="126"/>
+      <c r="M2" s="126"/>
+      <c r="N2" s="126"/>
+      <c r="O2" s="126"/>
+      <c r="P2" s="126"/>
+      <c r="Q2" s="126"/>
+      <c r="R2" s="126"/>
+      <c r="S2" s="126"/>
+      <c r="T2" s="126"/>
+      <c r="U2" s="126"/>
+      <c r="V2" s="126"/>
+      <c r="W2" s="126"/>
+      <c r="X2" s="126"/>
+      <c r="Y2" s="126"/>
+      <c r="Z2" s="127"/>
+      <c r="AA2" s="117" t="s">
         <v>34</v>
       </c>
-      <c r="AC2" s="126" t="s">
+      <c r="AC2" s="123" t="s">
         <v>35</v>
       </c>
-      <c r="AD2" s="126" t="s">
+      <c r="AD2" s="123" t="s">
         <v>36</v>
       </c>
-      <c r="AE2" s="126" t="s">
+      <c r="AE2" s="123" t="s">
         <v>37</v>
       </c>
-      <c r="AF2" s="126" t="s">
+      <c r="AF2" s="123" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:32" ht="12.6" customHeight="1">
-      <c r="A3" s="121"/>
-      <c r="B3" s="121"/>
-      <c r="C3" s="121"/>
+      <c r="A3" s="118"/>
+      <c r="B3" s="118"/>
+      <c r="C3" s="118"/>
       <c r="D3" s="131"/>
-      <c r="E3" s="135"/>
-      <c r="F3" s="129"/>
-      <c r="G3" s="121"/>
+      <c r="E3" s="129"/>
+      <c r="F3" s="132"/>
+      <c r="G3" s="118"/>
       <c r="H3" s="131"/>
-      <c r="I3" s="121"/>
-      <c r="J3" s="140" t="s">
+      <c r="I3" s="118"/>
+      <c r="J3" s="141" t="s">
         <v>39</v>
       </c>
-      <c r="K3" s="133"/>
-      <c r="L3" s="134"/>
-      <c r="M3" s="144" t="s">
-        <v>176</v>
-      </c>
-      <c r="N3" s="133"/>
-      <c r="O3" s="134"/>
-      <c r="P3" s="126" t="s">
+      <c r="K3" s="136"/>
+      <c r="L3" s="130"/>
+      <c r="M3" s="135" t="s">
+        <v>177</v>
+      </c>
+      <c r="N3" s="136"/>
+      <c r="O3" s="130"/>
+      <c r="P3" s="123" t="s">
         <v>40</v>
       </c>
-      <c r="Q3" s="133"/>
-      <c r="R3" s="134"/>
-      <c r="S3" s="120" t="s">
+      <c r="Q3" s="136"/>
+      <c r="R3" s="130"/>
+      <c r="S3" s="117" t="s">
         <v>41</v>
       </c>
-      <c r="T3" s="133"/>
-      <c r="U3" s="134"/>
-      <c r="V3" s="120" t="s">
+      <c r="T3" s="136"/>
+      <c r="U3" s="130"/>
+      <c r="V3" s="117" t="s">
         <v>42</v>
       </c>
-      <c r="W3" s="120" t="s">
+      <c r="W3" s="117" t="s">
         <v>43</v>
       </c>
-      <c r="X3" s="134"/>
-      <c r="Y3" s="120" t="s">
+      <c r="X3" s="130"/>
+      <c r="Y3" s="117" t="s">
         <v>44</v>
       </c>
-      <c r="Z3" s="120" t="s">
-        <v>177</v>
-      </c>
-      <c r="AA3" s="121"/>
-      <c r="AC3" s="121"/>
-      <c r="AD3" s="121"/>
-      <c r="AE3" s="121"/>
-      <c r="AF3" s="121"/>
+      <c r="Z3" s="117" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA3" s="118"/>
+      <c r="AC3" s="118"/>
+      <c r="AD3" s="118"/>
+      <c r="AE3" s="118"/>
+      <c r="AF3" s="118"/>
     </row>
     <row r="4" spans="1:32" ht="12.6" customHeight="1">
-      <c r="A4" s="121"/>
-      <c r="B4" s="121"/>
-      <c r="C4" s="121"/>
+      <c r="A4" s="118"/>
+      <c r="B4" s="118"/>
+      <c r="C4" s="118"/>
       <c r="D4" s="131"/>
-      <c r="E4" s="135"/>
-      <c r="F4" s="129"/>
-      <c r="G4" s="121"/>
+      <c r="E4" s="129"/>
+      <c r="F4" s="132"/>
+      <c r="G4" s="118"/>
       <c r="H4" s="131"/>
-      <c r="I4" s="121"/>
+      <c r="I4" s="118"/>
       <c r="J4" s="131"/>
-      <c r="K4" s="135"/>
-      <c r="L4" s="129"/>
+      <c r="K4" s="129"/>
+      <c r="L4" s="132"/>
       <c r="M4" s="131"/>
-      <c r="N4" s="135"/>
-      <c r="O4" s="129"/>
+      <c r="N4" s="129"/>
+      <c r="O4" s="132"/>
       <c r="P4" s="131"/>
-      <c r="Q4" s="135"/>
-      <c r="R4" s="129"/>
+      <c r="Q4" s="129"/>
+      <c r="R4" s="132"/>
       <c r="S4" s="131"/>
-      <c r="T4" s="135"/>
-      <c r="U4" s="129"/>
-      <c r="V4" s="121"/>
+      <c r="T4" s="129"/>
+      <c r="U4" s="132"/>
+      <c r="V4" s="118"/>
       <c r="W4" s="131"/>
-      <c r="X4" s="129"/>
-      <c r="Y4" s="121"/>
-      <c r="Z4" s="121"/>
-      <c r="AA4" s="121"/>
-      <c r="AC4" s="121"/>
-      <c r="AD4" s="121"/>
-      <c r="AE4" s="121"/>
-      <c r="AF4" s="121"/>
+      <c r="X4" s="132"/>
+      <c r="Y4" s="118"/>
+      <c r="Z4" s="118"/>
+      <c r="AA4" s="118"/>
+      <c r="AC4" s="118"/>
+      <c r="AD4" s="118"/>
+      <c r="AE4" s="118"/>
+      <c r="AF4" s="118"/>
     </row>
     <row r="5" spans="1:32" ht="25.15" customHeight="1">
-      <c r="A5" s="121"/>
-      <c r="B5" s="121"/>
-      <c r="C5" s="121"/>
+      <c r="A5" s="118"/>
+      <c r="B5" s="118"/>
+      <c r="C5" s="118"/>
       <c r="D5" s="131"/>
-      <c r="E5" s="135"/>
-      <c r="F5" s="129"/>
-      <c r="G5" s="121"/>
+      <c r="E5" s="129"/>
+      <c r="F5" s="132"/>
+      <c r="G5" s="118"/>
       <c r="H5" s="131"/>
-      <c r="I5" s="121"/>
+      <c r="I5" s="118"/>
       <c r="J5" s="131"/>
-      <c r="K5" s="135"/>
-      <c r="L5" s="129"/>
+      <c r="K5" s="129"/>
+      <c r="L5" s="132"/>
       <c r="M5" s="131"/>
-      <c r="N5" s="135"/>
-      <c r="O5" s="129"/>
+      <c r="N5" s="129"/>
+      <c r="O5" s="132"/>
       <c r="P5" s="131"/>
-      <c r="Q5" s="135"/>
-      <c r="R5" s="129"/>
+      <c r="Q5" s="129"/>
+      <c r="R5" s="132"/>
       <c r="S5" s="131"/>
-      <c r="T5" s="135"/>
-      <c r="U5" s="129"/>
-      <c r="V5" s="121"/>
+      <c r="T5" s="129"/>
+      <c r="U5" s="132"/>
+      <c r="V5" s="118"/>
       <c r="W5" s="131"/>
-      <c r="X5" s="129"/>
-      <c r="Y5" s="121"/>
-      <c r="Z5" s="121"/>
-      <c r="AA5" s="121"/>
-      <c r="AC5" s="121"/>
-      <c r="AD5" s="121"/>
-      <c r="AE5" s="121"/>
-      <c r="AF5" s="121"/>
+      <c r="X5" s="132"/>
+      <c r="Y5" s="118"/>
+      <c r="Z5" s="118"/>
+      <c r="AA5" s="118"/>
+      <c r="AC5" s="118"/>
+      <c r="AD5" s="118"/>
+      <c r="AE5" s="118"/>
+      <c r="AF5" s="118"/>
     </row>
     <row r="6" spans="1:32" ht="12.6" customHeight="1">
-      <c r="A6" s="121"/>
-      <c r="B6" s="121"/>
-      <c r="C6" s="121"/>
+      <c r="A6" s="118"/>
+      <c r="B6" s="118"/>
+      <c r="C6" s="118"/>
       <c r="D6" s="131"/>
-      <c r="E6" s="135"/>
-      <c r="F6" s="129"/>
-      <c r="G6" s="121"/>
+      <c r="E6" s="129"/>
+      <c r="F6" s="132"/>
+      <c r="G6" s="118"/>
       <c r="H6" s="131"/>
-      <c r="I6" s="121"/>
-      <c r="J6" s="132"/>
-      <c r="K6" s="125"/>
-      <c r="L6" s="136"/>
-      <c r="M6" s="132"/>
-      <c r="N6" s="125"/>
-      <c r="O6" s="136"/>
+      <c r="I6" s="118"/>
+      <c r="J6" s="133"/>
+      <c r="K6" s="122"/>
+      <c r="L6" s="134"/>
+      <c r="M6" s="133"/>
+      <c r="N6" s="122"/>
+      <c r="O6" s="134"/>
       <c r="P6" s="131"/>
-      <c r="Q6" s="135"/>
-      <c r="R6" s="129"/>
-      <c r="S6" s="132"/>
-      <c r="T6" s="125"/>
-      <c r="U6" s="136"/>
-      <c r="V6" s="121"/>
+      <c r="Q6" s="129"/>
+      <c r="R6" s="132"/>
+      <c r="S6" s="133"/>
+      <c r="T6" s="122"/>
+      <c r="U6" s="134"/>
+      <c r="V6" s="118"/>
       <c r="W6" s="131"/>
-      <c r="X6" s="129"/>
-      <c r="Y6" s="121"/>
-      <c r="Z6" s="121"/>
-      <c r="AA6" s="121"/>
-      <c r="AC6" s="121"/>
-      <c r="AD6" s="121"/>
-      <c r="AE6" s="121"/>
-      <c r="AF6" s="121"/>
+      <c r="X6" s="132"/>
+      <c r="Y6" s="118"/>
+      <c r="Z6" s="118"/>
+      <c r="AA6" s="118"/>
+      <c r="AC6" s="118"/>
+      <c r="AD6" s="118"/>
+      <c r="AE6" s="118"/>
+      <c r="AF6" s="118"/>
     </row>
     <row r="7" spans="1:32">
-      <c r="A7" s="122"/>
-      <c r="B7" s="122"/>
-      <c r="C7" s="122"/>
+      <c r="A7" s="119"/>
+      <c r="B7" s="119"/>
+      <c r="C7" s="119"/>
       <c r="D7" s="131"/>
-      <c r="E7" s="135"/>
-      <c r="F7" s="129"/>
-      <c r="G7" s="122"/>
-      <c r="H7" s="132"/>
-      <c r="I7" s="122"/>
+      <c r="E7" s="129"/>
+      <c r="F7" s="132"/>
+      <c r="G7" s="119"/>
+      <c r="H7" s="133"/>
+      <c r="I7" s="119"/>
       <c r="J7" s="137" t="s">
-        <v>45</v>
-      </c>
-      <c r="K7" s="138"/>
-      <c r="L7" s="139"/>
+        <v>46</v>
+      </c>
+      <c r="K7" s="126"/>
+      <c r="L7" s="127"/>
       <c r="M7" s="137" t="s">
-        <v>46</v>
-      </c>
-      <c r="N7" s="138"/>
-      <c r="O7" s="139"/>
-      <c r="P7" s="132"/>
-      <c r="Q7" s="125"/>
-      <c r="R7" s="136"/>
+        <v>47</v>
+      </c>
+      <c r="N7" s="126"/>
+      <c r="O7" s="127"/>
+      <c r="P7" s="133"/>
+      <c r="Q7" s="122"/>
+      <c r="R7" s="134"/>
       <c r="S7" s="137" t="s">
-        <v>47</v>
-      </c>
-      <c r="T7" s="138"/>
-      <c r="U7" s="139"/>
-      <c r="V7" s="122"/>
-      <c r="W7" s="132"/>
-      <c r="X7" s="136"/>
-      <c r="Y7" s="122"/>
-      <c r="Z7" s="122"/>
-      <c r="AA7" s="122"/>
-      <c r="AC7" s="122"/>
-      <c r="AD7" s="122"/>
-      <c r="AE7" s="122"/>
-      <c r="AF7" s="122"/>
+        <v>48</v>
+      </c>
+      <c r="T7" s="126"/>
+      <c r="U7" s="127"/>
+      <c r="V7" s="119"/>
+      <c r="W7" s="133"/>
+      <c r="X7" s="134"/>
+      <c r="Y7" s="119"/>
+      <c r="Z7" s="119"/>
+      <c r="AA7" s="119"/>
+      <c r="AC7" s="119"/>
+      <c r="AD7" s="119"/>
+      <c r="AE7" s="119"/>
+      <c r="AF7" s="119"/>
     </row>
     <row r="8" spans="1:32">
       <c r="A8" s="108">
@@ -4148,7 +4148,7 @@
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="56" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F8" s="15"/>
       <c r="G8" s="18" t="str">
@@ -4156,7 +4156,7 @@
         <v>1:STA1</v>
       </c>
       <c r="H8" s="40" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I8" s="96">
         <v>1</v>
@@ -4183,7 +4183,7 @@
       <c r="AD8" s="60"/>
       <c r="AE8" s="60"/>
       <c r="AF8" s="60" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:32">
@@ -4195,7 +4195,7 @@
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="56" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F9" s="15"/>
       <c r="G9" s="19" t="str">
@@ -4204,7 +4204,7 @@
       </c>
       <c r="H9" s="40"/>
       <c r="I9" s="96" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J9" s="77">
         <v>0</v>
@@ -4244,7 +4244,7 @@
       </c>
       <c r="V9" s="80"/>
       <c r="W9" s="81" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="X9" s="72"/>
       <c r="Y9" s="15">
@@ -4256,7 +4256,7 @@
       <c r="AD9" s="61"/>
       <c r="AE9" s="61"/>
       <c r="AF9" s="61" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:32">
@@ -4275,7 +4275,7 @@
       </c>
       <c r="H10" s="40"/>
       <c r="I10" s="96" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J10" s="77">
         <v>0</v>
@@ -4315,7 +4315,7 @@
       </c>
       <c r="V10" s="80"/>
       <c r="W10" s="81" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="X10" s="72"/>
       <c r="Y10" s="15">
@@ -4327,7 +4327,7 @@
       <c r="AD10" s="61"/>
       <c r="AE10" s="61"/>
       <c r="AF10" s="61" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:32">
@@ -4339,7 +4339,7 @@
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="56" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F11" s="15"/>
       <c r="G11" s="19" t="str">
@@ -4348,7 +4348,7 @@
       </c>
       <c r="H11" s="40"/>
       <c r="I11" s="96" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J11" s="77">
         <v>0</v>
@@ -4388,7 +4388,7 @@
       </c>
       <c r="V11" s="80"/>
       <c r="W11" s="81" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="X11" s="72"/>
       <c r="Y11" s="15">
@@ -4400,7 +4400,7 @@
       <c r="AD11" s="61"/>
       <c r="AE11" s="61"/>
       <c r="AF11" s="61" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:32">
@@ -4412,7 +4412,7 @@
       </c>
       <c r="D12" s="15"/>
       <c r="E12" s="56" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F12" s="15"/>
       <c r="G12" s="19" t="str">
@@ -4421,7 +4421,7 @@
       </c>
       <c r="H12" s="40"/>
       <c r="I12" s="97" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J12" s="77">
         <v>0</v>
@@ -4461,7 +4461,7 @@
       </c>
       <c r="V12" s="61"/>
       <c r="W12" s="81" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="X12" s="72"/>
       <c r="Y12" s="15">
@@ -4483,7 +4483,7 @@
       </c>
       <c r="D13" s="15"/>
       <c r="E13" s="56" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F13" s="15"/>
       <c r="G13" s="19" t="str">
@@ -4524,7 +4524,7 @@
       </c>
       <c r="D14" s="15"/>
       <c r="E14" s="56" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F14" s="15"/>
       <c r="G14" s="19" t="str">
@@ -4643,7 +4643,7 @@
       </c>
       <c r="D17" s="15"/>
       <c r="E17" s="56" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F17" s="15"/>
       <c r="G17" s="19" t="str">
@@ -4762,7 +4762,7 @@
       </c>
       <c r="D20" s="15"/>
       <c r="E20" s="56" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F20" s="15"/>
       <c r="G20" s="19" t="str">
@@ -4881,7 +4881,7 @@
       </c>
       <c r="D23" s="15"/>
       <c r="E23" s="56" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F23" s="15"/>
       <c r="G23" s="19" t="str">
@@ -5000,7 +5000,7 @@
       </c>
       <c r="D26" s="15"/>
       <c r="E26" s="56" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F26" s="15"/>
       <c r="G26" s="19" t="str">
@@ -5119,7 +5119,7 @@
       </c>
       <c r="D29" s="15"/>
       <c r="E29" s="56" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F29" s="15"/>
       <c r="G29" s="19" t="str">
@@ -5238,7 +5238,7 @@
       </c>
       <c r="D32" s="15"/>
       <c r="E32" s="56" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F32" s="15"/>
       <c r="G32" s="19" t="str">
@@ -5357,7 +5357,7 @@
       </c>
       <c r="D35" s="15"/>
       <c r="E35" s="56" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F35" s="15"/>
       <c r="G35" s="19" t="str">
@@ -10929,6 +10929,17 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="F2:F7"/>
+    <mergeCell ref="H2:H7"/>
+    <mergeCell ref="Y3:Y7"/>
+    <mergeCell ref="S3:U6"/>
+    <mergeCell ref="P3:R7"/>
+    <mergeCell ref="S7:U7"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="J3:L6"/>
+    <mergeCell ref="G2:G7"/>
+    <mergeCell ref="I2:I7"/>
+    <mergeCell ref="J7:L7"/>
     <mergeCell ref="AC1:AF1"/>
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="C2:C7"/>
@@ -10945,17 +10956,6 @@
     <mergeCell ref="B2:B7"/>
     <mergeCell ref="AE2:AE7"/>
     <mergeCell ref="D2:D7"/>
-    <mergeCell ref="F2:F7"/>
-    <mergeCell ref="H2:H7"/>
-    <mergeCell ref="Y3:Y7"/>
-    <mergeCell ref="S3:U6"/>
-    <mergeCell ref="P3:R7"/>
-    <mergeCell ref="S7:U7"/>
-    <mergeCell ref="M7:O7"/>
-    <mergeCell ref="J3:L6"/>
-    <mergeCell ref="G2:G7"/>
-    <mergeCell ref="I2:I7"/>
-    <mergeCell ref="J7:L7"/>
   </mergeCells>
   <conditionalFormatting sqref="I1:I1048576">
     <cfRule type="expression" dxfId="28" priority="41">
@@ -11057,7 +11057,7 @@
       <formula>$H8 &lt;&gt; "(FE) uniform"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations xWindow="1747" yWindow="323" count="25">
+  <dataValidations disablePrompts="1" xWindow="1747" yWindow="323" count="25">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="(FOR TRAPEZOIDAL LOADS ONLY)_x000a_PX1 - Enter your starting load in the X direction (kN/m)_x000a__x000a_PY1 - Enter your starting load in the Y direction (kN/m)_x000a__x000a_PZ1 - Enter your starting load in the Z direction (kN/m)" sqref="M7:O7" xr:uid="{00000000-0002-0000-0100-000000000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="(FOR TRAPEZOIDAL LOADS ONLY)_x000a_x2 - Absolute or relative distance of end of load along a member (m or m/L)_x000a__x000a_x1 - Absolute or relative distance of start of load along a member (m or m/L)" sqref="S7:U7" xr:uid="{00000000-0002-0000-0100-000001000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="(FOR TRAPEZOIDAL LOADS ONLY)_x000a_PX2 - Enter your finishing load in the X direction (kN/m)_x000a__x000a_PY2 - Enter your finishing load in the Y direction (kN/m)_x000a__x000a_PZ2 - Enter your finishing load in the Z direction (kN/m)" sqref="J7:L7" xr:uid="{00000000-0002-0000-0100-000002000000}"/>
@@ -11088,7 +11088,7 @@
       <formula2>150</formula2>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="1-Projected, 0- Not projected_x000a_" sqref="Y3:Y7" xr:uid="{00000000-0002-0000-0100-000016000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Contour identification index_x000a_" sqref="Z3:Z7" xr:uid="{00000000-0002-0000-0100-000017000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="1, 0 - For load on contour auto detect panels_x000a_" sqref="Z3:Z7" xr:uid="{00000000-0002-0000-0100-000017000000}"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H8:H177" xr:uid="{69C6861F-E4DE-4C73-AD67-80357667F890}">
       <formula1>"(FE) uniform, nodal force, member force, self-weight, trapezoidal load (2p), uniform load, (FE) linear load on edges, load on contour, load 3p on contour"</formula1>
     </dataValidation>
@@ -11500,17 +11500,17 @@
     </row>
     <row r="3" spans="1:4605" s="7" customFormat="1" ht="218.65" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="53" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="69" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F3" s="69" t="s">
         <v>7</v>
@@ -16123,12 +16123,12 @@
       <c r="A4" s="3"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
-      <c r="D4" s="146" t="s">
+      <c r="D4" s="143" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="133"/>
-      <c r="F4" s="133"/>
-      <c r="G4" s="133"/>
+      <c r="E4" s="136"/>
+      <c r="F4" s="136"/>
+      <c r="G4" s="136"/>
       <c r="H4" s="84">
         <v>1</v>
       </c>
@@ -20735,9 +20735,9 @@
       <c r="B5" s="21"/>
       <c r="C5" s="21"/>
       <c r="D5" s="131"/>
-      <c r="E5" s="147"/>
-      <c r="F5" s="147"/>
-      <c r="G5" s="147"/>
+      <c r="E5" s="144"/>
+      <c r="F5" s="144"/>
+      <c r="G5" s="144"/>
       <c r="H5" s="84"/>
       <c r="I5" s="84"/>
       <c r="J5" s="84"/>
@@ -21108,19 +21108,19 @@
       <c r="NK5" s="50"/>
     </row>
     <row r="6" spans="1:4605" s="4" customFormat="1" ht="15.6" customHeight="1">
-      <c r="A6" s="119" t="s">
-        <v>57</v>
-      </c>
-      <c r="B6" s="119" t="s">
+      <c r="A6" s="147" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="119" t="s">
+      <c r="B6" s="147" t="s">
         <v>59</v>
       </c>
-      <c r="D6" s="117"/>
-      <c r="E6" s="118"/>
-      <c r="F6" s="118"/>
-      <c r="G6" s="118"/>
+      <c r="C6" s="147" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" s="145"/>
+      <c r="E6" s="146"/>
+      <c r="F6" s="146"/>
+      <c r="G6" s="146"/>
       <c r="H6" s="84"/>
       <c r="I6" s="84"/>
       <c r="J6" s="84"/>
@@ -31997,81 +31997,81 @@
   <sheetData>
     <row r="1" spans="1:23">
       <c r="A1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" t="s">
         <v>61</v>
       </c>
-      <c r="G1" t="s">
-        <v>60</v>
-      </c>
       <c r="H1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="M1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="N1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="S1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="T1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:23">
       <c r="A2" s="100" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B2" s="100" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="100" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="100" t="s">
+      <c r="H2" t="s">
         <v>67</v>
       </c>
-      <c r="D2" t="s">
+      <c r="I2" t="s">
         <v>68</v>
       </c>
-      <c r="G2" t="s">
-        <v>65</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
+        <v>69</v>
+      </c>
+      <c r="M2" t="s">
         <v>66</v>
       </c>
-      <c r="I2" t="s">
+      <c r="N2" t="s">
         <v>67</v>
       </c>
-      <c r="J2" t="s">
+      <c r="O2" t="s">
         <v>68</v>
       </c>
-      <c r="M2" t="s">
-        <v>65</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
+        <v>69</v>
+      </c>
+      <c r="S2" t="s">
         <v>66</v>
       </c>
-      <c r="O2" t="s">
+      <c r="T2" t="s">
         <v>67</v>
       </c>
-      <c r="P2" t="s">
+      <c r="U2" t="s">
         <v>68</v>
       </c>
-      <c r="S2" t="s">
-        <v>65</v>
-      </c>
-      <c r="T2" t="s">
-        <v>66</v>
-      </c>
-      <c r="U2" t="s">
-        <v>67</v>
-      </c>
       <c r="V2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="W2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:23">
@@ -32124,7 +32124,7 @@
         <v>0</v>
       </c>
       <c r="W3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:23">
@@ -32177,7 +32177,7 @@
         <v>0</v>
       </c>
       <c r="W4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:23">
@@ -32230,7 +32230,7 @@
         <v>0</v>
       </c>
       <c r="W5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:23">
@@ -32428,81 +32428,81 @@
   <sheetData>
     <row r="1" spans="1:23">
       <c r="A1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" t="s">
         <v>61</v>
       </c>
-      <c r="G1" t="s">
-        <v>60</v>
-      </c>
       <c r="H1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="M1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="N1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="S1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="T1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:23">
       <c r="A2" s="100" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B2" s="100" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="100" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="100" t="s">
+      <c r="H2" t="s">
         <v>67</v>
       </c>
-      <c r="D2" t="s">
+      <c r="I2" t="s">
         <v>68</v>
       </c>
-      <c r="G2" t="s">
-        <v>65</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
+        <v>69</v>
+      </c>
+      <c r="M2" t="s">
         <v>66</v>
       </c>
-      <c r="I2" t="s">
+      <c r="N2" t="s">
         <v>67</v>
       </c>
-      <c r="J2" t="s">
+      <c r="O2" t="s">
         <v>68</v>
       </c>
-      <c r="M2" t="s">
-        <v>65</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
+        <v>69</v>
+      </c>
+      <c r="S2" t="s">
         <v>66</v>
       </c>
-      <c r="O2" t="s">
+      <c r="T2" t="s">
         <v>67</v>
       </c>
-      <c r="P2" t="s">
+      <c r="U2" t="s">
         <v>68</v>
       </c>
-      <c r="S2" t="s">
-        <v>65</v>
-      </c>
-      <c r="T2" t="s">
-        <v>66</v>
-      </c>
-      <c r="U2" t="s">
-        <v>67</v>
-      </c>
       <c r="V2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="W2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:23">
@@ -32555,7 +32555,7 @@
         <v>0</v>
       </c>
       <c r="W3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:23">
@@ -32608,7 +32608,7 @@
         <v>0</v>
       </c>
       <c r="W4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:23">
@@ -32661,7 +32661,7 @@
         <v>0</v>
       </c>
       <c r="W5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:23">
@@ -32880,7 +32880,7 @@
   <sheetData>
     <row r="1" spans="1:20" ht="13.5" customHeight="1" thickBot="1">
       <c r="A1" s="17" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F1" s="24">
         <v>0.5</v>
@@ -32889,77 +32889,77 @@
         <v>0.1</v>
       </c>
       <c r="M1" s="17" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="S1" s="17" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="15.75" customHeight="1">
       <c r="A2" s="17" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H2" s="25" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="K2" s="17" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="M2" s="17" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="N2" s="17" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O2" s="17">
         <v>1</v>
       </c>
       <c r="P2" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="S2" s="17" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="T2" s="17" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="39" customHeight="1">
       <c r="A3" s="17" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F3" s="25" t="e">
         <f>PlatformName &amp;" member utilisations $&gt;" &amp;F1&amp;"$"</f>
@@ -32974,107 +32974,107 @@
         <v>#REF!</v>
       </c>
       <c r="J3" s="26" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="K3" s="25" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="M3" s="17" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="N3" s="17" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O3" s="17">
         <v>1</v>
       </c>
       <c r="P3" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="S3" s="17" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="T3" s="26" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="15.75" customHeight="1">
       <c r="A4" s="17" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H4" s="25" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="M4" s="17" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="N4" s="17" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O4" s="17">
         <v>1</v>
       </c>
       <c r="P4" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="S4" s="17" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="15.75" customHeight="1">
       <c r="B5" s="17" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H5" s="25" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="M5" s="17" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="N5" s="17" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O5" s="17">
         <v>1</v>
       </c>
       <c r="P5" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="S5" s="17" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="15.75" customHeight="1">
@@ -33103,19 +33103,19 @@
         <v>#REF!</v>
       </c>
       <c r="H6" s="25" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="M6" s="17" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="N6" s="17" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O6" s="17">
         <v>1</v>
       </c>
       <c r="P6" s="17" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="S6" s="17" t="e">
         <f>"\includegraphics[width=\textwidth]{\"&amp;LaTeXFiguresFolder &amp;"\"&amp;PlatformName&amp; " "&amp;S3&amp;".png} "</f>
@@ -33148,61 +33148,61 @@
         <v>#REF!</v>
       </c>
       <c r="H7" s="25" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="J7" s="17">
         <f>COLUMN(J1)</f>
         <v>10</v>
       </c>
       <c r="M7" s="17" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="N7" s="17" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O7" s="17">
         <v>1</v>
       </c>
       <c r="P7" s="17" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="S7" s="17" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="15.75" customHeight="1">
       <c r="B8" s="17" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H8" s="25" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="M8" s="17" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="N8" s="17" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O8" s="17">
         <v>1</v>
       </c>
       <c r="P8" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="S8" s="17" t="e">
         <f>"    \caption{" &amp;PlatformName&amp; " " &amp; S3 &amp;".}"</f>
@@ -33211,37 +33211,37 @@
     </row>
     <row r="9" spans="1:20" ht="15.75" customHeight="1">
       <c r="B9" s="17" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H9" s="25" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="M9" s="17" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="N9" s="17" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O9" s="17">
         <v>1</v>
       </c>
       <c r="P9" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="S9" s="17" t="e">
         <f>"    \label{tabl:" &amp; PlatformName &amp;" "&amp;S3 &amp;"}"</f>
@@ -33250,107 +33250,107 @@
     </row>
     <row r="10" spans="1:20" ht="16.5" customHeight="1">
       <c r="B10" s="47" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H10" s="25" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="M10" s="17" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="N10" s="17" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O10" s="17">
         <v>1</v>
       </c>
       <c r="P10" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:20" ht="16.5" customHeight="1">
       <c r="B11" s="47" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C11" s="47" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D11" s="47" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E11" s="47" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F11" s="47" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="G11" s="47" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H11" s="25" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="M11" s="17" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="N11" s="17" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O11" s="17">
         <v>1</v>
       </c>
       <c r="P11" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="15.75" customHeight="1">
       <c r="H12" s="25" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="M12" s="17" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="N12" s="17" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O12" s="17">
         <v>1</v>
       </c>
       <c r="P12" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="16.5" customHeight="1">
       <c r="C13" s="47"/>
       <c r="H13" s="25" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="M13" s="17" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="N13" s="17" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O13" s="17">
         <v>1</v>
       </c>
       <c r="P13" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="16.5" customHeight="1">
@@ -33360,16 +33360,16 @@
         <v>#REF!</v>
       </c>
       <c r="M14" s="17" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="N14" s="17" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O14" s="17">
         <v>1</v>
       </c>
       <c r="P14" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="S14" s="26"/>
     </row>
@@ -33380,49 +33380,49 @@
         <v>#REF!</v>
       </c>
       <c r="M15" s="17" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="N15" s="17" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O15" s="17">
         <v>1</v>
       </c>
       <c r="P15" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="16.5" customHeight="1">
       <c r="C16" s="47"/>
       <c r="H16" s="25" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="M16" s="17" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="N16" s="17" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O16" s="17">
         <v>1</v>
       </c>
       <c r="P16" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="3:16" ht="16.5" customHeight="1">
       <c r="C17" s="47"/>
       <c r="M17" s="17" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="N17" s="17" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O17" s="17">
         <v>1</v>
       </c>
       <c r="P17" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="3:16" ht="16.5" customHeight="1">
@@ -33486,79 +33486,79 @@
   <sheetData>
     <row r="1" spans="1:25">
       <c r="A1" s="28" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B1" s="29" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C1" s="29" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D1" s="30" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E1" s="29" t="s">
+        <v>152</v>
+      </c>
+      <c r="F1" s="29" t="s">
         <v>151</v>
       </c>
-      <c r="F1" s="29" t="s">
-        <v>150</v>
-      </c>
       <c r="G1" s="29" t="s">
+        <v>152</v>
+      </c>
+      <c r="H1" s="29" t="s">
         <v>151</v>
       </c>
-      <c r="H1" s="29" t="s">
-        <v>150</v>
-      </c>
       <c r="I1" s="29" t="s">
+        <v>152</v>
+      </c>
+      <c r="J1" s="29" t="s">
         <v>151</v>
       </c>
-      <c r="J1" s="29" t="s">
-        <v>150</v>
-      </c>
       <c r="K1" s="29" t="s">
+        <v>152</v>
+      </c>
+      <c r="L1" s="29" t="s">
         <v>151</v>
       </c>
-      <c r="L1" s="29" t="s">
-        <v>150</v>
-      </c>
       <c r="M1" s="29" t="s">
+        <v>152</v>
+      </c>
+      <c r="N1" s="29" t="s">
         <v>151</v>
       </c>
-      <c r="N1" s="29" t="s">
-        <v>150</v>
-      </c>
       <c r="O1" s="29" t="s">
+        <v>152</v>
+      </c>
+      <c r="P1" s="29" t="s">
         <v>151</v>
       </c>
-      <c r="P1" s="29" t="s">
-        <v>150</v>
-      </c>
       <c r="Q1" s="29" t="s">
+        <v>152</v>
+      </c>
+      <c r="R1" s="29" t="s">
         <v>151</v>
       </c>
-      <c r="R1" s="29" t="s">
-        <v>150</v>
-      </c>
       <c r="S1" s="29" t="s">
+        <v>152</v>
+      </c>
+      <c r="T1" s="29" t="s">
         <v>151</v>
       </c>
-      <c r="T1" s="29" t="s">
-        <v>150</v>
-      </c>
       <c r="U1" s="29" t="s">
+        <v>152</v>
+      </c>
+      <c r="V1" s="29" t="s">
         <v>151</v>
       </c>
-      <c r="V1" s="29" t="s">
-        <v>150</v>
-      </c>
       <c r="W1" s="29" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="X1" s="33" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="Y1" s="29" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:25">
@@ -33566,10 +33566,10 @@
         <v>1000</v>
       </c>
       <c r="B2" s="86" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C2" s="87" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D2" s="85">
         <v>1</v>
@@ -33609,10 +33609,10 @@
         <v>1001</v>
       </c>
       <c r="B3" s="90" t="s">
+        <v>157</v>
+      </c>
+      <c r="C3" s="87" t="s">
         <v>156</v>
-      </c>
-      <c r="C3" s="87" t="s">
-        <v>155</v>
       </c>
       <c r="D3" s="87">
         <v>2</v>
@@ -33652,10 +33652,10 @@
         <v>2000</v>
       </c>
       <c r="B4" s="90" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C4" s="87" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D4" s="87">
         <v>2</v>
@@ -33703,10 +33703,10 @@
         <v>2001</v>
       </c>
       <c r="B5" s="90" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C5" s="87" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D5" s="87">
         <v>2</v>
@@ -33754,10 +33754,10 @@
         <v>2002</v>
       </c>
       <c r="B6" s="90" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C6" s="87" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D6" s="87">
         <v>2</v>
@@ -33805,10 +33805,10 @@
         <v>2100</v>
       </c>
       <c r="B7" s="90" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C7" s="87" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D7" s="87">
         <v>1</v>
@@ -33856,10 +33856,10 @@
         <v>2101</v>
       </c>
       <c r="B8" s="90" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C8" s="87" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D8" s="87">
         <v>1</v>
@@ -33907,10 +33907,10 @@
         <v>2102</v>
       </c>
       <c r="B9" s="90" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C9" s="87" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D9" s="87">
         <v>1</v>
@@ -33958,10 +33958,10 @@
         <v>2103</v>
       </c>
       <c r="B10" s="90" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C10" s="87" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D10" s="87">
         <v>1</v>
@@ -34009,10 +34009,10 @@
         <v>2104</v>
       </c>
       <c r="B11" s="90" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C11" s="87" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D11" s="87">
         <v>1</v>
@@ -34060,10 +34060,10 @@
         <v>2105</v>
       </c>
       <c r="B12" s="90" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C12" s="87" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D12" s="87">
         <v>1</v>
@@ -34111,10 +34111,10 @@
         <v>2106</v>
       </c>
       <c r="B13" s="90" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C13" s="87" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D13" s="87">
         <v>1</v>
@@ -34162,10 +34162,10 @@
         <v>2107</v>
       </c>
       <c r="B14" s="90" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C14" s="87" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D14" s="87">
         <v>1</v>
@@ -34213,10 +34213,10 @@
         <v>2108</v>
       </c>
       <c r="B15" s="90" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C15" s="87" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D15" s="87">
         <v>1</v>
@@ -34264,10 +34264,10 @@
         <v>2109</v>
       </c>
       <c r="B16" s="90" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C16" s="87" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D16" s="87">
         <v>1</v>
@@ -34315,10 +34315,10 @@
         <v>3001</v>
       </c>
       <c r="B17" s="90" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C17" s="87" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D17" s="87">
         <v>1</v>
@@ -34362,10 +34362,10 @@
         <v>3002</v>
       </c>
       <c r="B18" s="90" t="s">
+        <v>173</v>
+      </c>
+      <c r="C18" s="87" t="s">
         <v>172</v>
-      </c>
-      <c r="C18" s="87" t="s">
-        <v>171</v>
       </c>
       <c r="D18" s="87">
         <v>2</v>
@@ -34409,10 +34409,10 @@
         <v>3004</v>
       </c>
       <c r="B19" s="90" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C19" s="87" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D19" s="87">
         <v>2</v>
@@ -34460,10 +34460,10 @@
         <v>3005</v>
       </c>
       <c r="B20" s="90" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C20" s="87" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D20" s="87">
         <v>2</v>
@@ -34511,10 +34511,10 @@
         <v>3006</v>
       </c>
       <c r="B21" s="90" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C21" s="87" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D21" s="87">
         <v>2</v>

</xml_diff>

<commit_message>
Reapply "Merge branch 'main' of https://github.com/WT-MWO/pyMasterLoadsTool"
This reverts commit 75aa5212d00be97172672b141ab3f95e95a42be9.
</commit_message>
<xml_diff>
--- a/pyMaster_loads_tool.xlsx
+++ b/pyMaster_loads_tool.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://atlec-my.sharepoint.com/personal/mwo_woodthilsted_com/Documents/Professional/5_PYTHON/pyMasterLoadsTool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="11_8A5DF8D2319AF32EF13E9B2AED69841309E87D61" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{45CF6D4B-FCBF-473E-A9E9-D8A8F18C7DE1}"/>
+  <xr:revisionPtr revIDLastSave="39" documentId="11_8A5DF8D2319AF32EF13E9B2AED69841309E87D61" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{83D54F16-90C7-443E-ABBD-7DDC4607E1FD}"/>
   <bookViews>
-    <workbookView xWindow="8385" yWindow="4260" windowWidth="25860" windowHeight="14880" tabRatio="858" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="858" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Load case definition" sheetId="1" r:id="rId1"/>
@@ -189,9 +189,6 @@
   </si>
   <si>
     <t>Projected</t>
-  </si>
-  <si>
-    <t>Auto detect</t>
   </si>
   <si>
     <t xml:space="preserve"> PX2              PY2             PZ2</t>
@@ -592,6 +589,9 @@
   <si>
     <t xml:space="preserve">         CX              CY             CZ
           </t>
+  </si>
+  <si>
+    <t>Contour index</t>
   </si>
 </sst>
 </file>
@@ -1220,6 +1220,13 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1238,53 +1245,46 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1847,43 +1847,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="123" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="124" t="s">
+      <c r="B1" s="127" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="123" t="s">
+      <c r="C1" s="126" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="121" t="s">
+      <c r="D1" s="124" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="122"/>
-      <c r="F1" s="122"/>
-      <c r="G1" s="122"/>
-      <c r="H1" s="122"/>
+      <c r="E1" s="125"/>
+      <c r="F1" s="125"/>
+      <c r="G1" s="125"/>
+      <c r="H1" s="125"/>
       <c r="K1" s="100" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="12.95" customHeight="1">
-      <c r="A2" s="118"/>
-      <c r="B2" s="118"/>
-      <c r="C2" s="118"/>
-      <c r="D2" s="117" t="s">
+      <c r="A2" s="121"/>
+      <c r="B2" s="121"/>
+      <c r="C2" s="121"/>
+      <c r="D2" s="120" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="117" t="s">
+      <c r="E2" s="120" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="117" t="s">
+      <c r="F2" s="120" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="117" t="s">
+      <c r="G2" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="117" t="s">
+      <c r="H2" s="120" t="s">
         <v>9</v>
       </c>
       <c r="J2" s="100" t="s">
@@ -1897,14 +1897,14 @@
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="118"/>
-      <c r="B3" s="118"/>
-      <c r="C3" s="118"/>
-      <c r="D3" s="118"/>
-      <c r="E3" s="118"/>
-      <c r="F3" s="118"/>
-      <c r="G3" s="118"/>
-      <c r="H3" s="118"/>
+      <c r="A3" s="121"/>
+      <c r="B3" s="121"/>
+      <c r="C3" s="121"/>
+      <c r="D3" s="121"/>
+      <c r="E3" s="121"/>
+      <c r="F3" s="121"/>
+      <c r="G3" s="121"/>
+      <c r="H3" s="121"/>
       <c r="J3" s="100" t="s">
         <v>12</v>
       </c>
@@ -1916,14 +1916,14 @@
       </c>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="118"/>
-      <c r="B4" s="118"/>
-      <c r="C4" s="118"/>
-      <c r="D4" s="118"/>
-      <c r="E4" s="118"/>
-      <c r="F4" s="118"/>
-      <c r="G4" s="118"/>
-      <c r="H4" s="118"/>
+      <c r="A4" s="121"/>
+      <c r="B4" s="121"/>
+      <c r="C4" s="121"/>
+      <c r="D4" s="121"/>
+      <c r="E4" s="121"/>
+      <c r="F4" s="121"/>
+      <c r="G4" s="121"/>
+      <c r="H4" s="121"/>
       <c r="J4" s="100" t="s">
         <v>14</v>
       </c>
@@ -1935,14 +1935,14 @@
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="118"/>
-      <c r="B5" s="118"/>
-      <c r="C5" s="118"/>
-      <c r="D5" s="118"/>
-      <c r="E5" s="118"/>
-      <c r="F5" s="118"/>
-      <c r="G5" s="118"/>
-      <c r="H5" s="118"/>
+      <c r="A5" s="121"/>
+      <c r="B5" s="121"/>
+      <c r="C5" s="121"/>
+      <c r="D5" s="121"/>
+      <c r="E5" s="121"/>
+      <c r="F5" s="121"/>
+      <c r="G5" s="121"/>
+      <c r="H5" s="121"/>
       <c r="J5" s="100" t="s">
         <v>16</v>
       </c>
@@ -1954,14 +1954,14 @@
       </c>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="119"/>
-      <c r="B6" s="119"/>
-      <c r="C6" s="119"/>
-      <c r="D6" s="119"/>
-      <c r="E6" s="119"/>
-      <c r="F6" s="119"/>
-      <c r="G6" s="119"/>
-      <c r="H6" s="119"/>
+      <c r="A6" s="122"/>
+      <c r="B6" s="122"/>
+      <c r="C6" s="122"/>
+      <c r="D6" s="122"/>
+      <c r="E6" s="122"/>
+      <c r="F6" s="122"/>
+      <c r="G6" s="122"/>
+      <c r="H6" s="122"/>
       <c r="J6" s="100" t="s">
         <v>18</v>
       </c>
@@ -3821,10 +3821,10 @@
   </sheetPr>
   <dimension ref="A1:AK177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="AE13" sqref="AE13"/>
-      <selection pane="bottomLeft" activeCell="I21" sqref="I21"/>
+      <selection pane="bottomLeft" activeCell="Z9" sqref="Z9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
@@ -3884,256 +3884,256 @@
       <c r="Y1" s="15"/>
       <c r="Z1" s="15"/>
       <c r="AA1" s="15"/>
-      <c r="AC1" s="125" t="s">
+      <c r="AC1" s="142" t="s">
         <v>30</v>
       </c>
-      <c r="AD1" s="126"/>
-      <c r="AE1" s="126"/>
-      <c r="AF1" s="127"/>
+      <c r="AD1" s="138"/>
+      <c r="AE1" s="138"/>
+      <c r="AF1" s="139"/>
     </row>
     <row r="2" spans="1:32" ht="12.4" customHeight="1">
-      <c r="A2" s="120" t="s">
+      <c r="A2" s="123" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="124" t="s">
+      <c r="B2" s="127" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="123" t="s">
+      <c r="C2" s="126" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="138"/>
-      <c r="E2" s="128"/>
-      <c r="F2" s="139"/>
-      <c r="G2" s="123" t="s">
+      <c r="D2" s="145"/>
+      <c r="E2" s="143"/>
+      <c r="F2" s="128"/>
+      <c r="G2" s="126" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="140" t="s">
+      <c r="H2" s="130" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="142" t="s">
+      <c r="I2" s="141" t="s">
         <v>32</v>
       </c>
       <c r="J2" s="137" t="s">
         <v>33</v>
       </c>
-      <c r="K2" s="126"/>
-      <c r="L2" s="126"/>
-      <c r="M2" s="126"/>
-      <c r="N2" s="126"/>
-      <c r="O2" s="126"/>
-      <c r="P2" s="126"/>
-      <c r="Q2" s="126"/>
-      <c r="R2" s="126"/>
-      <c r="S2" s="126"/>
-      <c r="T2" s="126"/>
-      <c r="U2" s="126"/>
-      <c r="V2" s="126"/>
-      <c r="W2" s="126"/>
-      <c r="X2" s="126"/>
-      <c r="Y2" s="126"/>
-      <c r="Z2" s="127"/>
-      <c r="AA2" s="117" t="s">
+      <c r="K2" s="138"/>
+      <c r="L2" s="138"/>
+      <c r="M2" s="138"/>
+      <c r="N2" s="138"/>
+      <c r="O2" s="138"/>
+      <c r="P2" s="138"/>
+      <c r="Q2" s="138"/>
+      <c r="R2" s="138"/>
+      <c r="S2" s="138"/>
+      <c r="T2" s="138"/>
+      <c r="U2" s="138"/>
+      <c r="V2" s="138"/>
+      <c r="W2" s="138"/>
+      <c r="X2" s="138"/>
+      <c r="Y2" s="138"/>
+      <c r="Z2" s="139"/>
+      <c r="AA2" s="120" t="s">
         <v>34</v>
       </c>
-      <c r="AC2" s="123" t="s">
+      <c r="AC2" s="126" t="s">
         <v>35</v>
       </c>
-      <c r="AD2" s="123" t="s">
+      <c r="AD2" s="126" t="s">
         <v>36</v>
       </c>
-      <c r="AE2" s="123" t="s">
+      <c r="AE2" s="126" t="s">
         <v>37</v>
       </c>
-      <c r="AF2" s="123" t="s">
+      <c r="AF2" s="126" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:32" ht="12.6" customHeight="1">
-      <c r="A3" s="118"/>
-      <c r="B3" s="118"/>
-      <c r="C3" s="118"/>
+      <c r="A3" s="121"/>
+      <c r="B3" s="121"/>
+      <c r="C3" s="121"/>
       <c r="D3" s="131"/>
-      <c r="E3" s="129"/>
-      <c r="F3" s="132"/>
-      <c r="G3" s="118"/>
+      <c r="E3" s="135"/>
+      <c r="F3" s="129"/>
+      <c r="G3" s="121"/>
       <c r="H3" s="131"/>
-      <c r="I3" s="118"/>
-      <c r="J3" s="141" t="s">
+      <c r="I3" s="121"/>
+      <c r="J3" s="140" t="s">
         <v>39</v>
       </c>
-      <c r="K3" s="136"/>
-      <c r="L3" s="130"/>
-      <c r="M3" s="135" t="s">
+      <c r="K3" s="133"/>
+      <c r="L3" s="134"/>
+      <c r="M3" s="144" t="s">
+        <v>176</v>
+      </c>
+      <c r="N3" s="133"/>
+      <c r="O3" s="134"/>
+      <c r="P3" s="126" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q3" s="133"/>
+      <c r="R3" s="134"/>
+      <c r="S3" s="120" t="s">
+        <v>41</v>
+      </c>
+      <c r="T3" s="133"/>
+      <c r="U3" s="134"/>
+      <c r="V3" s="120" t="s">
+        <v>42</v>
+      </c>
+      <c r="W3" s="120" t="s">
+        <v>43</v>
+      </c>
+      <c r="X3" s="134"/>
+      <c r="Y3" s="120" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z3" s="120" t="s">
         <v>177</v>
       </c>
-      <c r="N3" s="136"/>
-      <c r="O3" s="130"/>
-      <c r="P3" s="123" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q3" s="136"/>
-      <c r="R3" s="130"/>
-      <c r="S3" s="117" t="s">
-        <v>41</v>
-      </c>
-      <c r="T3" s="136"/>
-      <c r="U3" s="130"/>
-      <c r="V3" s="117" t="s">
-        <v>42</v>
-      </c>
-      <c r="W3" s="117" t="s">
-        <v>43</v>
-      </c>
-      <c r="X3" s="130"/>
-      <c r="Y3" s="117" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z3" s="117" t="s">
+      <c r="AA3" s="121"/>
+      <c r="AC3" s="121"/>
+      <c r="AD3" s="121"/>
+      <c r="AE3" s="121"/>
+      <c r="AF3" s="121"/>
+    </row>
+    <row r="4" spans="1:32" ht="12.6" customHeight="1">
+      <c r="A4" s="121"/>
+      <c r="B4" s="121"/>
+      <c r="C4" s="121"/>
+      <c r="D4" s="131"/>
+      <c r="E4" s="135"/>
+      <c r="F4" s="129"/>
+      <c r="G4" s="121"/>
+      <c r="H4" s="131"/>
+      <c r="I4" s="121"/>
+      <c r="J4" s="131"/>
+      <c r="K4" s="135"/>
+      <c r="L4" s="129"/>
+      <c r="M4" s="131"/>
+      <c r="N4" s="135"/>
+      <c r="O4" s="129"/>
+      <c r="P4" s="131"/>
+      <c r="Q4" s="135"/>
+      <c r="R4" s="129"/>
+      <c r="S4" s="131"/>
+      <c r="T4" s="135"/>
+      <c r="U4" s="129"/>
+      <c r="V4" s="121"/>
+      <c r="W4" s="131"/>
+      <c r="X4" s="129"/>
+      <c r="Y4" s="121"/>
+      <c r="Z4" s="121"/>
+      <c r="AA4" s="121"/>
+      <c r="AC4" s="121"/>
+      <c r="AD4" s="121"/>
+      <c r="AE4" s="121"/>
+      <c r="AF4" s="121"/>
+    </row>
+    <row r="5" spans="1:32" ht="25.15" customHeight="1">
+      <c r="A5" s="121"/>
+      <c r="B5" s="121"/>
+      <c r="C5" s="121"/>
+      <c r="D5" s="131"/>
+      <c r="E5" s="135"/>
+      <c r="F5" s="129"/>
+      <c r="G5" s="121"/>
+      <c r="H5" s="131"/>
+      <c r="I5" s="121"/>
+      <c r="J5" s="131"/>
+      <c r="K5" s="135"/>
+      <c r="L5" s="129"/>
+      <c r="M5" s="131"/>
+      <c r="N5" s="135"/>
+      <c r="O5" s="129"/>
+      <c r="P5" s="131"/>
+      <c r="Q5" s="135"/>
+      <c r="R5" s="129"/>
+      <c r="S5" s="131"/>
+      <c r="T5" s="135"/>
+      <c r="U5" s="129"/>
+      <c r="V5" s="121"/>
+      <c r="W5" s="131"/>
+      <c r="X5" s="129"/>
+      <c r="Y5" s="121"/>
+      <c r="Z5" s="121"/>
+      <c r="AA5" s="121"/>
+      <c r="AC5" s="121"/>
+      <c r="AD5" s="121"/>
+      <c r="AE5" s="121"/>
+      <c r="AF5" s="121"/>
+    </row>
+    <row r="6" spans="1:32" ht="12.6" customHeight="1">
+      <c r="A6" s="121"/>
+      <c r="B6" s="121"/>
+      <c r="C6" s="121"/>
+      <c r="D6" s="131"/>
+      <c r="E6" s="135"/>
+      <c r="F6" s="129"/>
+      <c r="G6" s="121"/>
+      <c r="H6" s="131"/>
+      <c r="I6" s="121"/>
+      <c r="J6" s="132"/>
+      <c r="K6" s="125"/>
+      <c r="L6" s="136"/>
+      <c r="M6" s="132"/>
+      <c r="N6" s="125"/>
+      <c r="O6" s="136"/>
+      <c r="P6" s="131"/>
+      <c r="Q6" s="135"/>
+      <c r="R6" s="129"/>
+      <c r="S6" s="132"/>
+      <c r="T6" s="125"/>
+      <c r="U6" s="136"/>
+      <c r="V6" s="121"/>
+      <c r="W6" s="131"/>
+      <c r="X6" s="129"/>
+      <c r="Y6" s="121"/>
+      <c r="Z6" s="121"/>
+      <c r="AA6" s="121"/>
+      <c r="AC6" s="121"/>
+      <c r="AD6" s="121"/>
+      <c r="AE6" s="121"/>
+      <c r="AF6" s="121"/>
+    </row>
+    <row r="7" spans="1:32">
+      <c r="A7" s="122"/>
+      <c r="B7" s="122"/>
+      <c r="C7" s="122"/>
+      <c r="D7" s="131"/>
+      <c r="E7" s="135"/>
+      <c r="F7" s="129"/>
+      <c r="G7" s="122"/>
+      <c r="H7" s="132"/>
+      <c r="I7" s="122"/>
+      <c r="J7" s="137" t="s">
         <v>45</v>
       </c>
-      <c r="AA3" s="118"/>
-      <c r="AC3" s="118"/>
-      <c r="AD3" s="118"/>
-      <c r="AE3" s="118"/>
-      <c r="AF3" s="118"/>
-    </row>
-    <row r="4" spans="1:32" ht="12.6" customHeight="1">
-      <c r="A4" s="118"/>
-      <c r="B4" s="118"/>
-      <c r="C4" s="118"/>
-      <c r="D4" s="131"/>
-      <c r="E4" s="129"/>
-      <c r="F4" s="132"/>
-      <c r="G4" s="118"/>
-      <c r="H4" s="131"/>
-      <c r="I4" s="118"/>
-      <c r="J4" s="131"/>
-      <c r="K4" s="129"/>
-      <c r="L4" s="132"/>
-      <c r="M4" s="131"/>
-      <c r="N4" s="129"/>
-      <c r="O4" s="132"/>
-      <c r="P4" s="131"/>
-      <c r="Q4" s="129"/>
-      <c r="R4" s="132"/>
-      <c r="S4" s="131"/>
-      <c r="T4" s="129"/>
-      <c r="U4" s="132"/>
-      <c r="V4" s="118"/>
-      <c r="W4" s="131"/>
-      <c r="X4" s="132"/>
-      <c r="Y4" s="118"/>
-      <c r="Z4" s="118"/>
-      <c r="AA4" s="118"/>
-      <c r="AC4" s="118"/>
-      <c r="AD4" s="118"/>
-      <c r="AE4" s="118"/>
-      <c r="AF4" s="118"/>
-    </row>
-    <row r="5" spans="1:32" ht="25.15" customHeight="1">
-      <c r="A5" s="118"/>
-      <c r="B5" s="118"/>
-      <c r="C5" s="118"/>
-      <c r="D5" s="131"/>
-      <c r="E5" s="129"/>
-      <c r="F5" s="132"/>
-      <c r="G5" s="118"/>
-      <c r="H5" s="131"/>
-      <c r="I5" s="118"/>
-      <c r="J5" s="131"/>
-      <c r="K5" s="129"/>
-      <c r="L5" s="132"/>
-      <c r="M5" s="131"/>
-      <c r="N5" s="129"/>
-      <c r="O5" s="132"/>
-      <c r="P5" s="131"/>
-      <c r="Q5" s="129"/>
-      <c r="R5" s="132"/>
-      <c r="S5" s="131"/>
-      <c r="T5" s="129"/>
-      <c r="U5" s="132"/>
-      <c r="V5" s="118"/>
-      <c r="W5" s="131"/>
-      <c r="X5" s="132"/>
-      <c r="Y5" s="118"/>
-      <c r="Z5" s="118"/>
-      <c r="AA5" s="118"/>
-      <c r="AC5" s="118"/>
-      <c r="AD5" s="118"/>
-      <c r="AE5" s="118"/>
-      <c r="AF5" s="118"/>
-    </row>
-    <row r="6" spans="1:32" ht="12.6" customHeight="1">
-      <c r="A6" s="118"/>
-      <c r="B6" s="118"/>
-      <c r="C6" s="118"/>
-      <c r="D6" s="131"/>
-      <c r="E6" s="129"/>
-      <c r="F6" s="132"/>
-      <c r="G6" s="118"/>
-      <c r="H6" s="131"/>
-      <c r="I6" s="118"/>
-      <c r="J6" s="133"/>
-      <c r="K6" s="122"/>
-      <c r="L6" s="134"/>
-      <c r="M6" s="133"/>
-      <c r="N6" s="122"/>
-      <c r="O6" s="134"/>
-      <c r="P6" s="131"/>
-      <c r="Q6" s="129"/>
-      <c r="R6" s="132"/>
-      <c r="S6" s="133"/>
-      <c r="T6" s="122"/>
-      <c r="U6" s="134"/>
-      <c r="V6" s="118"/>
-      <c r="W6" s="131"/>
-      <c r="X6" s="132"/>
-      <c r="Y6" s="118"/>
-      <c r="Z6" s="118"/>
-      <c r="AA6" s="118"/>
-      <c r="AC6" s="118"/>
-      <c r="AD6" s="118"/>
-      <c r="AE6" s="118"/>
-      <c r="AF6" s="118"/>
-    </row>
-    <row r="7" spans="1:32">
-      <c r="A7" s="119"/>
-      <c r="B7" s="119"/>
-      <c r="C7" s="119"/>
-      <c r="D7" s="131"/>
-      <c r="E7" s="129"/>
-      <c r="F7" s="132"/>
-      <c r="G7" s="119"/>
-      <c r="H7" s="133"/>
-      <c r="I7" s="119"/>
-      <c r="J7" s="137" t="s">
+      <c r="K7" s="138"/>
+      <c r="L7" s="139"/>
+      <c r="M7" s="137" t="s">
         <v>46</v>
       </c>
-      <c r="K7" s="126"/>
-      <c r="L7" s="127"/>
-      <c r="M7" s="137" t="s">
+      <c r="N7" s="138"/>
+      <c r="O7" s="139"/>
+      <c r="P7" s="132"/>
+      <c r="Q7" s="125"/>
+      <c r="R7" s="136"/>
+      <c r="S7" s="137" t="s">
         <v>47</v>
       </c>
-      <c r="N7" s="126"/>
-      <c r="O7" s="127"/>
-      <c r="P7" s="133"/>
-      <c r="Q7" s="122"/>
-      <c r="R7" s="134"/>
-      <c r="S7" s="137" t="s">
-        <v>48</v>
-      </c>
-      <c r="T7" s="126"/>
-      <c r="U7" s="127"/>
-      <c r="V7" s="119"/>
-      <c r="W7" s="133"/>
-      <c r="X7" s="134"/>
-      <c r="Y7" s="119"/>
-      <c r="Z7" s="119"/>
-      <c r="AA7" s="119"/>
-      <c r="AC7" s="119"/>
-      <c r="AD7" s="119"/>
-      <c r="AE7" s="119"/>
-      <c r="AF7" s="119"/>
+      <c r="T7" s="138"/>
+      <c r="U7" s="139"/>
+      <c r="V7" s="122"/>
+      <c r="W7" s="132"/>
+      <c r="X7" s="136"/>
+      <c r="Y7" s="122"/>
+      <c r="Z7" s="122"/>
+      <c r="AA7" s="122"/>
+      <c r="AC7" s="122"/>
+      <c r="AD7" s="122"/>
+      <c r="AE7" s="122"/>
+      <c r="AF7" s="122"/>
     </row>
     <row r="8" spans="1:32">
       <c r="A8" s="108">
@@ -4148,7 +4148,7 @@
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="56" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F8" s="15"/>
       <c r="G8" s="18" t="str">
@@ -4156,7 +4156,7 @@
         <v>1:STA1</v>
       </c>
       <c r="H8" s="40" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I8" s="96">
         <v>1</v>
@@ -4183,7 +4183,7 @@
       <c r="AD8" s="60"/>
       <c r="AE8" s="60"/>
       <c r="AF8" s="60" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:32">
@@ -4195,7 +4195,7 @@
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="56" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F9" s="15"/>
       <c r="G9" s="19" t="str">
@@ -4204,7 +4204,7 @@
       </c>
       <c r="H9" s="40"/>
       <c r="I9" s="96" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J9" s="77">
         <v>0</v>
@@ -4244,7 +4244,7 @@
       </c>
       <c r="V9" s="80"/>
       <c r="W9" s="81" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="X9" s="72"/>
       <c r="Y9" s="15">
@@ -4256,7 +4256,7 @@
       <c r="AD9" s="61"/>
       <c r="AE9" s="61"/>
       <c r="AF9" s="61" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:32">
@@ -4275,7 +4275,7 @@
       </c>
       <c r="H10" s="40"/>
       <c r="I10" s="96" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J10" s="77">
         <v>0</v>
@@ -4315,7 +4315,7 @@
       </c>
       <c r="V10" s="80"/>
       <c r="W10" s="81" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="X10" s="72"/>
       <c r="Y10" s="15">
@@ -4327,7 +4327,7 @@
       <c r="AD10" s="61"/>
       <c r="AE10" s="61"/>
       <c r="AF10" s="61" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:32">
@@ -4339,7 +4339,7 @@
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="56" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F11" s="15"/>
       <c r="G11" s="19" t="str">
@@ -4348,7 +4348,7 @@
       </c>
       <c r="H11" s="40"/>
       <c r="I11" s="96" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J11" s="77">
         <v>0</v>
@@ -4388,7 +4388,7 @@
       </c>
       <c r="V11" s="80"/>
       <c r="W11" s="81" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="X11" s="72"/>
       <c r="Y11" s="15">
@@ -4400,7 +4400,7 @@
       <c r="AD11" s="61"/>
       <c r="AE11" s="61"/>
       <c r="AF11" s="61" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:32">
@@ -4412,7 +4412,7 @@
       </c>
       <c r="D12" s="15"/>
       <c r="E12" s="56" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F12" s="15"/>
       <c r="G12" s="19" t="str">
@@ -4421,7 +4421,7 @@
       </c>
       <c r="H12" s="40"/>
       <c r="I12" s="97" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J12" s="77">
         <v>0</v>
@@ -4461,7 +4461,7 @@
       </c>
       <c r="V12" s="61"/>
       <c r="W12" s="81" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="X12" s="72"/>
       <c r="Y12" s="15">
@@ -4483,7 +4483,7 @@
       </c>
       <c r="D13" s="15"/>
       <c r="E13" s="56" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F13" s="15"/>
       <c r="G13" s="19" t="str">
@@ -4524,7 +4524,7 @@
       </c>
       <c r="D14" s="15"/>
       <c r="E14" s="56" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F14" s="15"/>
       <c r="G14" s="19" t="str">
@@ -4643,7 +4643,7 @@
       </c>
       <c r="D17" s="15"/>
       <c r="E17" s="56" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F17" s="15"/>
       <c r="G17" s="19" t="str">
@@ -4762,7 +4762,7 @@
       </c>
       <c r="D20" s="15"/>
       <c r="E20" s="56" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F20" s="15"/>
       <c r="G20" s="19" t="str">
@@ -4881,7 +4881,7 @@
       </c>
       <c r="D23" s="15"/>
       <c r="E23" s="56" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F23" s="15"/>
       <c r="G23" s="19" t="str">
@@ -5000,7 +5000,7 @@
       </c>
       <c r="D26" s="15"/>
       <c r="E26" s="56" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F26" s="15"/>
       <c r="G26" s="19" t="str">
@@ -5119,7 +5119,7 @@
       </c>
       <c r="D29" s="15"/>
       <c r="E29" s="56" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F29" s="15"/>
       <c r="G29" s="19" t="str">
@@ -5238,7 +5238,7 @@
       </c>
       <c r="D32" s="15"/>
       <c r="E32" s="56" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F32" s="15"/>
       <c r="G32" s="19" t="str">
@@ -5357,7 +5357,7 @@
       </c>
       <c r="D35" s="15"/>
       <c r="E35" s="56" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F35" s="15"/>
       <c r="G35" s="19" t="str">
@@ -10929,17 +10929,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="F2:F7"/>
-    <mergeCell ref="H2:H7"/>
-    <mergeCell ref="Y3:Y7"/>
-    <mergeCell ref="S3:U6"/>
-    <mergeCell ref="P3:R7"/>
-    <mergeCell ref="S7:U7"/>
-    <mergeCell ref="M7:O7"/>
-    <mergeCell ref="J3:L6"/>
-    <mergeCell ref="G2:G7"/>
-    <mergeCell ref="I2:I7"/>
-    <mergeCell ref="J7:L7"/>
     <mergeCell ref="AC1:AF1"/>
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="C2:C7"/>
@@ -10956,6 +10945,17 @@
     <mergeCell ref="B2:B7"/>
     <mergeCell ref="AE2:AE7"/>
     <mergeCell ref="D2:D7"/>
+    <mergeCell ref="F2:F7"/>
+    <mergeCell ref="H2:H7"/>
+    <mergeCell ref="Y3:Y7"/>
+    <mergeCell ref="S3:U6"/>
+    <mergeCell ref="P3:R7"/>
+    <mergeCell ref="S7:U7"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="J3:L6"/>
+    <mergeCell ref="G2:G7"/>
+    <mergeCell ref="I2:I7"/>
+    <mergeCell ref="J7:L7"/>
   </mergeCells>
   <conditionalFormatting sqref="I1:I1048576">
     <cfRule type="expression" dxfId="28" priority="41">
@@ -11057,7 +11057,7 @@
       <formula>$H8 &lt;&gt; "(FE) uniform"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" xWindow="1747" yWindow="323" count="25">
+  <dataValidations xWindow="1747" yWindow="323" count="25">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="(FOR TRAPEZOIDAL LOADS ONLY)_x000a_PX1 - Enter your starting load in the X direction (kN/m)_x000a__x000a_PY1 - Enter your starting load in the Y direction (kN/m)_x000a__x000a_PZ1 - Enter your starting load in the Z direction (kN/m)" sqref="M7:O7" xr:uid="{00000000-0002-0000-0100-000000000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="(FOR TRAPEZOIDAL LOADS ONLY)_x000a_x2 - Absolute or relative distance of end of load along a member (m or m/L)_x000a__x000a_x1 - Absolute or relative distance of start of load along a member (m or m/L)" sqref="S7:U7" xr:uid="{00000000-0002-0000-0100-000001000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="(FOR TRAPEZOIDAL LOADS ONLY)_x000a_PX2 - Enter your finishing load in the X direction (kN/m)_x000a__x000a_PY2 - Enter your finishing load in the Y direction (kN/m)_x000a__x000a_PZ2 - Enter your finishing load in the Z direction (kN/m)" sqref="J7:L7" xr:uid="{00000000-0002-0000-0100-000002000000}"/>
@@ -11088,7 +11088,7 @@
       <formula2>150</formula2>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="1-Projected, 0- Not projected_x000a_" sqref="Y3:Y7" xr:uid="{00000000-0002-0000-0100-000016000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="1, 0 - For load on contour auto detect panels_x000a_" sqref="Z3:Z7" xr:uid="{00000000-0002-0000-0100-000017000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Contour identification index_x000a_" sqref="Z3:Z7" xr:uid="{00000000-0002-0000-0100-000017000000}"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H8:H177" xr:uid="{69C6861F-E4DE-4C73-AD67-80357667F890}">
       <formula1>"(FE) uniform, nodal force, member force, self-weight, trapezoidal load (2p), uniform load, (FE) linear load on edges, load on contour, load 3p on contour"</formula1>
     </dataValidation>
@@ -11500,17 +11500,17 @@
     </row>
     <row r="3" spans="1:4605" s="7" customFormat="1" ht="218.65" customHeight="1">
       <c r="A3" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="53" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="69" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F3" s="69" t="s">
         <v>7</v>
@@ -16123,12 +16123,12 @@
       <c r="A4" s="3"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
-      <c r="D4" s="143" t="s">
+      <c r="D4" s="146" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="136"/>
-      <c r="F4" s="136"/>
-      <c r="G4" s="136"/>
+      <c r="E4" s="133"/>
+      <c r="F4" s="133"/>
+      <c r="G4" s="133"/>
       <c r="H4" s="84">
         <v>1</v>
       </c>
@@ -20735,9 +20735,9 @@
       <c r="B5" s="21"/>
       <c r="C5" s="21"/>
       <c r="D5" s="131"/>
-      <c r="E5" s="144"/>
-      <c r="F5" s="144"/>
-      <c r="G5" s="144"/>
+      <c r="E5" s="147"/>
+      <c r="F5" s="147"/>
+      <c r="G5" s="147"/>
       <c r="H5" s="84"/>
       <c r="I5" s="84"/>
       <c r="J5" s="84"/>
@@ -21108,19 +21108,19 @@
       <c r="NK5" s="50"/>
     </row>
     <row r="6" spans="1:4605" s="4" customFormat="1" ht="15.6" customHeight="1">
-      <c r="A6" s="147" t="s">
+      <c r="A6" s="119" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="119" t="s">
         <v>58</v>
       </c>
-      <c r="B6" s="147" t="s">
+      <c r="C6" s="119" t="s">
         <v>59</v>
       </c>
-      <c r="C6" s="147" t="s">
-        <v>60</v>
-      </c>
-      <c r="D6" s="145"/>
-      <c r="E6" s="146"/>
-      <c r="F6" s="146"/>
-      <c r="G6" s="146"/>
+      <c r="D6" s="117"/>
+      <c r="E6" s="118"/>
+      <c r="F6" s="118"/>
+      <c r="G6" s="118"/>
       <c r="H6" s="84"/>
       <c r="I6" s="84"/>
       <c r="J6" s="84"/>
@@ -31997,81 +31997,81 @@
   <sheetData>
     <row r="1" spans="1:23">
       <c r="A1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" t="s">
         <v>61</v>
       </c>
-      <c r="B1" t="s">
+      <c r="G1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" t="s">
         <v>62</v>
       </c>
-      <c r="G1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="M1" t="s">
+        <v>60</v>
+      </c>
+      <c r="N1" t="s">
         <v>63</v>
       </c>
-      <c r="M1" t="s">
-        <v>61</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="S1" t="s">
+        <v>60</v>
+      </c>
+      <c r="T1" t="s">
         <v>64</v>
-      </c>
-      <c r="S1" t="s">
-        <v>61</v>
-      </c>
-      <c r="T1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:23">
       <c r="A2" s="100" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="100" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="100" t="s">
+      <c r="C2" s="100" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="100" t="s">
+      <c r="D2" t="s">
         <v>68</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J2" t="s">
+        <v>68</v>
+      </c>
+      <c r="M2" t="s">
+        <v>65</v>
+      </c>
+      <c r="N2" t="s">
+        <v>66</v>
+      </c>
+      <c r="O2" t="s">
+        <v>67</v>
+      </c>
+      <c r="P2" t="s">
+        <v>68</v>
+      </c>
+      <c r="S2" t="s">
+        <v>65</v>
+      </c>
+      <c r="T2" t="s">
+        <v>66</v>
+      </c>
+      <c r="U2" t="s">
+        <v>67</v>
+      </c>
+      <c r="V2" t="s">
+        <v>68</v>
+      </c>
+      <c r="W2" t="s">
         <v>69</v>
-      </c>
-      <c r="G2" t="s">
-        <v>66</v>
-      </c>
-      <c r="H2" t="s">
-        <v>67</v>
-      </c>
-      <c r="I2" t="s">
-        <v>68</v>
-      </c>
-      <c r="J2" t="s">
-        <v>69</v>
-      </c>
-      <c r="M2" t="s">
-        <v>66</v>
-      </c>
-      <c r="N2" t="s">
-        <v>67</v>
-      </c>
-      <c r="O2" t="s">
-        <v>68</v>
-      </c>
-      <c r="P2" t="s">
-        <v>69</v>
-      </c>
-      <c r="S2" t="s">
-        <v>66</v>
-      </c>
-      <c r="T2" t="s">
-        <v>67</v>
-      </c>
-      <c r="U2" t="s">
-        <v>68</v>
-      </c>
-      <c r="V2" t="s">
-        <v>69</v>
-      </c>
-      <c r="W2" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:23">
@@ -32124,7 +32124,7 @@
         <v>0</v>
       </c>
       <c r="W3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:23">
@@ -32177,7 +32177,7 @@
         <v>0</v>
       </c>
       <c r="W4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:23">
@@ -32230,7 +32230,7 @@
         <v>0</v>
       </c>
       <c r="W5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:23">
@@ -32428,81 +32428,81 @@
   <sheetData>
     <row r="1" spans="1:23">
       <c r="A1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" t="s">
         <v>61</v>
       </c>
-      <c r="B1" t="s">
+      <c r="G1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" t="s">
         <v>62</v>
       </c>
-      <c r="G1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="M1" t="s">
+        <v>60</v>
+      </c>
+      <c r="N1" t="s">
         <v>63</v>
       </c>
-      <c r="M1" t="s">
-        <v>61</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="S1" t="s">
+        <v>60</v>
+      </c>
+      <c r="T1" t="s">
         <v>64</v>
-      </c>
-      <c r="S1" t="s">
-        <v>61</v>
-      </c>
-      <c r="T1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:23">
       <c r="A2" s="100" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="100" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="100" t="s">
+      <c r="C2" s="100" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="100" t="s">
+      <c r="D2" t="s">
         <v>68</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J2" t="s">
+        <v>68</v>
+      </c>
+      <c r="M2" t="s">
+        <v>65</v>
+      </c>
+      <c r="N2" t="s">
+        <v>66</v>
+      </c>
+      <c r="O2" t="s">
+        <v>67</v>
+      </c>
+      <c r="P2" t="s">
+        <v>68</v>
+      </c>
+      <c r="S2" t="s">
+        <v>65</v>
+      </c>
+      <c r="T2" t="s">
+        <v>66</v>
+      </c>
+      <c r="U2" t="s">
+        <v>67</v>
+      </c>
+      <c r="V2" t="s">
+        <v>68</v>
+      </c>
+      <c r="W2" t="s">
         <v>69</v>
-      </c>
-      <c r="G2" t="s">
-        <v>66</v>
-      </c>
-      <c r="H2" t="s">
-        <v>67</v>
-      </c>
-      <c r="I2" t="s">
-        <v>68</v>
-      </c>
-      <c r="J2" t="s">
-        <v>69</v>
-      </c>
-      <c r="M2" t="s">
-        <v>66</v>
-      </c>
-      <c r="N2" t="s">
-        <v>67</v>
-      </c>
-      <c r="O2" t="s">
-        <v>68</v>
-      </c>
-      <c r="P2" t="s">
-        <v>69</v>
-      </c>
-      <c r="S2" t="s">
-        <v>66</v>
-      </c>
-      <c r="T2" t="s">
-        <v>67</v>
-      </c>
-      <c r="U2" t="s">
-        <v>68</v>
-      </c>
-      <c r="V2" t="s">
-        <v>69</v>
-      </c>
-      <c r="W2" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:23">
@@ -32555,7 +32555,7 @@
         <v>0</v>
       </c>
       <c r="W3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:23">
@@ -32608,7 +32608,7 @@
         <v>0</v>
       </c>
       <c r="W4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:23">
@@ -32661,7 +32661,7 @@
         <v>0</v>
       </c>
       <c r="W5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:23">
@@ -32880,7 +32880,7 @@
   <sheetData>
     <row r="1" spans="1:20" ht="13.5" customHeight="1" thickBot="1">
       <c r="A1" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F1" s="24">
         <v>0.5</v>
@@ -32889,77 +32889,77 @@
         <v>0.1</v>
       </c>
       <c r="M1" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="S1" s="17" t="s">
         <v>75</v>
-      </c>
-      <c r="S1" s="17" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="15.75" customHeight="1">
       <c r="A2" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="C2" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="D2" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="E2" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="F2" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="G2" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="H2" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="J2" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="J2" s="17" t="s">
+      <c r="K2" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="K2" s="17" t="s">
+      <c r="M2" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="M2" s="17" t="s">
-        <v>87</v>
-      </c>
       <c r="N2" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O2" s="17">
         <v>1</v>
       </c>
       <c r="P2" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="S2" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="S2" s="17" t="s">
+      <c r="T2" s="17" t="s">
         <v>89</v>
-      </c>
-      <c r="T2" s="17" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="39" customHeight="1">
       <c r="A3" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="C3" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="C3" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="D3" s="17" t="s">
+      <c r="E3" s="17" t="s">
         <v>93</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>94</v>
       </c>
       <c r="F3" s="25" t="e">
         <f>PlatformName &amp;" member utilisations $&gt;" &amp;F1&amp;"$"</f>
@@ -32974,107 +32974,107 @@
         <v>#REF!</v>
       </c>
       <c r="J3" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="K3" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="K3" s="25" t="s">
+      <c r="M3" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="M3" s="17" t="s">
-        <v>97</v>
-      </c>
       <c r="N3" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O3" s="17">
         <v>1</v>
       </c>
       <c r="P3" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="S3" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="T3" s="26" t="s">
         <v>98</v>
-      </c>
-      <c r="T3" s="26" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="15.75" customHeight="1">
       <c r="A4" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="C4" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="H4" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="C4" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="F4" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="G4" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="H4" s="25" t="s">
+      <c r="M4" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="M4" s="17" t="s">
-        <v>103</v>
-      </c>
       <c r="N4" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O4" s="17">
         <v>1</v>
       </c>
       <c r="P4" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="S4" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="15.75" customHeight="1">
       <c r="B5" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="H5" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="C5" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="F5" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="G5" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="H5" s="25" t="s">
+      <c r="M5" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="M5" s="17" t="s">
-        <v>107</v>
-      </c>
       <c r="N5" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O5" s="17">
         <v>1</v>
       </c>
       <c r="P5" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="S5" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="15.75" customHeight="1">
@@ -33103,19 +33103,19 @@
         <v>#REF!</v>
       </c>
       <c r="H6" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="M6" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="M6" s="17" t="s">
-        <v>110</v>
-      </c>
       <c r="N6" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O6" s="17">
         <v>1</v>
       </c>
       <c r="P6" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="S6" s="17" t="e">
         <f>"\includegraphics[width=\textwidth]{\"&amp;LaTeXFiguresFolder &amp;"\"&amp;PlatformName&amp; " "&amp;S3&amp;".png} "</f>
@@ -33148,61 +33148,61 @@
         <v>#REF!</v>
       </c>
       <c r="H7" s="25" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J7" s="17">
         <f>COLUMN(J1)</f>
         <v>10</v>
       </c>
       <c r="M7" s="17" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N7" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O7" s="17">
         <v>1</v>
       </c>
       <c r="P7" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="S7" s="17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="15.75" customHeight="1">
       <c r="B8" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="C8" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="D8" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="E8" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="F8" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="G8" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="H8" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="H8" s="25" t="s">
+      <c r="M8" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="M8" s="17" t="s">
-        <v>122</v>
-      </c>
       <c r="N8" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O8" s="17">
         <v>1</v>
       </c>
       <c r="P8" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="S8" s="17" t="e">
         <f>"    \caption{" &amp;PlatformName&amp; " " &amp; S3 &amp;".}"</f>
@@ -33211,37 +33211,37 @@
     </row>
     <row r="9" spans="1:20" ht="15.75" customHeight="1">
       <c r="B9" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="C9" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="D9" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="E9" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="F9" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="G9" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="G9" s="17" t="s">
+      <c r="H9" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="M9" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="H9" s="25" t="s">
-        <v>106</v>
-      </c>
-      <c r="M9" s="17" t="s">
-        <v>129</v>
-      </c>
       <c r="N9" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O9" s="17">
         <v>1</v>
       </c>
       <c r="P9" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="S9" s="17" t="e">
         <f>"    \label{tabl:" &amp; PlatformName &amp;" "&amp;S3 &amp;"}"</f>
@@ -33250,107 +33250,107 @@
     </row>
     <row r="10" spans="1:20" ht="16.5" customHeight="1">
       <c r="B10" s="47" t="s">
+        <v>129</v>
+      </c>
+      <c r="C10" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="D10" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="E10" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="F10" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="F10" s="17" t="s">
+      <c r="G10" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="H10" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="G10" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="H10" s="25" t="s">
+      <c r="M10" s="17" t="s">
         <v>135</v>
       </c>
-      <c r="M10" s="17" t="s">
-        <v>136</v>
-      </c>
       <c r="N10" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O10" s="17">
         <v>1</v>
       </c>
       <c r="P10" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:20" ht="16.5" customHeight="1">
       <c r="B11" s="47" t="s">
+        <v>136</v>
+      </c>
+      <c r="C11" s="47" t="s">
+        <v>136</v>
+      </c>
+      <c r="D11" s="47" t="s">
+        <v>136</v>
+      </c>
+      <c r="E11" s="47" t="s">
+        <v>136</v>
+      </c>
+      <c r="F11" s="47" t="s">
+        <v>136</v>
+      </c>
+      <c r="G11" s="47" t="s">
+        <v>136</v>
+      </c>
+      <c r="H11" s="25" t="s">
         <v>137</v>
       </c>
-      <c r="C11" s="47" t="s">
-        <v>137</v>
-      </c>
-      <c r="D11" s="47" t="s">
-        <v>137</v>
-      </c>
-      <c r="E11" s="47" t="s">
-        <v>137</v>
-      </c>
-      <c r="F11" s="47" t="s">
-        <v>137</v>
-      </c>
-      <c r="G11" s="47" t="s">
-        <v>137</v>
-      </c>
-      <c r="H11" s="25" t="s">
+      <c r="M11" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="M11" s="17" t="s">
-        <v>139</v>
-      </c>
       <c r="N11" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O11" s="17">
         <v>1</v>
       </c>
       <c r="P11" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="15.75" customHeight="1">
       <c r="H12" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="M12" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="M12" s="17" t="s">
-        <v>141</v>
-      </c>
       <c r="N12" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O12" s="17">
         <v>1</v>
       </c>
       <c r="P12" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="16.5" customHeight="1">
       <c r="C13" s="47"/>
       <c r="H13" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="M13" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="M13" s="17" t="s">
-        <v>143</v>
-      </c>
       <c r="N13" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O13" s="17">
         <v>1</v>
       </c>
       <c r="P13" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="16.5" customHeight="1">
@@ -33360,16 +33360,16 @@
         <v>#REF!</v>
       </c>
       <c r="M14" s="17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N14" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O14" s="17">
         <v>1</v>
       </c>
       <c r="P14" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="S14" s="26"/>
     </row>
@@ -33380,49 +33380,49 @@
         <v>#REF!</v>
       </c>
       <c r="M15" s="17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N15" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O15" s="17">
         <v>1</v>
       </c>
       <c r="P15" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="16.5" customHeight="1">
       <c r="C16" s="47"/>
       <c r="H16" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="M16" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="M16" s="17" t="s">
-        <v>147</v>
-      </c>
       <c r="N16" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O16" s="17">
         <v>1</v>
       </c>
       <c r="P16" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="3:16" ht="16.5" customHeight="1">
       <c r="C17" s="47"/>
       <c r="M17" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="N17" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O17" s="17">
         <v>1</v>
       </c>
       <c r="P17" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="3:16" ht="16.5" customHeight="1">
@@ -33486,79 +33486,79 @@
   <sheetData>
     <row r="1" spans="1:25">
       <c r="A1" s="28" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1" s="29" t="s">
         <v>149</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="C1" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="30" t="s">
         <v>150</v>
       </c>
-      <c r="C1" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="D1" s="30" t="s">
+      <c r="E1" s="29" t="s">
         <v>151</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="F1" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="G1" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="H1" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="I1" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="J1" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="K1" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="L1" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="M1" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="N1" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="O1" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="P1" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q1" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="R1" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="S1" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="T1" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="U1" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="V1" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="W1" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="X1" s="33" t="s">
         <v>152</v>
       </c>
-      <c r="F1" s="29" t="s">
-        <v>151</v>
-      </c>
-      <c r="G1" s="29" t="s">
-        <v>152</v>
-      </c>
-      <c r="H1" s="29" t="s">
-        <v>151</v>
-      </c>
-      <c r="I1" s="29" t="s">
-        <v>152</v>
-      </c>
-      <c r="J1" s="29" t="s">
-        <v>151</v>
-      </c>
-      <c r="K1" s="29" t="s">
-        <v>152</v>
-      </c>
-      <c r="L1" s="29" t="s">
-        <v>151</v>
-      </c>
-      <c r="M1" s="29" t="s">
-        <v>152</v>
-      </c>
-      <c r="N1" s="29" t="s">
-        <v>151</v>
-      </c>
-      <c r="O1" s="29" t="s">
-        <v>152</v>
-      </c>
-      <c r="P1" s="29" t="s">
-        <v>151</v>
-      </c>
-      <c r="Q1" s="29" t="s">
-        <v>152</v>
-      </c>
-      <c r="R1" s="29" t="s">
-        <v>151</v>
-      </c>
-      <c r="S1" s="29" t="s">
-        <v>152</v>
-      </c>
-      <c r="T1" s="29" t="s">
-        <v>151</v>
-      </c>
-      <c r="U1" s="29" t="s">
-        <v>152</v>
-      </c>
-      <c r="V1" s="29" t="s">
-        <v>151</v>
-      </c>
-      <c r="W1" s="29" t="s">
-        <v>152</v>
-      </c>
-      <c r="X1" s="33" t="s">
+      <c r="Y1" s="29" t="s">
         <v>153</v>
-      </c>
-      <c r="Y1" s="29" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:25">
@@ -33566,10 +33566,10 @@
         <v>1000</v>
       </c>
       <c r="B2" s="86" t="s">
+        <v>154</v>
+      </c>
+      <c r="C2" s="87" t="s">
         <v>155</v>
-      </c>
-      <c r="C2" s="87" t="s">
-        <v>156</v>
       </c>
       <c r="D2" s="85">
         <v>1</v>
@@ -33609,10 +33609,10 @@
         <v>1001</v>
       </c>
       <c r="B3" s="90" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C3" s="87" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D3" s="87">
         <v>2</v>
@@ -33652,10 +33652,10 @@
         <v>2000</v>
       </c>
       <c r="B4" s="90" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C4" s="87" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D4" s="87">
         <v>2</v>
@@ -33703,10 +33703,10 @@
         <v>2001</v>
       </c>
       <c r="B5" s="90" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C5" s="87" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D5" s="87">
         <v>2</v>
@@ -33754,10 +33754,10 @@
         <v>2002</v>
       </c>
       <c r="B6" s="90" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C6" s="87" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D6" s="87">
         <v>2</v>
@@ -33805,10 +33805,10 @@
         <v>2100</v>
       </c>
       <c r="B7" s="90" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C7" s="87" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D7" s="87">
         <v>1</v>
@@ -33856,10 +33856,10 @@
         <v>2101</v>
       </c>
       <c r="B8" s="90" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C8" s="87" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D8" s="87">
         <v>1</v>
@@ -33907,10 +33907,10 @@
         <v>2102</v>
       </c>
       <c r="B9" s="90" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C9" s="87" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D9" s="87">
         <v>1</v>
@@ -33958,10 +33958,10 @@
         <v>2103</v>
       </c>
       <c r="B10" s="90" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C10" s="87" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D10" s="87">
         <v>1</v>
@@ -34009,10 +34009,10 @@
         <v>2104</v>
       </c>
       <c r="B11" s="90" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C11" s="87" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D11" s="87">
         <v>1</v>
@@ -34060,10 +34060,10 @@
         <v>2105</v>
       </c>
       <c r="B12" s="90" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C12" s="87" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D12" s="87">
         <v>1</v>
@@ -34111,10 +34111,10 @@
         <v>2106</v>
       </c>
       <c r="B13" s="90" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C13" s="87" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D13" s="87">
         <v>1</v>
@@ -34162,10 +34162,10 @@
         <v>2107</v>
       </c>
       <c r="B14" s="90" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C14" s="87" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D14" s="87">
         <v>1</v>
@@ -34213,10 +34213,10 @@
         <v>2108</v>
       </c>
       <c r="B15" s="90" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C15" s="87" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D15" s="87">
         <v>1</v>
@@ -34264,10 +34264,10 @@
         <v>2109</v>
       </c>
       <c r="B16" s="90" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C16" s="87" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D16" s="87">
         <v>1</v>
@@ -34315,10 +34315,10 @@
         <v>3001</v>
       </c>
       <c r="B17" s="90" t="s">
+        <v>170</v>
+      </c>
+      <c r="C17" s="87" t="s">
         <v>171</v>
-      </c>
-      <c r="C17" s="87" t="s">
-        <v>172</v>
       </c>
       <c r="D17" s="87">
         <v>1</v>
@@ -34362,10 +34362,10 @@
         <v>3002</v>
       </c>
       <c r="B18" s="90" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C18" s="87" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D18" s="87">
         <v>2</v>
@@ -34409,10 +34409,10 @@
         <v>3004</v>
       </c>
       <c r="B19" s="90" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C19" s="87" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D19" s="87">
         <v>2</v>
@@ -34460,10 +34460,10 @@
         <v>3005</v>
       </c>
       <c r="B20" s="90" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C20" s="87" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D20" s="87">
         <v>2</v>
@@ -34511,10 +34511,10 @@
         <v>3006</v>
       </c>
       <c r="B21" s="90" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C21" s="87" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D21" s="87">
         <v>2</v>

</xml_diff>